<commit_message>
RPA datasets push 2023-09-18
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="88">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-09-14</t>
+  </si>
+  <si>
     <t>2023-09-07</t>
   </si>
   <si>
@@ -112,205 +115,169 @@
     <t>2023-07-26</t>
   </si>
   <si>
-    <t>2023-07-25</t>
-  </si>
-  <si>
-    <t>2023-07-21</t>
+    <t>상상인제4호스팩</t>
+  </si>
+  <si>
+    <t>한화플러스제4호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제16호스팩</t>
+  </si>
+  <si>
+    <t>유안타제11호스팩</t>
+  </si>
+  <si>
+    <t>한국제12호스팩</t>
+  </si>
+  <si>
+    <t>대신밸런스제15호스팩</t>
+  </si>
+  <si>
+    <t>시큐레터</t>
+  </si>
+  <si>
+    <t>스마트레이더시스템</t>
+  </si>
+  <si>
+    <t>넥스틸</t>
+  </si>
+  <si>
+    <t>빅텐츠</t>
+  </si>
+  <si>
+    <t>큐리옥스바이오시스템즈</t>
+  </si>
+  <si>
+    <t>하나28호스팩</t>
+  </si>
+  <si>
+    <t>SK증권제10호스팩</t>
+  </si>
+  <si>
+    <t>코츠테크놀로지</t>
+  </si>
+  <si>
+    <t>KB제26호스팩</t>
+  </si>
+  <si>
+    <t>파두</t>
+  </si>
+  <si>
+    <t>엠아이큐브솔루션</t>
+  </si>
+  <si>
+    <t>시지트로닉스</t>
+  </si>
+  <si>
+    <t>파로스아이바이오</t>
+  </si>
+  <si>
+    <t>유안타제14호스팩</t>
+  </si>
+  <si>
+    <t>에이엘티</t>
+  </si>
+  <si>
+    <t>버넥트</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>상상인</t>
+  </si>
+  <si>
+    <t>한화</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>2023-08-23</t>
+  </si>
+  <si>
+    <t>2023-08-14</t>
+  </si>
+  <si>
+    <t>2023-08-09</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>2023-07-31</t>
+  </si>
+  <si>
+    <t>2023-07-24</t>
+  </si>
+  <si>
+    <t>2023-07-17</t>
+  </si>
+  <si>
+    <t>2023-08-28</t>
+  </si>
+  <si>
+    <t>2023-08-25</t>
+  </si>
+  <si>
+    <t>2023-08-18</t>
+  </si>
+  <si>
+    <t>2023-08-16</t>
   </si>
   <si>
     <t>2023-07-20</t>
-  </si>
-  <si>
-    <t>2023-07-19</t>
-  </si>
-  <si>
-    <t>한화플러스제4호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제16호스팩</t>
-  </si>
-  <si>
-    <t>유안타제11호스팩</t>
-  </si>
-  <si>
-    <t>한국제12호스팩</t>
-  </si>
-  <si>
-    <t>대신밸런스제15호스팩</t>
-  </si>
-  <si>
-    <t>시큐레터</t>
-  </si>
-  <si>
-    <t>스마트레이더시스템</t>
-  </si>
-  <si>
-    <t>넥스틸</t>
-  </si>
-  <si>
-    <t>빅텐츠</t>
-  </si>
-  <si>
-    <t>큐리옥스바이오시스템즈</t>
-  </si>
-  <si>
-    <t>하나28호스팩</t>
-  </si>
-  <si>
-    <t>SK증권제10호스팩</t>
-  </si>
-  <si>
-    <t>코츠테크놀로지</t>
-  </si>
-  <si>
-    <t>KB제26호스팩</t>
-  </si>
-  <si>
-    <t>파두</t>
-  </si>
-  <si>
-    <t>엠아이큐브솔루션</t>
-  </si>
-  <si>
-    <t>시지트로닉스</t>
-  </si>
-  <si>
-    <t>파로스아이바이오</t>
-  </si>
-  <si>
-    <t>유안타제14호스팩</t>
-  </si>
-  <si>
-    <t>에이엘티</t>
-  </si>
-  <si>
-    <t>버넥트</t>
-  </si>
-  <si>
-    <t>뷰티스킨</t>
-  </si>
-  <si>
-    <t>SK증권제9호스팩</t>
-  </si>
-  <si>
-    <t>와이랩</t>
-  </si>
-  <si>
-    <t>센서뷰</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>한화</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>SK</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-08-29</t>
-  </si>
-  <si>
-    <t>2023-08-23</t>
-  </si>
-  <si>
-    <t>2023-08-14</t>
-  </si>
-  <si>
-    <t>2023-08-09</t>
-  </si>
-  <si>
-    <t>2023-08-01</t>
-  </si>
-  <si>
-    <t>2023-07-31</t>
-  </si>
-  <si>
-    <t>2023-07-24</t>
-  </si>
-  <si>
-    <t>2023-07-17</t>
-  </si>
-  <si>
-    <t>2023-07-13</t>
-  </si>
-  <si>
-    <t>2023-07-11</t>
-  </si>
-  <si>
-    <t>2023-07-10</t>
-  </si>
-  <si>
-    <t>2023-08-28</t>
-  </si>
-  <si>
-    <t>2023-08-25</t>
-  </si>
-  <si>
-    <t>2023-08-18</t>
-  </si>
-  <si>
-    <t>2023-08-16</t>
-  </si>
-  <si>
-    <t>2023-07-18</t>
-  </si>
-  <si>
-    <t>2023-07-14</t>
   </si>
 </sst>
 </file>
@@ -668,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -732,37 +699,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F2">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -771,13 +738,13 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q2">
-        <v>3562500</v>
+        <v>3375000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -785,37 +752,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D3">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F3">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -824,13 +791,13 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="Q3">
-        <v>4875000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -838,37 +805,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -877,13 +844,13 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="P4" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="Q4">
-        <v>3750000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -891,37 +858,37 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F5">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -933,48 +900,48 @@
         <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="Q5">
-        <v>3000000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6">
+        <v>80</v>
+      </c>
+      <c r="E6" t="s">
         <v>61</v>
       </c>
-      <c r="D6">
-        <v>130</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
-      </c>
       <c r="F6">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M6">
         <v>2000</v>
@@ -983,13 +950,13 @@
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q6">
-        <v>4875000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -997,52 +964,52 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D7">
-        <v>160.0662</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F7">
-        <v>160.0662</v>
+        <v>130</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M7">
-        <v>12000</v>
+        <v>2000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="Q7">
-        <v>1000414</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1050,52 +1017,52 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D8">
-        <v>177.6</v>
+        <v>160.0662</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F8">
-        <v>177.6</v>
+        <v>160.0662</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M8">
-        <v>8000</v>
+        <v>12000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="P8" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="Q8">
-        <v>1665000</v>
+        <v>1000414</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1103,52 +1070,52 @@
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D9">
-        <v>805</v>
+        <v>177.6</v>
       </c>
       <c r="E9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F9">
-        <v>805</v>
+        <v>177.6</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M9">
-        <v>11500</v>
+        <v>8000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="P9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="Q9">
-        <v>5239200</v>
+        <v>1665000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1156,52 +1123,52 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D10">
-        <v>107.686</v>
+        <v>805</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F10">
-        <v>107.686</v>
+        <v>805</v>
       </c>
       <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K10" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10">
+        <v>11500</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10" t="s">
         <v>78</v>
       </c>
-      <c r="H10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" t="s">
-        <v>78</v>
-      </c>
-      <c r="M10">
-        <v>23000</v>
-      </c>
-      <c r="N10">
-        <v>100</v>
-      </c>
-      <c r="O10" t="s">
-        <v>27</v>
-      </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="Q10">
-        <v>351150</v>
+        <v>5239200</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1209,105 +1176,105 @@
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D11">
-        <v>182</v>
+        <v>107.686</v>
       </c>
       <c r="E11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F11">
-        <v>182</v>
+        <v>107.686</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M11">
-        <v>13000</v>
+        <v>23000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="P11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Q11">
-        <v>1050000</v>
+        <v>351150</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D12">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F12">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K12" t="s">
+        <v>72</v>
+      </c>
+      <c r="L12" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12">
+        <v>13000</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12" t="s">
         <v>79</v>
       </c>
-      <c r="L12" t="s">
-        <v>78</v>
-      </c>
-      <c r="M12">
-        <v>2000</v>
-      </c>
-      <c r="N12">
-        <v>100</v>
-      </c>
-      <c r="O12" t="s">
-        <v>86</v>
-      </c>
       <c r="P12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q12">
-        <v>4875000</v>
+        <v>1050000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1315,37 +1282,37 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D13">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F13">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1354,116 +1321,116 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="P13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q13">
-        <v>2250000</v>
+        <v>4875000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D14">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14">
-        <v>123.5</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M14">
+        <v>2000</v>
+      </c>
+      <c r="N14">
+        <v>100</v>
+      </c>
+      <c r="O14" t="s">
         <v>79</v>
       </c>
-      <c r="L14" t="s">
-        <v>78</v>
-      </c>
-      <c r="M14">
-        <v>13000</v>
-      </c>
-      <c r="N14">
-        <v>95</v>
-      </c>
-      <c r="O14" t="s">
-        <v>86</v>
-      </c>
       <c r="P14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q14">
-        <v>1348698</v>
+        <v>2250000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>130</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F15">
-        <v>6.5</v>
+        <v>123.5</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M15">
         <v>13000</v>
       </c>
       <c r="N15">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="O15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="P15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q15">
         <v>1348698</v>
@@ -1471,158 +1438,158 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D16">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F16">
-        <v>100</v>
+        <v>6.5</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J16" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" t="s">
+        <v>71</v>
+      </c>
+      <c r="M16">
+        <v>13000</v>
+      </c>
+      <c r="N16">
+        <v>5</v>
+      </c>
+      <c r="O16" t="s">
         <v>79</v>
-      </c>
-      <c r="L16" t="s">
-        <v>78</v>
-      </c>
-      <c r="M16">
-        <v>2000</v>
-      </c>
-      <c r="N16">
-        <v>100</v>
-      </c>
-      <c r="O16" t="s">
-        <v>87</v>
       </c>
       <c r="P16" t="s">
         <v>29</v>
       </c>
       <c r="Q16">
-        <v>3750000</v>
+        <v>1348698</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D17">
-        <v>1937.5</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F17">
-        <v>1240</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L17" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M17">
-        <v>31000</v>
+        <v>2000</v>
       </c>
       <c r="N17">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
+        <v>80</v>
+      </c>
+      <c r="P17" t="s">
         <v>30</v>
       </c>
-      <c r="P17" t="s">
-        <v>86</v>
-      </c>
       <c r="Q17">
-        <v>26542452</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D18">
         <v>1937.5</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F18">
-        <v>542.5</v>
+        <v>1240</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M18">
         <v>31000</v>
       </c>
       <c r="N18">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="O18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P18" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q18">
         <v>26542452</v>
@@ -1630,52 +1597,52 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D19">
         <v>1937.5</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F19">
-        <v>38.75</v>
+        <v>542.5</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M19">
         <v>31000</v>
       </c>
       <c r="N19">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="O19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q19">
         <v>26542452</v>
@@ -1683,40 +1650,40 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>1937.5</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>38.75</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M20">
         <v>31000</v>
@@ -1725,10 +1692,10 @@
         <v>2</v>
       </c>
       <c r="O20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P20" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q20">
         <v>26542452</v>
@@ -1736,40 +1703,40 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21">
         <v>1937.5</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F21">
         <v>38.75</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K21" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="L21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M21">
         <v>31000</v>
@@ -1778,10 +1745,10 @@
         <v>2</v>
       </c>
       <c r="O21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P21" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q21">
         <v>26542452</v>
@@ -1789,40 +1756,40 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D22">
         <v>1937.5</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F22">
         <v>38.75</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K22" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M22">
         <v>31000</v>
@@ -1831,10 +1798,10 @@
         <v>2</v>
       </c>
       <c r="O22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P22" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q22">
         <v>26542452</v>
@@ -1845,52 +1812,52 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D23">
-        <v>145.2</v>
+        <v>1937.5</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F23">
-        <v>145.2</v>
+        <v>38.75</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M23">
-        <v>12000</v>
+        <v>31000</v>
       </c>
       <c r="N23">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="O23" t="s">
         <v>31</v>
       </c>
       <c r="P23" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Q23">
-        <v>786500</v>
+        <v>26542452</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1898,52 +1865,52 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24">
+        <v>145.2</v>
+      </c>
+      <c r="E24" t="s">
         <v>61</v>
       </c>
-      <c r="D24">
-        <v>225</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
       <c r="F24">
-        <v>225</v>
+        <v>145.2</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M24">
-        <v>25000</v>
+        <v>12000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="P24" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="Q24">
-        <v>675000</v>
+        <v>786500</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1951,158 +1918,158 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D25">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F25">
-        <v>196</v>
+        <v>225</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K25" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L25" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M25">
-        <v>14000</v>
+        <v>25000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="P25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q25">
-        <v>1050000</v>
+        <v>675000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26">
+        <v>196</v>
+      </c>
+      <c r="E26" t="s">
         <v>61</v>
       </c>
-      <c r="D26">
-        <v>80</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
       <c r="F26">
-        <v>80</v>
+        <v>196</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K26" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M26">
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="P26" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="Q26">
-        <v>3000000</v>
+        <v>1050000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D27">
-        <v>225</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="F27">
-        <v>225</v>
+        <v>80</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K27" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M27">
-        <v>25000</v>
+        <v>2000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="P27" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="Q27">
-        <v>675000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2110,52 +2077,52 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D28">
-        <v>307.2</v>
+        <v>225</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F28">
-        <v>307.2</v>
+        <v>225</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K28" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L28" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M28">
-        <v>16000</v>
+        <v>25000</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="P28" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="Q28">
-        <v>1440000</v>
+        <v>675000</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2163,211 +2130,52 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D29">
-        <v>114.4</v>
+        <v>307.2</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="F29">
-        <v>114.4</v>
+        <v>307.2</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="J29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="K29" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="L29" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M29">
-        <v>26000</v>
+        <v>16000</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="P29" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="Q29">
-        <v>261188</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30">
-        <v>80</v>
-      </c>
-      <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30">
-        <v>80</v>
-      </c>
-      <c r="G30" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I30" t="s">
-        <v>78</v>
-      </c>
-      <c r="J30" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" t="s">
-        <v>79</v>
-      </c>
-      <c r="L30" t="s">
-        <v>78</v>
-      </c>
-      <c r="M30">
-        <v>2000</v>
-      </c>
-      <c r="N30">
-        <v>100</v>
-      </c>
-      <c r="O30" t="s">
-        <v>91</v>
-      </c>
-      <c r="P30" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q30">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31">
-        <v>270</v>
-      </c>
-      <c r="E31" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31">
-        <v>270</v>
-      </c>
-      <c r="G31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" t="s">
-        <v>78</v>
-      </c>
-      <c r="K31" t="s">
-        <v>79</v>
-      </c>
-      <c r="L31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31">
-        <v>9000</v>
-      </c>
-      <c r="N31">
-        <v>100</v>
-      </c>
-      <c r="O31" t="s">
-        <v>92</v>
-      </c>
-      <c r="P31" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q31">
-        <v>2160000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32">
-        <v>175.5</v>
-      </c>
-      <c r="E32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F32">
-        <v>175.5</v>
-      </c>
-      <c r="G32" t="s">
-        <v>78</v>
-      </c>
-      <c r="H32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" t="s">
-        <v>78</v>
-      </c>
-      <c r="K32" t="s">
-        <v>79</v>
-      </c>
-      <c r="L32" t="s">
-        <v>78</v>
-      </c>
-      <c r="M32">
-        <v>4500</v>
-      </c>
-      <c r="N32">
-        <v>100</v>
-      </c>
-      <c r="O32" t="s">
-        <v>92</v>
-      </c>
-      <c r="P32" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q32">
-        <v>2925000</v>
+        <v>1440000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-10
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="89">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,12 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-09</t>
+  </si>
+  <si>
+    <t>2023-11-10</t>
+  </si>
+  <si>
     <t>2023-11-07</t>
   </si>
   <si>
@@ -112,6 +118,18 @@
     <t>2023-09-25</t>
   </si>
   <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
     <t>쏘닉스</t>
   </si>
   <si>
@@ -169,12 +187,24 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
     <t>KB</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>신한</t>
   </si>
   <si>
@@ -187,9 +217,6 @@
     <t>하나</t>
   </si>
   <si>
-    <t>미래</t>
-  </si>
-  <si>
     <t>현대차</t>
   </si>
   <si>
@@ -202,9 +229,6 @@
     <t>유비에스</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
     <t>유안타</t>
   </si>
   <si>
@@ -214,18 +238,21 @@
     <t>-</t>
   </si>
   <si>
+    <t>공동대표</t>
+  </si>
+  <si>
     <t>대표</t>
   </si>
   <si>
-    <t>공동대표</t>
-  </si>
-  <si>
     <t>공동</t>
   </si>
   <si>
     <t>인수</t>
   </si>
   <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
     <t>2023-10-24</t>
   </si>
   <si>
@@ -245,9 +272,6 @@
   </si>
   <si>
     <t>2023-09-14</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
   </si>
   <si>
     <t>2023-10-11</t>
@@ -614,7 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -678,688 +702,688 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D2">
-        <v>270</v>
+        <v>320</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F2">
-        <v>270</v>
+        <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M2">
-        <v>7500</v>
+        <v>20000</v>
       </c>
       <c r="N2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="P2" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="Q2">
-        <v>2600000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <v>320</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F3">
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
       </c>
       <c r="Q3">
-        <v>9375000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>178.41194</v>
+        <v>249.6</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F4">
-        <v>178.41194</v>
+        <v>249.6</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M4">
-        <v>17000</v>
+        <v>4800</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>787111</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D5">
-        <v>49.66368</v>
+        <v>463.5</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F5">
-        <v>49.66368</v>
+        <v>463.5</v>
       </c>
       <c r="G5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M5">
-        <v>4400</v>
+        <v>22500</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q5">
-        <v>846540</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D6">
-        <v>306</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F6">
-        <v>306</v>
+        <v>156</v>
       </c>
       <c r="G6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M6">
-        <v>17000</v>
+        <v>13000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="P6" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="Q6">
-        <v>1119600</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D7">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F7">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L7" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M7">
-        <v>6500</v>
+        <v>7500</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="Q7">
-        <v>2880000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D8">
-        <v>53.9</v>
+        <v>250</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F8">
-        <v>53.9</v>
+        <v>250</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L8" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M8">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q8">
-        <v>577500</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D9">
-        <v>520</v>
+        <v>178.41194</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F9">
-        <v>520</v>
+        <v>178.41194</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M9">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q9">
-        <v>1300000</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D10">
-        <v>442.659</v>
+        <v>49.66368</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F10">
-        <v>442.659</v>
+        <v>49.66368</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M10">
-        <v>10700</v>
+        <v>4400</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="P10" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="Q10">
-        <v>3102750</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D11">
-        <v>80</v>
+        <v>306</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="F11">
-        <v>80</v>
+        <v>306</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>17000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="Q11">
-        <v>3000000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D12">
-        <v>4212</v>
+        <v>260</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F12">
-        <v>1263.6</v>
+        <v>260</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M12">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N12">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="P12" t="s">
-        <v>79</v>
+        <v>25</v>
       </c>
       <c r="Q12">
-        <v>87871545</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D13">
-        <v>4212</v>
+        <v>53.9</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F13">
-        <v>1263.6</v>
+        <v>53.9</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M13">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N13">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="P13" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="Q13">
-        <v>87871545</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D14">
-        <v>4212</v>
+        <v>520</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F14">
-        <v>421.2</v>
+        <v>520</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K14" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M14">
         <v>26000</v>
       </c>
       <c r="N14">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="P14" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="Q14">
-        <v>87871545</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1367,155 +1391,155 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D15">
-        <v>4212</v>
+        <v>442.659</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F15">
-        <v>421.2</v>
+        <v>442.659</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K15" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M15">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="N15">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="P15" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="Q15">
-        <v>87871545</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D16">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F16">
-        <v>421.2</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K16" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M16">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N16">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="P16" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="Q16">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D17">
         <v>4212</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F17">
-        <v>126.36</v>
+        <v>1263.6</v>
       </c>
       <c r="G17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K17" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="L17" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M17">
         <v>26000</v>
       </c>
       <c r="N17">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="P17" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="Q17">
         <v>87871545</v>
@@ -1523,52 +1547,52 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D18">
         <v>4212</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F18">
-        <v>126.36</v>
+        <v>1263.6</v>
       </c>
       <c r="G18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="L18" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M18">
         <v>26000</v>
       </c>
       <c r="N18">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="O18" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="P18" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="Q18">
         <v>87871545</v>
@@ -1576,52 +1600,52 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D19">
         <v>4212</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F19">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K19" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="L19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M19">
         <v>26000</v>
       </c>
       <c r="N19">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O19" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="P19" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="Q19">
         <v>87871545</v>
@@ -1629,52 +1653,52 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>4212</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F20">
-        <v>42.12</v>
+        <v>421.2</v>
       </c>
       <c r="G20" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K20" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="L20" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M20">
         <v>26000</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O20" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="P20" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="Q20">
         <v>87871545</v>
@@ -1682,108 +1706,108 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D21">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F21">
-        <v>360</v>
+        <v>421.2</v>
       </c>
       <c r="G21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="L21" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M21">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N21">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="O21" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="P21" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Q21">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D22">
-        <v>187.5</v>
+        <v>4212</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="F22">
-        <v>187.5</v>
+        <v>126.36</v>
       </c>
       <c r="G22" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J22" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L22" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M22">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N22">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O22" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="P22" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Q22">
-        <v>1020000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1791,263 +1815,528 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D23">
-        <v>336</v>
+        <v>4212</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="F23">
-        <v>336</v>
+        <v>126.36</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J23" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L23" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M23">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="N23">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O23" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="P23" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="Q23">
-        <v>1619200</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D24">
-        <v>221.2</v>
+        <v>4212</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F24">
-        <v>154.84</v>
+        <v>126.36</v>
       </c>
       <c r="G24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="L24" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M24">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="N24">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="O24" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="P24" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="Q24">
-        <v>2370000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D25">
-        <v>221.2</v>
+        <v>4212</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F25">
-        <v>66.36</v>
+        <v>42.12</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K25" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="L25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M25">
-        <v>14000</v>
+        <v>26000</v>
       </c>
       <c r="N25">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O25" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="P25" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="Q25">
-        <v>2370000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D26">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F26">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K26" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L26" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M26">
-        <v>23000</v>
+        <v>2000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="P26" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="Q26">
-        <v>1125000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D27">
-        <v>264</v>
+        <v>187.5</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F27">
-        <v>264</v>
+        <v>187.5</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H27" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J27" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="K27" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="L27" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="M27">
-        <v>24000</v>
+        <v>12500</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="P27" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="Q27">
+        <v>1020000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28">
+        <v>336</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28">
+        <v>336</v>
+      </c>
+      <c r="G28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" t="s">
+        <v>75</v>
+      </c>
+      <c r="L28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M28">
+        <v>15000</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
+      <c r="O28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P28" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q28">
+        <v>1619200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>221.2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F29">
+        <v>154.84</v>
+      </c>
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" t="s">
+        <v>75</v>
+      </c>
+      <c r="L29" t="s">
+        <v>73</v>
+      </c>
+      <c r="M29">
+        <v>14000</v>
+      </c>
+      <c r="N29">
+        <v>70</v>
+      </c>
+      <c r="O29" t="s">
+        <v>84</v>
+      </c>
+      <c r="P29" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q29">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30">
+        <v>221.2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30">
+        <v>66.36</v>
+      </c>
+      <c r="G30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" t="s">
+        <v>73</v>
+      </c>
+      <c r="K30" t="s">
+        <v>77</v>
+      </c>
+      <c r="L30" t="s">
+        <v>73</v>
+      </c>
+      <c r="M30">
+        <v>14000</v>
+      </c>
+      <c r="N30">
+        <v>30</v>
+      </c>
+      <c r="O30" t="s">
+        <v>84</v>
+      </c>
+      <c r="P30" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q30">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>345</v>
+      </c>
+      <c r="E31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31">
+        <v>345</v>
+      </c>
+      <c r="G31" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" t="s">
+        <v>73</v>
+      </c>
+      <c r="J31" t="s">
+        <v>73</v>
+      </c>
+      <c r="K31" t="s">
+        <v>75</v>
+      </c>
+      <c r="L31" t="s">
+        <v>73</v>
+      </c>
+      <c r="M31">
+        <v>23000</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>84</v>
+      </c>
+      <c r="P31" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q31">
+        <v>1125000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32">
+        <v>264</v>
+      </c>
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32">
+        <v>264</v>
+      </c>
+      <c r="G32" t="s">
+        <v>73</v>
+      </c>
+      <c r="H32" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" t="s">
+        <v>73</v>
+      </c>
+      <c r="K32" t="s">
+        <v>75</v>
+      </c>
+      <c r="L32" t="s">
+        <v>73</v>
+      </c>
+      <c r="M32">
+        <v>24000</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32" t="s">
+        <v>85</v>
+      </c>
+      <c r="P32" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q32">
         <v>825000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-14
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="96">
   <si>
     <t>상장일</t>
   </si>
@@ -70,6 +70,12 @@
     <t>2023-11-09</t>
   </si>
   <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
     <t>2023-11-10</t>
   </si>
   <si>
@@ -121,6 +127,15 @@
     <t>큐로셀</t>
   </si>
   <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
     <t>메가터치</t>
   </si>
   <si>
@@ -193,6 +208,12 @@
     <t>삼성</t>
   </si>
   <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -202,15 +223,9 @@
     <t>IBK</t>
   </si>
   <si>
-    <t>KB</t>
-  </si>
-  <si>
     <t>신한</t>
   </si>
   <si>
-    <t>한국</t>
-  </si>
-  <si>
     <t>키움</t>
   </si>
   <si>
@@ -253,6 +268,9 @@
     <t>2023-10-31</t>
   </si>
   <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
     <t>2023-10-24</t>
   </si>
   <si>
@@ -272,6 +290,9 @@
   </si>
   <si>
     <t>2023-09-14</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
   </si>
   <si>
     <t>2023-10-11</t>
@@ -638,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -702,37 +723,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D2">
         <v>320</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F2">
         <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M2">
         <v>20000</v>
@@ -741,10 +762,10 @@
         <v>50</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q2">
         <v>2254770</v>
@@ -755,37 +776,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>320</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F3">
         <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M3">
         <v>20000</v>
@@ -794,10 +815,10 @@
         <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q3">
         <v>2254770</v>
@@ -808,317 +829,317 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D4">
-        <v>249.6</v>
+        <v>659.0825</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>249.6</v>
+        <v>659.0825</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M4">
-        <v>4800</v>
+        <v>25000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>78</v>
+        <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4">
-        <v>3900000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>463.5</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F5">
-        <v>463.5</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M5">
-        <v>22500</v>
+        <v>2000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P5" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="Q5">
-        <v>1545000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D6">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F6">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M6">
-        <v>13000</v>
+        <v>1800</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="Q6">
-        <v>840000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D7">
-        <v>270</v>
+        <v>249.6</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F7">
-        <v>270</v>
+        <v>249.6</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M7">
-        <v>7500</v>
+        <v>4800</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="P7" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="Q7">
-        <v>2600000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D8">
-        <v>250</v>
+        <v>463.5</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F8">
-        <v>250</v>
+        <v>463.5</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M8">
-        <v>2000</v>
+        <v>22500</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="P8" t="s">
         <v>22</v>
       </c>
       <c r="Q8">
-        <v>9375000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D9">
-        <v>178.41194</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="F9">
-        <v>178.41194</v>
+        <v>156</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M9">
-        <v>17000</v>
+        <v>13000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q9">
-        <v>787111</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1126,52 +1147,52 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>49.66368</v>
+        <v>270</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F10">
-        <v>49.66368</v>
+        <v>270</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M10">
-        <v>4400</v>
+        <v>7500</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="Q10">
-        <v>846540</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1179,52 +1200,52 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>306</v>
+        <v>250</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F11">
-        <v>306</v>
+        <v>250</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L11" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M11">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="P11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="Q11">
-        <v>1119600</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1232,252 +1253,252 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D12">
-        <v>260</v>
+        <v>178.41194</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F12">
-        <v>260</v>
+        <v>178.41194</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M12">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="P12" t="s">
         <v>25</v>
       </c>
       <c r="Q12">
-        <v>2880000</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D13">
-        <v>53.9</v>
+        <v>49.66368</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F13">
-        <v>53.9</v>
+        <v>49.66368</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L13" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M13">
-        <v>7000</v>
+        <v>4400</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
       <c r="P13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q13">
-        <v>577500</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>520</v>
+        <v>306</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="F14">
-        <v>520</v>
+        <v>306</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L14" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M14">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="P14" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="Q14">
-        <v>1300000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>442.659</v>
+        <v>260</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="F15">
-        <v>442.659</v>
+        <v>260</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K15" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M15">
-        <v>10700</v>
+        <v>6500</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="P15" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="Q15">
-        <v>3102750</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D16">
+        <v>53.9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16">
+        <v>53.9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K16" t="s">
         <v>80</v>
       </c>
-      <c r="E16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16">
-        <v>80</v>
-      </c>
-      <c r="G16" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" t="s">
-        <v>73</v>
-      </c>
-      <c r="K16" t="s">
-        <v>75</v>
-      </c>
       <c r="L16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M16">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N16">
         <v>100</v>
@@ -1489,60 +1510,60 @@
         <v>29</v>
       </c>
       <c r="Q16">
-        <v>3000000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>4212</v>
+        <v>520</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17">
-        <v>1263.6</v>
+        <v>520</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K17" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M17">
         <v>26000</v>
       </c>
       <c r="N17">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="P17" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="Q17">
-        <v>87871545</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1550,155 +1571,155 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D18">
-        <v>4212</v>
+        <v>442.659</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F18">
-        <v>1263.6</v>
+        <v>442.659</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M18">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18" t="s">
         <v>30</v>
       </c>
-      <c r="O18" t="s">
-        <v>82</v>
-      </c>
       <c r="P18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="Q18">
-        <v>87871545</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D19">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="F19">
-        <v>421.2</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M19">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N19">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="P19" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="Q19">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D20">
         <v>4212</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F20">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M20">
         <v>26000</v>
       </c>
       <c r="N20">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O20" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="P20" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Q20">
         <v>87871545</v>
@@ -1706,52 +1727,52 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D21">
         <v>4212</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F21">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M21">
         <v>26000</v>
       </c>
       <c r="N21">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="P21" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Q21">
         <v>87871545</v>
@@ -1759,52 +1780,52 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D22">
         <v>4212</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F22">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K22" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L22" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M22">
         <v>26000</v>
       </c>
       <c r="N22">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O22" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="P22" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Q22">
         <v>87871545</v>
@@ -1812,52 +1833,52 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D23">
         <v>4212</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F23">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J23" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L23" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M23">
         <v>26000</v>
       </c>
       <c r="N23">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O23" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="P23" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Q23">
         <v>87871545</v>
@@ -1865,52 +1886,52 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>4212</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F24">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K24" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M24">
         <v>26000</v>
       </c>
       <c r="N24">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="P24" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Q24">
         <v>87871545</v>
@@ -1918,13 +1939,13 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>4212</v>
@@ -1933,37 +1954,37 @@
         <v>70</v>
       </c>
       <c r="F25">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K25" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="L25" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M25">
         <v>26000</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="P25" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="Q25">
         <v>87871545</v>
@@ -1971,108 +1992,108 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D26">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F26">
-        <v>360</v>
+        <v>126.36</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K26" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="L26" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M26">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N26">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="P26" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="Q26">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D27">
-        <v>187.5</v>
+        <v>4212</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F27">
-        <v>187.5</v>
+        <v>126.36</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K27" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="L27" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M27">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N27">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="P27" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="Q27">
-        <v>1020000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2080,52 +2101,52 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D28">
-        <v>336</v>
+        <v>4212</v>
       </c>
       <c r="E28" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F28">
-        <v>336</v>
+        <v>42.12</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="L28" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M28">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="N28">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O28" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="P28" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="Q28">
-        <v>1619200</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2133,52 +2154,52 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D29">
-        <v>221.2</v>
+        <v>360</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F29">
-        <v>154.84</v>
+        <v>360</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K29" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L29" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M29">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N29">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P29" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="Q29">
-        <v>2370000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2186,52 +2207,52 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D30">
-        <v>221.2</v>
+        <v>187.5</v>
       </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F30">
-        <v>66.36</v>
+        <v>187.5</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L30" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M30">
-        <v>14000</v>
+        <v>12500</v>
       </c>
       <c r="N30">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P30" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="Q30">
-        <v>2370000</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2239,52 +2260,52 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D31">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F31">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I31" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J31" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="K31" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L31" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M31">
-        <v>23000</v>
+        <v>15000</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="P31" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="Q31">
-        <v>1125000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2292,51 +2313,210 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D32">
+        <v>221.2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32">
+        <v>154.84</v>
+      </c>
+      <c r="G32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" t="s">
+        <v>78</v>
+      </c>
+      <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L32" t="s">
+        <v>78</v>
+      </c>
+      <c r="M32">
+        <v>14000</v>
+      </c>
+      <c r="N32">
+        <v>70</v>
+      </c>
+      <c r="O32" t="s">
+        <v>90</v>
+      </c>
+      <c r="P32" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q32">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33">
+        <v>221.2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33">
+        <v>66.36</v>
+      </c>
+      <c r="G33" t="s">
+        <v>78</v>
+      </c>
+      <c r="H33" t="s">
+        <v>78</v>
+      </c>
+      <c r="I33" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" t="s">
+        <v>78</v>
+      </c>
+      <c r="K33" t="s">
+        <v>82</v>
+      </c>
+      <c r="L33" t="s">
+        <v>78</v>
+      </c>
+      <c r="M33">
+        <v>14000</v>
+      </c>
+      <c r="N33">
+        <v>30</v>
+      </c>
+      <c r="O33" t="s">
+        <v>90</v>
+      </c>
+      <c r="P33" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q33">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>345</v>
+      </c>
+      <c r="E34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34">
+        <v>345</v>
+      </c>
+      <c r="G34" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I34" t="s">
+        <v>78</v>
+      </c>
+      <c r="J34" t="s">
+        <v>78</v>
+      </c>
+      <c r="K34" t="s">
+        <v>80</v>
+      </c>
+      <c r="L34" t="s">
+        <v>78</v>
+      </c>
+      <c r="M34">
+        <v>23000</v>
+      </c>
+      <c r="N34">
+        <v>100</v>
+      </c>
+      <c r="O34" t="s">
+        <v>90</v>
+      </c>
+      <c r="P34" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q34">
+        <v>1125000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35">
         <v>264</v>
       </c>
-      <c r="E32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32">
+      <c r="E35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35">
         <v>264</v>
       </c>
-      <c r="G32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H32" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" t="s">
-        <v>73</v>
-      </c>
-      <c r="J32" t="s">
-        <v>73</v>
-      </c>
-      <c r="K32" t="s">
-        <v>75</v>
-      </c>
-      <c r="L32" t="s">
-        <v>73</v>
-      </c>
-      <c r="M32">
+      <c r="G35" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I35" t="s">
+        <v>78</v>
+      </c>
+      <c r="J35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K35" t="s">
+        <v>80</v>
+      </c>
+      <c r="L35" t="s">
+        <v>78</v>
+      </c>
+      <c r="M35">
         <v>24000</v>
       </c>
-      <c r="N32">
+      <c r="N35">
         <v>100</v>
       </c>
-      <c r="O32" t="s">
-        <v>85</v>
-      </c>
-      <c r="P32" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q32">
+      <c r="O35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P35" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q35">
         <v>825000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-16
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="98">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
     <t>2023-11-09</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     <t>2023-09-25</t>
   </si>
   <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
     <t>큐로셀</t>
   </si>
   <si>
@@ -202,6 +208,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>미래</t>
   </si>
   <si>
@@ -214,9 +223,6 @@
     <t>KB</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>대신</t>
   </si>
   <si>
@@ -253,18 +259,21 @@
     <t>-</t>
   </si>
   <si>
+    <t>대표</t>
+  </si>
+  <si>
     <t>공동대표</t>
   </si>
   <si>
-    <t>대표</t>
-  </si>
-  <si>
     <t>공동</t>
   </si>
   <si>
     <t>인수</t>
   </si>
   <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
     <t>2023-10-31</t>
   </si>
   <si>
@@ -290,9 +299,6 @@
   </si>
   <si>
     <t>2023-09-14</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
   </si>
   <si>
     <t>2023-10-11</t>
@@ -659,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -723,90 +729,90 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F2">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M2">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="Q2">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>320</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3">
         <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M3">
         <v>20000</v>
@@ -815,10 +821,10 @@
         <v>50</v>
       </c>
       <c r="O3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="P3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q3">
         <v>2254770</v>
@@ -829,105 +835,105 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D4">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F4">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M4">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N4">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O4" t="s">
+        <v>86</v>
+      </c>
+      <c r="P4" t="s">
         <v>23</v>
       </c>
-      <c r="P4" t="s">
-        <v>21</v>
-      </c>
       <c r="Q4">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F5">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="Q5">
-        <v>3000000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -935,52 +941,52 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M6">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="Q6">
-        <v>4550000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -988,211 +994,211 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F7">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M7">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="Q7">
-        <v>3900000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D8">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F8">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M8">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="P8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q8">
-        <v>1545000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D9">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F9">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M9">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="P9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q9">
-        <v>840000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D10">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F10">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M10">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="P10" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="Q10">
-        <v>2600000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1200,52 +1206,52 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F11">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="Q11">
-        <v>9375000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1253,105 +1259,105 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F12">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M12">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="P12" t="s">
         <v>25</v>
       </c>
       <c r="Q12">
-        <v>787111</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F13">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M13">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="P13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q13">
-        <v>846540</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1359,52 +1365,52 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F14">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M14">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="P14" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="Q14">
-        <v>1119600</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1412,52 +1418,52 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F15">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M15">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>87</v>
+        <v>29</v>
       </c>
       <c r="P15" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="Q15">
-        <v>2880000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1465,52 +1471,52 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F16">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M16">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="P16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q16">
-        <v>577500</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1518,52 +1524,52 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E17" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F17">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M17">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q17">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1571,52 +1577,52 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F18">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L18" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M18">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" t="s">
         <v>30</v>
       </c>
-      <c r="P18" t="s">
-        <v>93</v>
-      </c>
       <c r="Q18">
-        <v>3102750</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1624,52 +1630,52 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F19">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M19">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="Q19">
-        <v>3000000</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1677,90 +1683,90 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D20">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F20">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M20">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N20">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="P20" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="Q20">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D21">
         <v>4212</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F21">
         <v>1263.6</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L21" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M21">
         <v>26000</v>
@@ -1769,10 +1775,10 @@
         <v>30</v>
       </c>
       <c r="O21" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P21" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q21">
         <v>87871545</v>
@@ -1780,52 +1786,52 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D22">
         <v>4212</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M22">
         <v>26000</v>
       </c>
       <c r="N22">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O22" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q22">
         <v>87871545</v>
@@ -1833,40 +1839,40 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D23">
         <v>4212</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23">
         <v>421.2</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M23">
         <v>26000</v>
@@ -1875,10 +1881,10 @@
         <v>10</v>
       </c>
       <c r="O23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q23">
         <v>87871545</v>
@@ -1886,40 +1892,40 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <v>4212</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F24">
         <v>421.2</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K24" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M24">
         <v>26000</v>
@@ -1928,10 +1934,10 @@
         <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P24" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q24">
         <v>87871545</v>
@@ -1939,52 +1945,52 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D25">
         <v>4212</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F25">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M25">
         <v>26000</v>
       </c>
       <c r="N25">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O25" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P25" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q25">
         <v>87871545</v>
@@ -1992,40 +1998,40 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <v>4212</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F26">
         <v>126.36</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L26" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M26">
         <v>26000</v>
@@ -2034,10 +2040,10 @@
         <v>3</v>
       </c>
       <c r="O26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q26">
         <v>87871545</v>
@@ -2045,40 +2051,40 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D27">
         <v>4212</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F27">
         <v>126.36</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K27" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L27" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M27">
         <v>26000</v>
@@ -2087,10 +2093,10 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P27" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q27">
         <v>87871545</v>
@@ -2098,52 +2104,52 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>4212</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F28">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L28" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M28">
         <v>26000</v>
       </c>
       <c r="N28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O28" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="Q28">
         <v>87871545</v>
@@ -2154,105 +2160,105 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D29">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F29">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K29" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L29" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M29">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N29">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q29">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D30">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F30">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M30">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N30">
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P30" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="Q30">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2260,52 +2266,52 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D31">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F31">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G31" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H31" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I31" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J31" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L31" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M31">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="Q31">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2313,102 +2319,102 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D32">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F32">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L32" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M32">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N32">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P32" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="Q32">
-        <v>2370000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D33">
         <v>221.2</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F33">
-        <v>66.36</v>
+        <v>154.84</v>
       </c>
       <c r="G33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L33" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M33">
         <v>14000</v>
       </c>
       <c r="N33">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="O33" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="P33" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q33">
         <v>2370000</v>
@@ -2419,52 +2425,52 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D34">
-        <v>345</v>
+        <v>221.2</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F34">
-        <v>345</v>
+        <v>66.36</v>
       </c>
       <c r="G34" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I34" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J34" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K34" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L34" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M34">
-        <v>23000</v>
+        <v>14000</v>
       </c>
       <c r="N34">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O34" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="P34" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q34">
-        <v>1125000</v>
+        <v>2370000</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2472,51 +2478,104 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D35">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F35">
-        <v>264</v>
+        <v>345</v>
       </c>
       <c r="G35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="K35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L35" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M35">
-        <v>24000</v>
+        <v>23000</v>
       </c>
       <c r="N35">
         <v>100</v>
       </c>
       <c r="O35" t="s">
+        <v>93</v>
+      </c>
+      <c r="P35" t="s">
         <v>91</v>
       </c>
-      <c r="P35" t="s">
-        <v>89</v>
-      </c>
       <c r="Q35">
+        <v>1125000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D36">
+        <v>264</v>
+      </c>
+      <c r="E36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36">
+        <v>264</v>
+      </c>
+      <c r="G36" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" t="s">
+        <v>80</v>
+      </c>
+      <c r="I36" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" t="s">
+        <v>80</v>
+      </c>
+      <c r="K36" t="s">
+        <v>81</v>
+      </c>
+      <c r="L36" t="s">
+        <v>80</v>
+      </c>
+      <c r="M36">
+        <v>24000</v>
+      </c>
+      <c r="N36">
+        <v>100</v>
+      </c>
+      <c r="O36" t="s">
+        <v>94</v>
+      </c>
+      <c r="P36" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q36">
         <v>825000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-19
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="100">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-17</t>
+  </si>
+  <si>
     <t>2023-11-15</t>
   </si>
   <si>
@@ -124,171 +127,177 @@
     <t>2023-09-27</t>
   </si>
   <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>아이엠티</t>
+  </si>
+  <si>
+    <t>밀리의서재</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>유진</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
     <t>2023-09-25</t>
   </si>
   <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>인스웨이브시스템즈</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
     <t>2023-09-21</t>
   </si>
   <si>
@@ -296,9 +305,6 @@
   </si>
   <si>
     <t>2023-09-18</t>
-  </si>
-  <si>
-    <t>2023-09-14</t>
   </si>
   <si>
     <t>2023-10-11</t>
@@ -665,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -735,205 +741,205 @@
         <v>62</v>
       </c>
       <c r="D2">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
       </c>
       <c r="F2">
-        <v>63.84</v>
+        <v>2846.537406</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M2">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N2">
-        <v>100</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="P2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="Q2">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>62</v>
       </c>
       <c r="D3">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E3" t="s">
         <v>65</v>
       </c>
       <c r="F3">
-        <v>160</v>
+        <v>1219.944706</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M3">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N3">
-        <v>50</v>
+        <v>29.1</v>
       </c>
       <c r="O3" t="s">
         <v>86</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q3">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
       </c>
       <c r="D4">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E4" t="s">
         <v>66</v>
       </c>
       <c r="F4">
-        <v>160</v>
+        <v>125.767488</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M4">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N4">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O4" t="s">
         <v>86</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5">
-        <v>659.0825</v>
+        <v>63.84</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5">
-        <v>659.0825</v>
+        <v>63.84</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M5">
-        <v>25000</v>
+        <v>4000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q5">
-        <v>1827247</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -941,264 +947,264 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P6" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="Q6">
-        <v>3000000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D7">
-        <v>126</v>
+        <v>320</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M7">
-        <v>1800</v>
+        <v>20000</v>
       </c>
       <c r="N7">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P7" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="Q7">
-        <v>4550000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D8">
-        <v>249.6</v>
+        <v>659.0825</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F8">
-        <v>249.6</v>
+        <v>659.0825</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M8">
-        <v>4800</v>
+        <v>25000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="P8" t="s">
         <v>23</v>
       </c>
       <c r="Q8">
-        <v>3900000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D9">
-        <v>463.5</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F9">
-        <v>463.5</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M9">
-        <v>22500</v>
+        <v>2000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="Q9">
-        <v>1545000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D10">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M10">
-        <v>13000</v>
+        <v>1800</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="Q10">
-        <v>840000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1206,93 +1212,93 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D11">
-        <v>270</v>
+        <v>249.6</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F11">
-        <v>270</v>
+        <v>249.6</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M11">
-        <v>7500</v>
+        <v>4800</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="P11" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="Q11">
-        <v>2600000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12">
-        <v>250</v>
+        <v>463.5</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F12">
-        <v>250</v>
+        <v>463.5</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>22500</v>
       </c>
       <c r="N12">
         <v>100</v>
@@ -1301,540 +1307,540 @@
         <v>88</v>
       </c>
       <c r="P12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q12">
-        <v>9375000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D13">
-        <v>178.41194</v>
+        <v>156</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F13">
-        <v>178.41194</v>
+        <v>156</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M13">
-        <v>17000</v>
+        <v>13000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q13">
-        <v>787111</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D14">
-        <v>49.66368</v>
+        <v>270</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F14">
-        <v>49.66368</v>
+        <v>270</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M14">
-        <v>4400</v>
+        <v>7500</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>89</v>
+        <v>27</v>
       </c>
       <c r="P14" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="Q14">
-        <v>846540</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15">
-        <v>306</v>
+        <v>250</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F15">
-        <v>306</v>
+        <v>250</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M15">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="P15" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="Q15">
-        <v>1119600</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16">
-        <v>260</v>
+        <v>178.41194</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F16">
-        <v>260</v>
+        <v>178.41194</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M16">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q16">
-        <v>2880000</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D17">
-        <v>53.9</v>
+        <v>49.66368</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17">
-        <v>53.9</v>
+        <v>49.66368</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M17">
-        <v>7000</v>
+        <v>4400</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="P17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="Q17">
-        <v>577500</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D18">
-        <v>520</v>
+        <v>306</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F18">
-        <v>520</v>
+        <v>306</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M18">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P18" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="Q18">
-        <v>1300000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D19">
-        <v>442.659</v>
+        <v>260</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F19">
-        <v>442.659</v>
+        <v>260</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M19">
-        <v>10700</v>
+        <v>6500</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="P19" t="s">
-        <v>95</v>
+        <v>29</v>
       </c>
       <c r="Q19">
-        <v>3102750</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>53.9</v>
       </c>
       <c r="E20" t="s">
         <v>74</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>53.9</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q20">
-        <v>3000000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>63</v>
       </c>
       <c r="D21">
-        <v>4212</v>
+        <v>520</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F21">
-        <v>1263.6</v>
+        <v>520</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K21" t="s">
         <v>82</v>
       </c>
       <c r="L21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M21">
         <v>26000</v>
       </c>
       <c r="N21">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="P21" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="Q21">
-        <v>87871545</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
         <v>63</v>
       </c>
       <c r="D22">
-        <v>4212</v>
+        <v>442.659</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22">
-        <v>1263.6</v>
+        <v>442.659</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K22" t="s">
         <v>82</v>
       </c>
       <c r="L22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M22">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="N22">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="Q22">
-        <v>87871545</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1848,57 +1854,57 @@
         <v>63</v>
       </c>
       <c r="D23">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F23">
-        <v>421.2</v>
+        <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M23">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N23">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="P23" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="Q23">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24">
         <v>4212</v>
@@ -1907,37 +1913,37 @@
         <v>68</v>
       </c>
       <c r="F24">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M24">
         <v>26000</v>
       </c>
       <c r="N24">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q24">
         <v>87871545</v>
@@ -1945,52 +1951,52 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25">
         <v>4212</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F25">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="L25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M25">
         <v>26000</v>
       </c>
       <c r="N25">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O25" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q25">
         <v>87871545</v>
@@ -1998,52 +2004,52 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26">
         <v>4212</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F26">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M26">
         <v>26000</v>
       </c>
       <c r="N26">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P26" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q26">
         <v>87871545</v>
@@ -2051,52 +2057,52 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>4212</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F27">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M27">
         <v>26000</v>
       </c>
       <c r="N27">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O27" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P27" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q27">
         <v>87871545</v>
@@ -2104,52 +2110,52 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28">
         <v>4212</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F28">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M28">
         <v>26000</v>
       </c>
       <c r="N28">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O28" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P28" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q28">
         <v>87871545</v>
@@ -2157,52 +2163,52 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>4212</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F29">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K29" t="s">
         <v>84</v>
       </c>
       <c r="L29" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M29">
         <v>26000</v>
       </c>
       <c r="N29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O29" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P29" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="Q29">
         <v>87871545</v>
@@ -2219,46 +2225,46 @@
         <v>62</v>
       </c>
       <c r="D30">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F30">
-        <v>360</v>
+        <v>126.36</v>
       </c>
       <c r="G30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K30" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M30">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N30">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q30">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2266,317 +2272,423 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
         <v>62</v>
       </c>
       <c r="D31">
-        <v>187.5</v>
+        <v>4212</v>
       </c>
       <c r="E31" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F31">
-        <v>187.5</v>
+        <v>126.36</v>
       </c>
       <c r="G31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K31" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M31">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N31">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O31" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q31">
-        <v>1020000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>62</v>
       </c>
       <c r="D32">
-        <v>336</v>
+        <v>4212</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="F32">
-        <v>336</v>
+        <v>42.12</v>
       </c>
       <c r="G32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K32" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M32">
-        <v>15000</v>
+        <v>26000</v>
       </c>
       <c r="N32">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Q32">
-        <v>1619200</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D33">
-        <v>221.2</v>
+        <v>360</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F33">
-        <v>154.84</v>
+        <v>360</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M33">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N33">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P33" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="Q33">
-        <v>2370000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D34">
-        <v>221.2</v>
+        <v>187.5</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F34">
-        <v>66.36</v>
+        <v>187.5</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M34">
-        <v>14000</v>
+        <v>12500</v>
       </c>
       <c r="N34">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P34" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="Q34">
-        <v>2370000</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D35">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E35" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F35">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="G35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M35">
-        <v>23000</v>
+        <v>15000</v>
       </c>
       <c r="N35">
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P35" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="Q35">
-        <v>1125000</v>
+        <v>1619200</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36">
+        <v>221.2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36">
+        <v>154.84</v>
+      </c>
+      <c r="G36" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" t="s">
+        <v>81</v>
+      </c>
+      <c r="J36" t="s">
+        <v>81</v>
+      </c>
+      <c r="K36" t="s">
+        <v>82</v>
+      </c>
+      <c r="L36" t="s">
+        <v>81</v>
+      </c>
+      <c r="M36">
+        <v>14000</v>
+      </c>
+      <c r="N36">
+        <v>70</v>
+      </c>
+      <c r="O36" t="s">
+        <v>96</v>
+      </c>
+      <c r="P36" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q36">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37">
+        <v>221.2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37">
+        <v>66.36</v>
+      </c>
+      <c r="G37" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" t="s">
+        <v>81</v>
+      </c>
+      <c r="I37" t="s">
+        <v>81</v>
+      </c>
+      <c r="J37" t="s">
+        <v>81</v>
+      </c>
+      <c r="K37" t="s">
+        <v>84</v>
+      </c>
+      <c r="L37" t="s">
+        <v>81</v>
+      </c>
+      <c r="M37">
+        <v>14000</v>
+      </c>
+      <c r="N37">
+        <v>30</v>
+      </c>
+      <c r="O37" t="s">
+        <v>96</v>
+      </c>
+      <c r="P37" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q37">
+        <v>2370000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>61</v>
       </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36">
-        <v>264</v>
-      </c>
-      <c r="E36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36">
-        <v>264</v>
-      </c>
-      <c r="G36" t="s">
-        <v>80</v>
-      </c>
-      <c r="H36" t="s">
-        <v>80</v>
-      </c>
-      <c r="I36" t="s">
-        <v>80</v>
-      </c>
-      <c r="J36" t="s">
-        <v>80</v>
-      </c>
-      <c r="K36" t="s">
-        <v>81</v>
-      </c>
-      <c r="L36" t="s">
-        <v>80</v>
-      </c>
-      <c r="M36">
-        <v>24000</v>
-      </c>
-      <c r="N36">
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38">
+        <v>345</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38">
+        <v>345</v>
+      </c>
+      <c r="G38" t="s">
+        <v>81</v>
+      </c>
+      <c r="H38" t="s">
+        <v>81</v>
+      </c>
+      <c r="I38" t="s">
+        <v>81</v>
+      </c>
+      <c r="J38" t="s">
+        <v>81</v>
+      </c>
+      <c r="K38" t="s">
+        <v>82</v>
+      </c>
+      <c r="L38" t="s">
+        <v>81</v>
+      </c>
+      <c r="M38">
+        <v>23000</v>
+      </c>
+      <c r="N38">
         <v>100</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O38" t="s">
+        <v>96</v>
+      </c>
+      <c r="P38" t="s">
         <v>94</v>
       </c>
-      <c r="P36" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q36">
-        <v>825000</v>
+      <c r="Q38">
+        <v>1125000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-21
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="96">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-20</t>
+  </si>
+  <si>
     <t>2023-11-17</t>
   </si>
   <si>
@@ -121,180 +124,168 @@
     <t>2023-10-06</t>
   </si>
   <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>두산로보틱스</t>
+  </si>
+  <si>
+    <t>신한제11호스팩</t>
+  </si>
+  <si>
+    <t>한싹</t>
+  </si>
+  <si>
+    <t>레뷰코퍼레이션</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유비에스</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
     <t>2023-10-10</t>
   </si>
   <si>
-    <t>2023-09-27</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
-    <t>아이엠티</t>
-  </si>
-  <si>
-    <t>밀리의서재</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>유진</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
     <t>2023-09-25</t>
   </si>
   <si>
@@ -302,9 +293,6 @@
   </si>
   <si>
     <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-09-18</t>
   </si>
   <si>
     <t>2023-10-11</t>
@@ -671,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -735,102 +723,102 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>368.5</v>
+      </c>
+      <c r="E2" t="s">
         <v>62</v>
       </c>
-      <c r="D2">
-        <v>4192.2496</v>
-      </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
       <c r="F2">
-        <v>2846.537406</v>
+        <v>368.5</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M2">
-        <v>36200</v>
+        <v>11000</v>
       </c>
       <c r="N2">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q2">
-        <v>19108320</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>4192.2496</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F3">
-        <v>1219.944706</v>
+        <v>2846.537406</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M3">
         <v>36200</v>
       </c>
       <c r="N3">
-        <v>29.1</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q3">
         <v>19108320</v>
@@ -838,52 +826,52 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>4192.2496</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F4">
-        <v>125.767488</v>
+        <v>1219.944706</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M4">
         <v>36200</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>29.1</v>
       </c>
       <c r="O4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4">
         <v>19108320</v>
@@ -894,52 +882,52 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F5">
-        <v>63.84</v>
+        <v>125.767488</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M5">
+        <v>36200</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
         <v>82</v>
       </c>
-      <c r="L5" t="s">
-        <v>81</v>
-      </c>
-      <c r="M5">
-        <v>4000</v>
-      </c>
-      <c r="N5">
-        <v>100</v>
-      </c>
-      <c r="O5" t="s">
-        <v>87</v>
-      </c>
       <c r="P5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q5">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -947,90 +935,90 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
       </c>
       <c r="F6">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M6">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N6">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="Q6">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>320</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F7">
         <v>160</v>
       </c>
       <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" t="s">
         <v>81</v>
       </c>
-      <c r="H7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" t="s">
-        <v>81</v>
-      </c>
-      <c r="J7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" t="s">
-        <v>85</v>
-      </c>
       <c r="L7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M7">
         <v>20000</v>
@@ -1039,10 +1027,10 @@
         <v>50</v>
       </c>
       <c r="O7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q7">
         <v>2254770</v>
@@ -1053,105 +1041,105 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" t="s">
         <v>81</v>
       </c>
-      <c r="H8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" t="s">
-        <v>82</v>
-      </c>
       <c r="L8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M8">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O8" t="s">
+        <v>84</v>
+      </c>
+      <c r="P8" t="s">
         <v>25</v>
       </c>
-      <c r="P8" t="s">
-        <v>23</v>
-      </c>
       <c r="Q8">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F9">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L9" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="P9" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="Q9">
-        <v>3000000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1159,52 +1147,52 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F10">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M10">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Q10">
-        <v>4550000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1212,211 +1200,211 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F11">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M11">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="Q11">
-        <v>3900000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D12">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F12">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M12">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q12">
-        <v>1545000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F13">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M13">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="P13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q13">
-        <v>840000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="E14" t="s">
         <v>69</v>
       </c>
       <c r="F14">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K14" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M14">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="P14" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="Q14">
-        <v>2600000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1424,52 +1412,52 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F15">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="P15" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="Q15">
-        <v>9375000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1477,105 +1465,105 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F16">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M16">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P16" t="s">
         <v>27</v>
       </c>
       <c r="Q16">
-        <v>787111</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F17">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="G17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M17">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="P17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q17">
-        <v>846540</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1583,52 +1571,52 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D18">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F18">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L18" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M18">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="P18" t="s">
-        <v>91</v>
+        <v>28</v>
       </c>
       <c r="Q18">
-        <v>1119600</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1636,52 +1624,52 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D19">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F19">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M19">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="Q19">
-        <v>2880000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1689,52 +1677,52 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D20">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F20">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="G20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M20">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="P20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q20">
-        <v>577500</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1742,52 +1730,52 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D21">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E21" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F21">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M21">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="P21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q21">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1795,52 +1783,52 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22">
+        <v>520</v>
+      </c>
+      <c r="E22" t="s">
         <v>63</v>
       </c>
-      <c r="D22">
-        <v>442.659</v>
-      </c>
-      <c r="E22" t="s">
-        <v>64</v>
-      </c>
       <c r="F22">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="G22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M22">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
+        <v>89</v>
+      </c>
+      <c r="P22" t="s">
         <v>32</v>
       </c>
-      <c r="P22" t="s">
-        <v>97</v>
-      </c>
       <c r="Q22">
-        <v>3102750</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1848,52 +1836,52 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23">
+        <v>442.659</v>
+      </c>
+      <c r="E23" t="s">
         <v>63</v>
       </c>
-      <c r="D23">
-        <v>80</v>
-      </c>
-      <c r="E23" t="s">
-        <v>75</v>
-      </c>
       <c r="F23">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M23">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" t="s">
         <v>93</v>
       </c>
-      <c r="P23" t="s">
-        <v>33</v>
-      </c>
       <c r="Q23">
-        <v>3000000</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1901,90 +1889,90 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D24">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F24">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="L24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M24">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N24">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="P24" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="Q24">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>4212</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F25">
         <v>1263.6</v>
       </c>
       <c r="G25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
         <v>81</v>
       </c>
-      <c r="H25" t="s">
-        <v>81</v>
-      </c>
-      <c r="I25" t="s">
-        <v>81</v>
-      </c>
-      <c r="J25" t="s">
-        <v>81</v>
-      </c>
-      <c r="K25" t="s">
-        <v>85</v>
-      </c>
       <c r="L25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M25">
         <v>26000</v>
@@ -1993,10 +1981,10 @@
         <v>30</v>
       </c>
       <c r="O25" t="s">
+        <v>91</v>
+      </c>
+      <c r="P25" t="s">
         <v>94</v>
-      </c>
-      <c r="P25" t="s">
-        <v>98</v>
       </c>
       <c r="Q25">
         <v>87871545</v>
@@ -2004,52 +1992,52 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>4212</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F26">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J26" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" t="s">
         <v>81</v>
       </c>
-      <c r="H26" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" t="s">
-        <v>81</v>
-      </c>
-      <c r="J26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K26" t="s">
-        <v>83</v>
-      </c>
       <c r="L26" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M26">
         <v>26000</v>
       </c>
       <c r="N26">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O26" t="s">
+        <v>91</v>
+      </c>
+      <c r="P26" t="s">
         <v>94</v>
-      </c>
-      <c r="P26" t="s">
-        <v>98</v>
       </c>
       <c r="Q26">
         <v>87871545</v>
@@ -2057,40 +2045,40 @@
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>4212</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F27">
         <v>421.2</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L27" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M27">
         <v>26000</v>
@@ -2099,10 +2087,10 @@
         <v>10</v>
       </c>
       <c r="O27" t="s">
+        <v>91</v>
+      </c>
+      <c r="P27" t="s">
         <v>94</v>
-      </c>
-      <c r="P27" t="s">
-        <v>98</v>
       </c>
       <c r="Q27">
         <v>87871545</v>
@@ -2110,40 +2098,40 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D28">
         <v>4212</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F28">
         <v>421.2</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M28">
         <v>26000</v>
@@ -2152,10 +2140,10 @@
         <v>10</v>
       </c>
       <c r="O28" t="s">
+        <v>91</v>
+      </c>
+      <c r="P28" t="s">
         <v>94</v>
-      </c>
-      <c r="P28" t="s">
-        <v>98</v>
       </c>
       <c r="Q28">
         <v>87871545</v>
@@ -2163,52 +2151,52 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
         <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D29">
         <v>4212</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F29">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K29" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="L29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M29">
         <v>26000</v>
       </c>
       <c r="N29">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O29" t="s">
+        <v>91</v>
+      </c>
+      <c r="P29" t="s">
         <v>94</v>
-      </c>
-      <c r="P29" t="s">
-        <v>98</v>
       </c>
       <c r="Q29">
         <v>87871545</v>
@@ -2216,40 +2204,40 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D30">
         <v>4212</v>
       </c>
       <c r="E30" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F30">
         <v>126.36</v>
       </c>
       <c r="G30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M30">
         <v>26000</v>
@@ -2258,10 +2246,10 @@
         <v>3</v>
       </c>
       <c r="O30" t="s">
+        <v>91</v>
+      </c>
+      <c r="P30" t="s">
         <v>94</v>
-      </c>
-      <c r="P30" t="s">
-        <v>98</v>
       </c>
       <c r="Q30">
         <v>87871545</v>
@@ -2269,40 +2257,40 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31">
         <v>4212</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F31">
         <v>126.36</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K31" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L31" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M31">
         <v>26000</v>
@@ -2311,10 +2299,10 @@
         <v>3</v>
       </c>
       <c r="O31" t="s">
+        <v>91</v>
+      </c>
+      <c r="P31" t="s">
         <v>94</v>
-      </c>
-      <c r="P31" t="s">
-        <v>98</v>
       </c>
       <c r="Q31">
         <v>87871545</v>
@@ -2322,52 +2310,52 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32">
         <v>4212</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F32">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M32">
         <v>26000</v>
       </c>
       <c r="N32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O32" t="s">
+        <v>91</v>
+      </c>
+      <c r="P32" t="s">
         <v>94</v>
-      </c>
-      <c r="P32" t="s">
-        <v>98</v>
       </c>
       <c r="Q32">
         <v>87871545</v>
@@ -2378,105 +2366,105 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F33">
-        <v>360</v>
+        <v>42.12</v>
       </c>
       <c r="G33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M33">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N33">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="P33" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="Q33">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D34">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F34">
-        <v>187.5</v>
+        <v>360</v>
       </c>
       <c r="G34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K34" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M34">
-        <v>12500</v>
+        <v>2000</v>
       </c>
       <c r="N34">
         <v>100</v>
       </c>
       <c r="O34" t="s">
+        <v>92</v>
+      </c>
+      <c r="P34" t="s">
         <v>95</v>
       </c>
-      <c r="P34" t="s">
-        <v>99</v>
-      </c>
       <c r="Q34">
-        <v>1020000</v>
+        <v>13500000</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2484,52 +2472,52 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D35">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="E35" t="s">
         <v>67</v>
       </c>
       <c r="F35">
-        <v>336</v>
+        <v>187.5</v>
       </c>
       <c r="G35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K35" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M35">
-        <v>15000</v>
+        <v>12500</v>
       </c>
       <c r="N35">
         <v>100</v>
       </c>
       <c r="O35" t="s">
+        <v>92</v>
+      </c>
+      <c r="P35" t="s">
         <v>95</v>
       </c>
-      <c r="P35" t="s">
-        <v>99</v>
-      </c>
       <c r="Q35">
-        <v>1619200</v>
+        <v>1020000</v>
       </c>
     </row>
     <row r="36" spans="1:17">
@@ -2537,158 +2525,52 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" t="s">
-        <v>63</v>
-      </c>
       <c r="D36">
-        <v>221.2</v>
+        <v>336</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F36">
-        <v>154.84</v>
+        <v>336</v>
       </c>
       <c r="G36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="L36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M36">
-        <v>14000</v>
+        <v>15000</v>
       </c>
       <c r="N36">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="O36" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P36" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q36">
-        <v>2370000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37">
-        <v>221.2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>80</v>
-      </c>
-      <c r="F37">
-        <v>66.36</v>
-      </c>
-      <c r="G37" t="s">
-        <v>81</v>
-      </c>
-      <c r="H37" t="s">
-        <v>81</v>
-      </c>
-      <c r="I37" t="s">
-        <v>81</v>
-      </c>
-      <c r="J37" t="s">
-        <v>81</v>
-      </c>
-      <c r="K37" t="s">
-        <v>84</v>
-      </c>
-      <c r="L37" t="s">
-        <v>81</v>
-      </c>
-      <c r="M37">
-        <v>14000</v>
-      </c>
-      <c r="N37">
-        <v>30</v>
-      </c>
-      <c r="O37" t="s">
-        <v>96</v>
-      </c>
-      <c r="P37" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q37">
-        <v>2370000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>61</v>
-      </c>
-      <c r="C38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38">
-        <v>345</v>
-      </c>
-      <c r="E38" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38">
-        <v>345</v>
-      </c>
-      <c r="G38" t="s">
-        <v>81</v>
-      </c>
-      <c r="H38" t="s">
-        <v>81</v>
-      </c>
-      <c r="I38" t="s">
-        <v>81</v>
-      </c>
-      <c r="J38" t="s">
-        <v>81</v>
-      </c>
-      <c r="K38" t="s">
-        <v>82</v>
-      </c>
-      <c r="L38" t="s">
-        <v>81</v>
-      </c>
-      <c r="M38">
-        <v>23000</v>
-      </c>
-      <c r="N38">
-        <v>100</v>
-      </c>
-      <c r="O38" t="s">
-        <v>96</v>
-      </c>
-      <c r="P38" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q38">
-        <v>1125000</v>
+        <v>1619200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-22
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="97">
   <si>
     <t>상장일</t>
   </si>
@@ -70,6 +70,12 @@
     <t>2023-11-20</t>
   </si>
   <si>
+    <t>2023-11-21</t>
+  </si>
+  <si>
+    <t>2023-11-22</t>
+  </si>
+  <si>
     <t>2023-11-17</t>
   </si>
   <si>
@@ -121,12 +127,15 @@
     <t>2023-10-04</t>
   </si>
   <si>
-    <t>2023-10-06</t>
-  </si>
-  <si>
     <t>스톰테크</t>
   </si>
   <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
     <t>에코프로머티</t>
   </si>
   <si>
@@ -190,12 +199,6 @@
     <t>신한제11호스팩</t>
   </si>
   <si>
-    <t>한싹</t>
-  </si>
-  <si>
-    <t>레뷰코퍼레이션</t>
-  </si>
-  <si>
     <t>코스닥</t>
   </si>
   <si>
@@ -205,19 +208,19 @@
     <t>하이</t>
   </si>
   <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>미래</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>삼성</t>
   </si>
   <si>
     <t>한국</t>
-  </si>
-  <si>
-    <t>KB</t>
   </si>
   <si>
     <t>대신</t>
@@ -723,37 +726,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>368.5</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F2">
         <v>368.5</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M2">
         <v>11000</v>
@@ -762,10 +765,10 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q2">
         <v>2374500</v>
@@ -776,155 +779,155 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>61</v>
       </c>
       <c r="D3">
-        <v>4192.2496</v>
+        <v>721.413</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F3">
-        <v>2846.537406</v>
+        <v>721.413</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M3">
-        <v>36200</v>
+        <v>34700</v>
       </c>
       <c r="N3">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
         <v>21</v>
       </c>
       <c r="Q3">
-        <v>19108320</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F4">
-        <v>1219.944706</v>
+        <v>441.12</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
         <v>79</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M4">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N4">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="Q4">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>4192.2496</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F5">
-        <v>125.767488</v>
+        <v>2846.537406</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M5">
         <v>36200</v>
       </c>
       <c r="N5">
-        <v>3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q5">
         <v>19108320</v>
@@ -932,55 +935,55 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D6">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F6">
-        <v>63.84</v>
+        <v>1219.944706</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M6">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>29.1</v>
       </c>
       <c r="O6" t="s">
         <v>83</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="Q6">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -988,264 +991,264 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E7" t="s">
         <v>63</v>
       </c>
       <c r="F7">
-        <v>160</v>
+        <v>125.767488</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
         <v>81</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M7">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N7">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q7">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D8">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E8" t="s">
         <v>65</v>
       </c>
       <c r="F8">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M8">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
         <v>84</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="Q8">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F9">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M9">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="Q9">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F10">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N10">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O10" t="s">
         <v>85</v>
       </c>
       <c r="P10" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
       <c r="Q10">
-        <v>3000000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="E11" t="s">
         <v>67</v>
       </c>
       <c r="F11">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M11">
-        <v>1800</v>
+        <v>25000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="P11" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="Q11">
-        <v>4550000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1253,264 +1256,264 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F12">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M12">
-        <v>4800</v>
+        <v>2000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
+        <v>86</v>
+      </c>
+      <c r="P12" t="s">
         <v>84</v>
       </c>
-      <c r="P12" t="s">
-        <v>25</v>
-      </c>
       <c r="Q12">
-        <v>3900000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D13">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F13">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M13">
-        <v>22500</v>
+        <v>1800</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
+        <v>86</v>
+      </c>
+      <c r="P13" t="s">
         <v>84</v>
       </c>
-      <c r="P13" t="s">
-        <v>25</v>
-      </c>
       <c r="Q13">
-        <v>1545000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F14">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M14">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q14">
-        <v>840000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F15">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M15">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="P15" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="Q15">
-        <v>2600000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F16">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M16">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P16" t="s">
         <v>27</v>
       </c>
       <c r="Q16">
-        <v>9375000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1518,93 +1521,93 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
       </c>
       <c r="F17">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M17">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="Q17">
-        <v>787111</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F18">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M18">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N18">
         <v>100</v>
@@ -1613,48 +1616,48 @@
         <v>87</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q18">
-        <v>846540</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D19">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M19">
         <v>17000</v>
@@ -1663,13 +1666,13 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="P19" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="Q19">
-        <v>1119600</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1677,40 +1680,40 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="E20" t="s">
         <v>71</v>
       </c>
       <c r="F20">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M20">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N20">
         <v>100</v>
@@ -1722,7 +1725,7 @@
         <v>30</v>
       </c>
       <c r="Q20">
-        <v>2880000</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1730,52 +1733,52 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F21">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M21">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="P21" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="Q21">
-        <v>577500</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1783,40 +1786,40 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F22">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M22">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N22">
         <v>100</v>
@@ -1828,7 +1831,7 @@
         <v>32</v>
       </c>
       <c r="Q22">
-        <v>1300000</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1836,52 +1839,52 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D23">
-        <v>442.659</v>
+        <v>53.9</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F23">
-        <v>442.659</v>
+        <v>53.9</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M23">
-        <v>10700</v>
+        <v>7000</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="P23" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="Q23">
-        <v>3102750</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1889,40 +1892,40 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>80</v>
+        <v>520</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F24">
-        <v>80</v>
+        <v>520</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M24">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N24">
         <v>100</v>
@@ -1934,7 +1937,7 @@
         <v>34</v>
       </c>
       <c r="Q24">
-        <v>3000000</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1942,155 +1945,155 @@
         <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>61</v>
       </c>
       <c r="D25">
-        <v>4212</v>
+        <v>442.659</v>
       </c>
       <c r="E25" t="s">
         <v>66</v>
       </c>
       <c r="F25">
-        <v>1263.6</v>
+        <v>442.659</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M25">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="N25">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="P25" t="s">
         <v>94</v>
       </c>
       <c r="Q25">
-        <v>87871545</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
         <v>61</v>
       </c>
       <c r="D26">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F26">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M26">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N26">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O26" t="s">
         <v>91</v>
       </c>
       <c r="P26" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="Q26">
-        <v>87871545</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27">
         <v>4212</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F27">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M27">
         <v>26000</v>
       </c>
       <c r="N27">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q27">
         <v>87871545</v>
@@ -2098,52 +2101,52 @@
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D28">
         <v>4212</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28">
-        <v>421.2</v>
+        <v>1263.6</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="L28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M28">
         <v>26000</v>
       </c>
       <c r="N28">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q28">
         <v>87871545</v>
@@ -2151,40 +2154,40 @@
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>4212</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F29">
         <v>421.2</v>
       </c>
       <c r="G29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M29">
         <v>26000</v>
@@ -2193,10 +2196,10 @@
         <v>10</v>
       </c>
       <c r="O29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q29">
         <v>87871545</v>
@@ -2204,52 +2207,52 @@
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D30">
         <v>4212</v>
       </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F30">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K30" t="s">
         <v>80</v>
       </c>
       <c r="L30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M30">
         <v>26000</v>
       </c>
       <c r="N30">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q30">
         <v>87871545</v>
@@ -2257,13 +2260,13 @@
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D31">
         <v>4212</v>
@@ -2272,37 +2275,37 @@
         <v>75</v>
       </c>
       <c r="F31">
-        <v>126.36</v>
+        <v>421.2</v>
       </c>
       <c r="G31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K31" t="s">
         <v>80</v>
       </c>
       <c r="L31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M31">
         <v>26000</v>
       </c>
       <c r="N31">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q31">
         <v>87871545</v>
@@ -2310,13 +2313,13 @@
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32">
         <v>4212</v>
@@ -2328,22 +2331,22 @@
         <v>126.36</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M32">
         <v>26000</v>
@@ -2352,10 +2355,10 @@
         <v>3</v>
       </c>
       <c r="O32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q32">
         <v>87871545</v>
@@ -2363,13 +2366,13 @@
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D33">
         <v>4212</v>
@@ -2378,37 +2381,37 @@
         <v>76</v>
       </c>
       <c r="F33">
-        <v>42.12</v>
+        <v>126.36</v>
       </c>
       <c r="G33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M33">
         <v>26000</v>
       </c>
       <c r="N33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q33">
         <v>87871545</v>
@@ -2416,46 +2419,46 @@
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D34">
-        <v>360</v>
+        <v>4212</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F34">
-        <v>360</v>
+        <v>126.36</v>
       </c>
       <c r="G34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K34" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M34">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N34">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O34" t="s">
         <v>92</v>
@@ -2464,51 +2467,51 @@
         <v>95</v>
       </c>
       <c r="Q34">
-        <v>13500000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D35">
-        <v>187.5</v>
+        <v>4212</v>
       </c>
       <c r="E35" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F35">
-        <v>187.5</v>
+        <v>42.12</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K35" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M35">
-        <v>12500</v>
+        <v>26000</v>
       </c>
       <c r="N35">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="O35" t="s">
         <v>92</v>
@@ -2517,60 +2520,60 @@
         <v>95</v>
       </c>
       <c r="Q35">
-        <v>1020000</v>
+        <v>87871545</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D36">
-        <v>336</v>
+        <v>360</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F36">
-        <v>336</v>
+        <v>360</v>
       </c>
       <c r="G36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M36">
-        <v>15000</v>
+        <v>2000</v>
       </c>
       <c r="N36">
         <v>100</v>
       </c>
       <c r="O36" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q36">
-        <v>1619200</v>
+        <v>13500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-26
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="92">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
     <t>2023-11-20</t>
   </si>
   <si>
@@ -121,190 +124,172 @@
     <t>2023-10-13</t>
   </si>
   <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>에이치엠씨제6호스팩</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>현대차</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-10-10</t>
+  </si>
+  <si>
     <t>2023-10-05</t>
   </si>
   <si>
+    <t>2023-09-25</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-10-11</t>
+  </si>
+  <si>
     <t>2023-10-04</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>두산로보틱스</t>
-  </si>
-  <si>
-    <t>신한제11호스팩</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유비에스</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
-    <t>2023-10-10</t>
-  </si>
-  <si>
-    <t>2023-09-25</t>
-  </si>
-  <si>
-    <t>2023-09-21</t>
-  </si>
-  <si>
-    <t>2023-09-19</t>
-  </si>
-  <si>
-    <t>2023-10-11</t>
-  </si>
-  <si>
-    <t>2023-09-26</t>
-  </si>
-  <si>
-    <t>2023-09-22</t>
   </si>
 </sst>
 </file>
@@ -662,7 +647,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -726,52 +711,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M2">
-        <v>11000</v>
+        <v>17000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="Q2">
-        <v>2374500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -779,158 +764,158 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M3">
-        <v>34700</v>
+        <v>11000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
       <c r="Q3">
-        <v>1537150</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M4">
-        <v>30000</v>
+        <v>7000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="Q4">
-        <v>1072999</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>4192.2496</v>
+        <v>721.413</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5">
-        <v>2846.537406</v>
+        <v>721.413</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M5">
-        <v>36200</v>
+        <v>34700</v>
       </c>
       <c r="N5">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>83</v>
+        <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q5">
-        <v>19108320</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -941,99 +926,99 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <v>441.12</v>
+      </c>
+      <c r="E6" t="s">
         <v>62</v>
       </c>
-      <c r="D6">
-        <v>4192.2496</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
-      </c>
       <c r="F6">
-        <v>1219.944706</v>
+        <v>441.12</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M6">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N6">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Q6">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <v>4192.2496</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F7">
-        <v>125.767488</v>
+        <v>2846.537406</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="L7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M7">
         <v>36200</v>
       </c>
       <c r="N7">
-        <v>3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q7">
         <v>19108320</v>
@@ -1050,99 +1035,99 @@
         <v>61</v>
       </c>
       <c r="D8">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F8">
-        <v>63.84</v>
+        <v>1219.944706</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M8">
+        <v>36200</v>
+      </c>
+      <c r="N8">
+        <v>29.1</v>
+      </c>
+      <c r="O8" t="s">
         <v>79</v>
       </c>
-      <c r="L8" t="s">
-        <v>78</v>
-      </c>
-      <c r="M8">
-        <v>4000</v>
-      </c>
-      <c r="N8">
-        <v>100</v>
-      </c>
-      <c r="O8" t="s">
-        <v>84</v>
-      </c>
       <c r="P8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
         <v>61</v>
       </c>
       <c r="D9">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9">
-        <v>160</v>
+        <v>125.767488</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M9">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N9">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="P9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="Q9">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1153,49 +1138,49 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F10">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M10">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N10">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="P10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="Q10">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1206,49 +1191,49 @@
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F11">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" t="s">
         <v>78</v>
       </c>
-      <c r="H11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I11" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K11" t="s">
-        <v>79</v>
-      </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M11">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N11">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O11" t="s">
+        <v>81</v>
+      </c>
+      <c r="P11" t="s">
         <v>28</v>
       </c>
-      <c r="P11" t="s">
-        <v>26</v>
-      </c>
       <c r="Q11">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1256,52 +1241,52 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F12">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" t="s">
+        <v>74</v>
+      </c>
+      <c r="K12" t="s">
         <v>78</v>
       </c>
-      <c r="H12" t="s">
-        <v>78</v>
-      </c>
-      <c r="I12" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K12" t="s">
-        <v>79</v>
-      </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N12">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="P12" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="Q12">
-        <v>3000000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1309,370 +1294,370 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F13">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M13">
-        <v>1800</v>
+        <v>25000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="P13" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="Q13">
-        <v>4550000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F14">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M14">
-        <v>4800</v>
+        <v>2000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="P14" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="Q14">
-        <v>3900000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F15">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M15">
-        <v>22500</v>
+        <v>1800</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="P15" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="Q15">
-        <v>1545000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F16">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M16">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q16">
-        <v>840000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
       </c>
       <c r="F17">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M17">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="P17" t="s">
-        <v>85</v>
+        <v>28</v>
       </c>
       <c r="Q17">
-        <v>2600000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F18">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="P18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q18">
-        <v>9375000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="E19" t="s">
         <v>65</v>
       </c>
       <c r="F19">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M19">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="P19" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="Q19">
-        <v>787111</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1680,52 +1665,52 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F20">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M20">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="P20" t="s">
         <v>30</v>
       </c>
       <c r="Q20">
-        <v>846540</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1733,37 +1718,37 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F21">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M21">
         <v>17000</v>
@@ -1772,331 +1757,331 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="P21" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="Q21">
-        <v>1119600</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F22">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M22">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="P22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q22">
-        <v>2880000</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F23">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M23">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
       <c r="P23" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="Q23">
-        <v>577500</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D24">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F24">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M24">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="P24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q24">
-        <v>1300000</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25">
-        <v>442.659</v>
+        <v>53.9</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F25">
-        <v>442.659</v>
+        <v>53.9</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L25" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M25">
-        <v>10700</v>
+        <v>7000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
+        <v>86</v>
+      </c>
+      <c r="P25" t="s">
         <v>35</v>
       </c>
-      <c r="P25" t="s">
-        <v>94</v>
-      </c>
       <c r="Q25">
-        <v>3102750</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26">
-        <v>80</v>
+        <v>520</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F26">
-        <v>80</v>
+        <v>520</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L26" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M26">
-        <v>2000</v>
+        <v>26000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="P26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q26">
-        <v>3000000</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27">
-        <v>4212</v>
+        <v>442.659</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F27">
-        <v>1263.6</v>
+        <v>442.659</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M27">
-        <v>26000</v>
+        <v>10700</v>
       </c>
       <c r="N27">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="P27" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="Q27">
-        <v>87871545</v>
+        <v>3102750</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2107,473 +2092,49 @@
         <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D28">
-        <v>4212</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F28">
-        <v>1263.6</v>
+        <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="K28" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="L28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="M28">
-        <v>26000</v>
+        <v>2000</v>
       </c>
       <c r="N28">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P28" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="Q28">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29">
-        <v>4212</v>
-      </c>
-      <c r="E29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29">
-        <v>421.2</v>
-      </c>
-      <c r="G29" t="s">
-        <v>78</v>
-      </c>
-      <c r="H29" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" t="s">
-        <v>78</v>
-      </c>
-      <c r="J29" t="s">
-        <v>78</v>
-      </c>
-      <c r="K29" t="s">
-        <v>80</v>
-      </c>
-      <c r="L29" t="s">
-        <v>78</v>
-      </c>
-      <c r="M29">
-        <v>26000</v>
-      </c>
-      <c r="N29">
-        <v>10</v>
-      </c>
-      <c r="O29" t="s">
-        <v>92</v>
-      </c>
-      <c r="P29" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q29">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30">
-        <v>4212</v>
-      </c>
-      <c r="E30" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30">
-        <v>421.2</v>
-      </c>
-      <c r="G30" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I30" t="s">
-        <v>78</v>
-      </c>
-      <c r="J30" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" t="s">
-        <v>80</v>
-      </c>
-      <c r="L30" t="s">
-        <v>78</v>
-      </c>
-      <c r="M30">
-        <v>26000</v>
-      </c>
-      <c r="N30">
-        <v>10</v>
-      </c>
-      <c r="O30" t="s">
-        <v>92</v>
-      </c>
-      <c r="P30" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q30">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31">
-        <v>4212</v>
-      </c>
-      <c r="E31" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31">
-        <v>421.2</v>
-      </c>
-      <c r="G31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" t="s">
-        <v>78</v>
-      </c>
-      <c r="K31" t="s">
-        <v>80</v>
-      </c>
-      <c r="L31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31">
-        <v>26000</v>
-      </c>
-      <c r="N31">
-        <v>10</v>
-      </c>
-      <c r="O31" t="s">
-        <v>92</v>
-      </c>
-      <c r="P31" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q31">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32">
-        <v>4212</v>
-      </c>
-      <c r="E32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32">
-        <v>126.36</v>
-      </c>
-      <c r="G32" t="s">
-        <v>78</v>
-      </c>
-      <c r="H32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I32" t="s">
-        <v>78</v>
-      </c>
-      <c r="J32" t="s">
-        <v>78</v>
-      </c>
-      <c r="K32" t="s">
-        <v>81</v>
-      </c>
-      <c r="L32" t="s">
-        <v>78</v>
-      </c>
-      <c r="M32">
-        <v>26000</v>
-      </c>
-      <c r="N32">
-        <v>3</v>
-      </c>
-      <c r="O32" t="s">
-        <v>92</v>
-      </c>
-      <c r="P32" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q32">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33">
-        <v>4212</v>
-      </c>
-      <c r="E33" t="s">
-        <v>76</v>
-      </c>
-      <c r="F33">
-        <v>126.36</v>
-      </c>
-      <c r="G33" t="s">
-        <v>78</v>
-      </c>
-      <c r="H33" t="s">
-        <v>78</v>
-      </c>
-      <c r="I33" t="s">
-        <v>78</v>
-      </c>
-      <c r="J33" t="s">
-        <v>78</v>
-      </c>
-      <c r="K33" t="s">
-        <v>81</v>
-      </c>
-      <c r="L33" t="s">
-        <v>78</v>
-      </c>
-      <c r="M33">
-        <v>26000</v>
-      </c>
-      <c r="N33">
-        <v>3</v>
-      </c>
-      <c r="O33" t="s">
-        <v>92</v>
-      </c>
-      <c r="P33" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q33">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34">
-        <v>4212</v>
-      </c>
-      <c r="E34" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34">
-        <v>126.36</v>
-      </c>
-      <c r="G34" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" t="s">
-        <v>78</v>
-      </c>
-      <c r="I34" t="s">
-        <v>78</v>
-      </c>
-      <c r="J34" t="s">
-        <v>78</v>
-      </c>
-      <c r="K34" t="s">
-        <v>81</v>
-      </c>
-      <c r="L34" t="s">
-        <v>78</v>
-      </c>
-      <c r="M34">
-        <v>26000</v>
-      </c>
-      <c r="N34">
-        <v>3</v>
-      </c>
-      <c r="O34" t="s">
-        <v>92</v>
-      </c>
-      <c r="P34" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q34">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35">
-        <v>4212</v>
-      </c>
-      <c r="E35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F35">
-        <v>42.12</v>
-      </c>
-      <c r="G35" t="s">
-        <v>78</v>
-      </c>
-      <c r="H35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I35" t="s">
-        <v>78</v>
-      </c>
-      <c r="J35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K35" t="s">
-        <v>81</v>
-      </c>
-      <c r="L35" t="s">
-        <v>78</v>
-      </c>
-      <c r="M35">
-        <v>26000</v>
-      </c>
-      <c r="N35">
-        <v>1</v>
-      </c>
-      <c r="O35" t="s">
-        <v>92</v>
-      </c>
-      <c r="P35" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q35">
-        <v>87871545</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36">
-        <v>360</v>
-      </c>
-      <c r="E36" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36">
-        <v>360</v>
-      </c>
-      <c r="G36" t="s">
-        <v>78</v>
-      </c>
-      <c r="H36" t="s">
-        <v>78</v>
-      </c>
-      <c r="I36" t="s">
-        <v>78</v>
-      </c>
-      <c r="J36" t="s">
-        <v>78</v>
-      </c>
-      <c r="K36" t="s">
-        <v>79</v>
-      </c>
-      <c r="L36" t="s">
-        <v>78</v>
-      </c>
-      <c r="M36">
-        <v>2000</v>
-      </c>
-      <c r="N36">
-        <v>100</v>
-      </c>
-      <c r="O36" t="s">
-        <v>93</v>
-      </c>
-      <c r="P36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q36">
-        <v>13500000</v>
+        <v>3000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-11-29
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="94">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
     <t>2023-11-24</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     <t>2023-10-13</t>
   </si>
   <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
     <t>그린리소스</t>
   </si>
   <si>
@@ -202,6 +208,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>미래</t>
+  </si>
+  <si>
     <t>NH</t>
   </si>
   <si>
@@ -214,9 +223,6 @@
     <t>KB</t>
   </si>
   <si>
-    <t>미래</t>
-  </si>
-  <si>
     <t>삼성</t>
   </si>
   <si>
@@ -253,6 +259,9 @@
     <t>공동대표</t>
   </si>
   <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
     <t>2023-11-08</t>
   </si>
   <si>
@@ -281,9 +290,6 @@
   </si>
   <si>
     <t>2023-09-25</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
   </si>
   <si>
     <t>2023-10-11</t>
@@ -647,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -711,52 +717,52 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D2">
-        <v>278.8</v>
+        <v>393.96</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F2">
-        <v>278.8</v>
+        <v>393.96</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M2">
-        <v>17000</v>
+        <v>28000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="P2" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="Q2">
-        <v>1221420</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -764,93 +770,93 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D3">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M3">
-        <v>11000</v>
+        <v>17000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="Q3">
-        <v>2374500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D4">
-        <v>297.5</v>
+        <v>368.5</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F4">
-        <v>297.5</v>
+        <v>368.5</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M4">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="N4">
         <v>100</v>
@@ -859,63 +865,63 @@
         <v>24</v>
       </c>
       <c r="P4" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="Q4">
-        <v>3187500</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D5">
-        <v>721.413</v>
+        <v>297.5</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F5">
-        <v>721.413</v>
+        <v>297.5</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M5">
-        <v>34700</v>
+        <v>7000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="Q5">
-        <v>1537150</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -923,52 +929,52 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D6">
-        <v>441.12</v>
+        <v>721.413</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F6">
-        <v>441.12</v>
+        <v>721.413</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M6">
-        <v>30000</v>
+        <v>34700</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" t="s">
         <v>23</v>
       </c>
-      <c r="P6" t="s">
-        <v>25</v>
-      </c>
       <c r="Q6">
-        <v>1072999</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -976,102 +982,102 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D7">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7">
-        <v>2846.537406</v>
+        <v>441.12</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M7">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N7">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q7">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>4192.2496</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F8">
-        <v>1219.944706</v>
+        <v>2846.537406</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M8">
         <v>36200</v>
       </c>
       <c r="N8">
-        <v>29.1</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O8" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q8">
         <v>19108320</v>
@@ -1079,52 +1085,52 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D9">
         <v>4192.2496</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F9">
-        <v>125.767488</v>
+        <v>1219.944706</v>
       </c>
       <c r="G9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M9">
         <v>36200</v>
       </c>
       <c r="N9">
-        <v>3</v>
+        <v>29.1</v>
       </c>
       <c r="O9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9">
         <v>19108320</v>
@@ -1135,52 +1141,52 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D10">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F10">
-        <v>63.84</v>
+        <v>125.767488</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K10" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M10">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N10">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="Q10">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1188,90 +1194,90 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M11">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N11">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="Q11">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D12">
         <v>320</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F12">
         <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M12">
         <v>20000</v>
@@ -1280,10 +1286,10 @@
         <v>50</v>
       </c>
       <c r="O12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q12">
         <v>2254770</v>
@@ -1294,105 +1300,105 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D13">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F13">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M13">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N13">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O13" t="s">
+        <v>84</v>
+      </c>
+      <c r="P13" t="s">
         <v>29</v>
       </c>
-      <c r="P13" t="s">
-        <v>27</v>
-      </c>
       <c r="Q13">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D14">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F14">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="Q14">
-        <v>3000000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1400,52 +1406,52 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D15">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F15">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K15" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M15">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Q15">
-        <v>4550000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1453,211 +1459,211 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F16">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="G16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M16">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P16" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="Q16">
-        <v>3900000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F17">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M17">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q17">
-        <v>1545000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="G18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K18" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M18">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q18">
-        <v>840000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F19">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K19" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M19">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>31</v>
+        <v>84</v>
       </c>
       <c r="P19" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="Q19">
-        <v>2600000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1665,52 +1671,52 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D20">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F20">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="P20" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="Q20">
-        <v>9375000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1718,105 +1724,105 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F21">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M21">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P21" t="s">
         <v>31</v>
       </c>
       <c r="Q21">
-        <v>787111</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D22">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F22">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="G22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K22" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M22">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q22">
-        <v>846540</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1824,52 +1830,52 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D23">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F23">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M23">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="P23" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="Q23">
-        <v>1119600</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1877,52 +1883,52 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D24">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M24">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="P24" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="Q24">
-        <v>2880000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1930,52 +1936,52 @@
         <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D25">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F25">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M25">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="P25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q25">
-        <v>577500</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1983,52 +1989,52 @@
         <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D26">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F26">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K26" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M26">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="P26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q26">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2036,52 +2042,52 @@
         <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D27">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F27">
-        <v>442.659</v>
+        <v>520</v>
       </c>
       <c r="G27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K27" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M27">
-        <v>10700</v>
+        <v>26000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P27" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="Q27">
-        <v>3102750</v>
+        <v>1300000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2089,51 +2095,104 @@
         <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D28">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F28">
-        <v>80</v>
+        <v>442.659</v>
       </c>
       <c r="G28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K28" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M28">
-        <v>2000</v>
+        <v>10700</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P28" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q28">
+        <v>3102750</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29">
+        <v>80</v>
+      </c>
+      <c r="G29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" t="s">
+        <v>76</v>
+      </c>
+      <c r="I29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J29" t="s">
+        <v>76</v>
+      </c>
+      <c r="K29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L29" t="s">
+        <v>76</v>
+      </c>
+      <c r="M29">
+        <v>2000</v>
+      </c>
+      <c r="N29">
+        <v>100</v>
+      </c>
+      <c r="O29" t="s">
         <v>91</v>
       </c>
-      <c r="Q28">
+      <c r="P29" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q29">
         <v>3000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-03
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="97">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-12-01</t>
+  </si>
+  <si>
     <t>2023-11-28</t>
   </si>
   <si>
@@ -127,6 +130,12 @@
     <t>2023-10-13</t>
   </si>
   <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
     <t>에이에스텍</t>
   </si>
   <si>
@@ -208,12 +217,15 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>미래</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>하이</t>
   </si>
   <si>
@@ -236,9 +248,6 @@
   </si>
   <si>
     <t>키움</t>
-  </si>
-  <si>
-    <t>하나</t>
   </si>
   <si>
     <t>현대차</t>
@@ -653,7 +662,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -717,211 +726,211 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D2">
-        <v>393.96</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F2">
-        <v>393.96</v>
+        <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M2">
-        <v>28000</v>
+        <v>18000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2">
-        <v>1055250</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D3">
-        <v>278.8</v>
+        <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F3">
-        <v>278.8</v>
+        <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M3">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="Q3">
-        <v>1221420</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D4">
-        <v>368.5</v>
+        <v>393.96</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F4">
-        <v>368.5</v>
+        <v>393.96</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M4">
-        <v>11000</v>
+        <v>28000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="P4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Q4">
-        <v>2374500</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D5">
-        <v>297.5</v>
+        <v>278.8</v>
       </c>
       <c r="E5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F5">
-        <v>297.5</v>
+        <v>278.8</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M5">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Q5">
-        <v>3187500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -929,158 +938,158 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D6">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F6">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M6">
-        <v>34700</v>
+        <v>11000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
         <v>27</v>
       </c>
-      <c r="P6" t="s">
-        <v>23</v>
-      </c>
       <c r="Q6">
-        <v>1537150</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="F7">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M7">
-        <v>30000</v>
+        <v>7000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="Q7">
-        <v>1072999</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D8">
-        <v>4192.2496</v>
+        <v>721.413</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F8">
-        <v>2846.537406</v>
+        <v>721.413</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M8">
-        <v>36200</v>
+        <v>34700</v>
       </c>
       <c r="N8">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="P8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>19108320</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1088,102 +1097,102 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D9">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F9">
-        <v>1219.944706</v>
+        <v>441.12</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M9">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N9">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q9">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>4192.2496</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>125.767488</v>
+        <v>2846.537406</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M10">
         <v>36200</v>
       </c>
       <c r="N10">
-        <v>3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O10" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q10">
         <v>19108320</v>
@@ -1194,105 +1203,105 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D11">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F11">
-        <v>63.84</v>
+        <v>1219.944706</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K11" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M11">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N11">
-        <v>100</v>
+        <v>29.1</v>
       </c>
       <c r="O11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="Q11">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D12">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F12">
-        <v>160</v>
+        <v>125.767488</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M12">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N12">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Q12">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1300,52 +1309,52 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D13">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F13">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K13" t="s">
         <v>80</v>
       </c>
       <c r="L13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M13">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N13">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Q13">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1353,52 +1362,52 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E14" t="s">
         <v>69</v>
       </c>
       <c r="F14">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K14" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="L14" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M14">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N14">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O14" t="s">
+        <v>87</v>
+      </c>
+      <c r="P14" t="s">
         <v>30</v>
       </c>
-      <c r="P14" t="s">
-        <v>28</v>
-      </c>
       <c r="Q14">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1406,52 +1415,52 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D15">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F15">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K15" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="L15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N15">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O15" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="P15" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="Q15">
-        <v>3000000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1459,370 +1468,370 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D16">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F16">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M16">
-        <v>1800</v>
+        <v>25000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="P16" t="s">
-        <v>83</v>
+        <v>29</v>
       </c>
       <c r="Q16">
-        <v>4550000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D17">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F17">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M17">
-        <v>4800</v>
+        <v>2000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P17" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="Q17">
-        <v>3900000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D18">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F18">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K18" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M18">
-        <v>22500</v>
+        <v>1800</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P18" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="Q18">
-        <v>1545000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D19">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F19">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L19" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M19">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q19">
-        <v>840000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D20">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F20">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="G20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M20">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="P20" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="Q20">
-        <v>2600000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D21">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="E21" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F21">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M21">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q21">
-        <v>9375000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D22">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="F22">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K22" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M22">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22" t="s">
         <v>87</v>
       </c>
-      <c r="P22" t="s">
-        <v>32</v>
-      </c>
       <c r="Q22">
-        <v>787111</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1830,52 +1839,52 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D23">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="E23" t="s">
         <v>72</v>
       </c>
       <c r="F23">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K23" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M23">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P23" t="s">
         <v>32</v>
       </c>
       <c r="Q23">
-        <v>846540</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1883,37 +1892,37 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D24">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="E24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F24">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="G24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K24" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M24">
         <v>17000</v>
@@ -1922,277 +1931,383 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="P24" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="Q24">
-        <v>1119600</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D25">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F25">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K25" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M25">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q25">
-        <v>2880000</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="E26" t="s">
         <v>74</v>
       </c>
       <c r="F26">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M26">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="P26" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="Q26">
-        <v>577500</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D27">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="E27" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F27">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="G27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K27" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M27">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q27">
-        <v>1300000</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D28">
-        <v>442.659</v>
+        <v>53.9</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F28">
-        <v>442.659</v>
+        <v>53.9</v>
       </c>
       <c r="G28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K28" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="L28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M28">
-        <v>10700</v>
+        <v>7000</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="P28" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="Q28">
-        <v>3102750</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>520</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29">
+        <v>520</v>
+      </c>
+      <c r="G29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" t="s">
+        <v>80</v>
+      </c>
+      <c r="L29" t="s">
+        <v>79</v>
+      </c>
+      <c r="M29">
+        <v>26000</v>
+      </c>
+      <c r="N29">
+        <v>100</v>
+      </c>
+      <c r="O29" t="s">
+        <v>92</v>
+      </c>
+      <c r="P29" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q29">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
         <v>36</v>
       </c>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29">
-        <v>80</v>
-      </c>
-      <c r="E29" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29">
-        <v>80</v>
-      </c>
-      <c r="G29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" t="s">
-        <v>76</v>
-      </c>
-      <c r="K29" t="s">
-        <v>77</v>
-      </c>
-      <c r="L29" t="s">
-        <v>76</v>
-      </c>
-      <c r="M29">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30">
+        <v>442.659</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30">
+        <v>442.659</v>
+      </c>
+      <c r="G30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" t="s">
+        <v>79</v>
+      </c>
+      <c r="J30" t="s">
+        <v>79</v>
+      </c>
+      <c r="K30" t="s">
+        <v>80</v>
+      </c>
+      <c r="L30" t="s">
+        <v>79</v>
+      </c>
+      <c r="M30">
+        <v>10700</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
+      </c>
+      <c r="O30" t="s">
+        <v>93</v>
+      </c>
+      <c r="P30" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q30">
+        <v>3102750</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31">
+        <v>80</v>
+      </c>
+      <c r="E31" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31">
+        <v>80</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K31" t="s">
+        <v>80</v>
+      </c>
+      <c r="L31" t="s">
+        <v>79</v>
+      </c>
+      <c r="M31">
         <v>2000</v>
       </c>
-      <c r="N29">
-        <v>100</v>
-      </c>
-      <c r="O29" t="s">
-        <v>91</v>
-      </c>
-      <c r="P29" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q29">
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>94</v>
+      </c>
+      <c r="P31" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q31">
         <v>3000000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-04
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="93">
   <si>
     <t>상장일</t>
   </si>
@@ -127,184 +127,172 @@
     <t>2023-10-18</t>
   </si>
   <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>퓨릿</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-10-10</t>
+  </si>
+  <si>
+    <t>2023-10-05</t>
+  </si>
+  <si>
     <t>2023-10-13</t>
   </si>
   <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>에이치엠씨제6호스팩</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>현대차</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
-    <t>2023-10-10</t>
-  </si>
-  <si>
-    <t>2023-10-05</t>
-  </si>
-  <si>
-    <t>2023-09-25</t>
-  </si>
-  <si>
     <t>2023-10-11</t>
-  </si>
-  <si>
-    <t>2023-10-04</t>
   </si>
 </sst>
 </file>
@@ -662,7 +650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -726,37 +714,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2">
         <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>117</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M2">
         <v>18000</v>
@@ -779,37 +767,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>160</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F3">
         <v>160</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M3">
         <v>2000</v>
@@ -832,37 +820,37 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>393.96</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F4">
         <v>393.96</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M4">
         <v>28000</v>
@@ -871,7 +859,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
@@ -885,37 +873,37 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>278.8</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5">
         <v>278.8</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M5">
         <v>17000</v>
@@ -927,7 +915,7 @@
         <v>26</v>
       </c>
       <c r="P5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q5">
         <v>1221420</v>
@@ -938,37 +926,37 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>368.5</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F6">
         <v>368.5</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M6">
         <v>11000</v>
@@ -991,37 +979,37 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>297.5</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F7">
         <v>297.5</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M7">
         <v>7000</v>
@@ -1033,7 +1021,7 @@
         <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="Q7">
         <v>3187500</v>
@@ -1044,37 +1032,37 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>721.413</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8">
         <v>721.413</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M8">
         <v>34700</v>
@@ -1097,37 +1085,37 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9">
         <v>441.12</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9">
         <v>441.12</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M9">
         <v>30000</v>
@@ -1150,37 +1138,37 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10">
         <v>4192.2496</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F10">
         <v>2846.537406</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M10">
         <v>36200</v>
@@ -1189,7 +1177,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="P10" t="s">
         <v>26</v>
@@ -1203,37 +1191,37 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D11">
         <v>4192.2496</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11">
         <v>1219.944706</v>
       </c>
       <c r="G11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M11">
         <v>36200</v>
@@ -1242,7 +1230,7 @@
         <v>29.1</v>
       </c>
       <c r="O11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="P11" t="s">
         <v>26</v>
@@ -1256,37 +1244,37 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>4192.2496</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F12">
         <v>125.767488</v>
       </c>
       <c r="G12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" t="s">
         <v>79</v>
       </c>
-      <c r="H12" t="s">
-        <v>79</v>
-      </c>
-      <c r="I12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" t="s">
-        <v>79</v>
-      </c>
-      <c r="K12" t="s">
-        <v>82</v>
-      </c>
       <c r="L12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M12">
         <v>36200</v>
@@ -1295,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="P12" t="s">
         <v>26</v>
@@ -1309,37 +1297,37 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D13">
         <v>63.84</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13">
         <v>63.84</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M13">
         <v>4000</v>
@@ -1348,7 +1336,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P13" t="s">
         <v>25</v>
@@ -1362,37 +1350,37 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>320</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F14">
         <v>160</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M14">
         <v>20000</v>
@@ -1401,7 +1389,7 @@
         <v>50</v>
       </c>
       <c r="O14" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P14" t="s">
         <v>30</v>
@@ -1415,37 +1403,37 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15">
         <v>320</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15">
         <v>160</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L15" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M15">
         <v>20000</v>
@@ -1454,7 +1442,7 @@
         <v>50</v>
       </c>
       <c r="O15" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P15" t="s">
         <v>30</v>
@@ -1468,37 +1456,37 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D16">
         <v>659.0825</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F16">
         <v>659.0825</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M16">
         <v>25000</v>
@@ -1521,37 +1509,37 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D17">
         <v>80</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F17">
         <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M17">
         <v>2000</v>
@@ -1560,10 +1548,10 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Q17">
         <v>3000000</v>
@@ -1574,37 +1562,37 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>126</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F18">
         <v>126</v>
       </c>
       <c r="G18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M18">
         <v>1800</v>
@@ -1613,10 +1601,10 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P18" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="Q18">
         <v>4550000</v>
@@ -1627,37 +1615,37 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D19">
         <v>249.6</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F19">
         <v>249.6</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M19">
         <v>4800</v>
@@ -1666,7 +1654,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P19" t="s">
         <v>30</v>
@@ -1680,37 +1668,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D20">
         <v>463.5</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F20">
         <v>463.5</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K20" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M20">
         <v>22500</v>
@@ -1719,7 +1707,7 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P20" t="s">
         <v>30</v>
@@ -1733,37 +1721,37 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D21">
         <v>156</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F21">
         <v>156</v>
       </c>
       <c r="G21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M21">
         <v>13000</v>
@@ -1772,7 +1760,7 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P21" t="s">
         <v>30</v>
@@ -1786,37 +1774,37 @@
         <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22">
         <v>270</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F22">
         <v>270</v>
       </c>
       <c r="G22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M22">
         <v>7500</v>
@@ -1828,7 +1816,7 @@
         <v>33</v>
       </c>
       <c r="P22" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q22">
         <v>2600000</v>
@@ -1839,37 +1827,37 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23">
         <v>250</v>
       </c>
       <c r="E23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F23">
         <v>250</v>
       </c>
       <c r="G23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1878,7 +1866,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P23" t="s">
         <v>32</v>
@@ -1892,37 +1880,37 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <v>178.41194</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F24">
         <v>178.41194</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M24">
         <v>17000</v>
@@ -1931,7 +1919,7 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P24" t="s">
         <v>33</v>
@@ -1945,37 +1933,37 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D25">
         <v>49.66368</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F25">
         <v>49.66368</v>
       </c>
       <c r="G25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M25">
         <v>4400</v>
@@ -1984,7 +1972,7 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P25" t="s">
         <v>33</v>
@@ -1998,37 +1986,37 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <v>306</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F26">
         <v>306</v>
       </c>
       <c r="G26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M26">
         <v>17000</v>
@@ -2040,7 +2028,7 @@
         <v>36</v>
       </c>
       <c r="P26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Q26">
         <v>1119600</v>
@@ -2051,37 +2039,37 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D27">
         <v>260</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F27">
         <v>260</v>
       </c>
       <c r="G27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M27">
         <v>6500</v>
@@ -2090,7 +2078,7 @@
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="P27" t="s">
         <v>35</v>
@@ -2104,37 +2092,37 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28">
         <v>53.9</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F28">
         <v>53.9</v>
       </c>
       <c r="G28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K28" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M28">
         <v>7000</v>
@@ -2143,10 +2131,10 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P28" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="Q28">
         <v>577500</v>
@@ -2157,37 +2145,37 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D29">
         <v>520</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F29">
         <v>520</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M29">
         <v>26000</v>
@@ -2196,10 +2184,10 @@
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="P29" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="Q29">
         <v>1300000</v>
@@ -2210,37 +2198,37 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D30">
         <v>442.659</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F30">
         <v>442.659</v>
       </c>
       <c r="G30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="K30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M30">
         <v>10700</v>
@@ -2249,66 +2237,13 @@
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="P30" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q30">
         <v>3102750</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31">
-        <v>80</v>
-      </c>
-      <c r="E31" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31">
-        <v>80</v>
-      </c>
-      <c r="G31" t="s">
-        <v>79</v>
-      </c>
-      <c r="H31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" t="s">
-        <v>79</v>
-      </c>
-      <c r="J31" t="s">
-        <v>79</v>
-      </c>
-      <c r="K31" t="s">
-        <v>80</v>
-      </c>
-      <c r="L31" t="s">
-        <v>79</v>
-      </c>
-      <c r="M31">
-        <v>2000</v>
-      </c>
-      <c r="N31">
-        <v>100</v>
-      </c>
-      <c r="O31" t="s">
-        <v>94</v>
-      </c>
-      <c r="P31" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q31">
-        <v>3000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-05
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="96">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-12-04</t>
+  </si>
+  <si>
     <t>2023-12-01</t>
   </si>
   <si>
@@ -127,6 +130,9 @@
     <t>2023-10-18</t>
   </si>
   <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
     <t>에이텀</t>
   </si>
   <si>
@@ -211,6 +217,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>삼성</t>
+  </si>
+  <si>
     <t>하나</t>
   </si>
   <si>
@@ -229,9 +238,6 @@
     <t>KB</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
     <t>한국</t>
   </si>
   <si>
@@ -257,6 +263,9 @@
   </si>
   <si>
     <t>공동대표</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
   </si>
   <si>
     <t>2023-11-16</t>
@@ -650,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -714,105 +723,105 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F2">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M2">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N2">
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="P2" t="s">
         <v>19</v>
       </c>
       <c r="Q2">
-        <v>487500</v>
+        <v>7500000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F3">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q3">
-        <v>6000000</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -820,52 +829,52 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D4">
-        <v>393.96</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F4">
-        <v>393.96</v>
+        <v>160</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M4">
-        <v>28000</v>
+        <v>2000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4">
-        <v>1055250</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -873,52 +882,52 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D5">
-        <v>278.8</v>
+        <v>393.96</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F5">
-        <v>278.8</v>
+        <v>393.96</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M5">
-        <v>17000</v>
+        <v>28000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="P5" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="Q5">
-        <v>1221420</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -926,93 +935,93 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F6">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M6">
-        <v>11000</v>
+        <v>17000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P6" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="Q6">
-        <v>2374500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D7">
-        <v>297.5</v>
+        <v>368.5</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F7">
-        <v>297.5</v>
+        <v>368.5</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M7">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="N7">
         <v>100</v>
@@ -1021,63 +1030,63 @@
         <v>26</v>
       </c>
       <c r="P7" t="s">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="Q7">
-        <v>3187500</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D8">
-        <v>721.413</v>
+        <v>297.5</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F8">
-        <v>721.413</v>
+        <v>297.5</v>
       </c>
       <c r="G8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M8">
-        <v>34700</v>
+        <v>7000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="Q8">
-        <v>1537150</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1085,52 +1094,52 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9">
-        <v>441.12</v>
+        <v>721.413</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F9">
-        <v>441.12</v>
+        <v>721.413</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M9">
-        <v>30000</v>
+        <v>34700</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P9" t="s">
         <v>25</v>
       </c>
-      <c r="P9" t="s">
-        <v>27</v>
-      </c>
       <c r="Q9">
-        <v>1072999</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1138,102 +1147,102 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D10">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F10">
-        <v>2846.537406</v>
+        <v>441.12</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M10">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N10">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q10">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D11">
         <v>4192.2496</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F11">
-        <v>1219.944706</v>
+        <v>2846.537406</v>
       </c>
       <c r="G11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M11">
         <v>36200</v>
       </c>
       <c r="N11">
-        <v>29.1</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O11" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q11">
         <v>19108320</v>
@@ -1241,52 +1250,52 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <v>4192.2496</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F12">
-        <v>125.767488</v>
+        <v>1219.944706</v>
       </c>
       <c r="G12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M12">
         <v>36200</v>
       </c>
       <c r="N12">
-        <v>3</v>
+        <v>29.1</v>
       </c>
       <c r="O12" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q12">
         <v>19108320</v>
@@ -1297,52 +1306,52 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D13">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F13">
-        <v>63.84</v>
+        <v>125.767488</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L13" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M13">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N13">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q13">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1350,90 +1359,90 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F14">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M14">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N14">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="Q14">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>320</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15">
         <v>160</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M15">
         <v>20000</v>
@@ -1442,10 +1451,10 @@
         <v>50</v>
       </c>
       <c r="O15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q15">
         <v>2254770</v>
@@ -1456,105 +1465,105 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F16">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="L16" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M16">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N16">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O16" t="s">
+        <v>87</v>
+      </c>
+      <c r="P16" t="s">
         <v>31</v>
       </c>
-      <c r="P16" t="s">
-        <v>29</v>
-      </c>
       <c r="Q16">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D17">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F17">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="P17" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="Q17">
-        <v>3000000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1562,52 +1571,52 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D18">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F18">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L18" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M18">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="P18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q18">
-        <v>4550000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1615,211 +1624,211 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D19">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F19">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="G19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M19">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P19" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="Q19">
-        <v>3900000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D20">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="E20" t="s">
         <v>69</v>
       </c>
       <c r="F20">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="G20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M20">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q20">
-        <v>1545000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D21">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="G21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L21" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M21">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q21">
-        <v>840000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D22">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F22">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K22" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M22">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="P22" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
       <c r="Q22">
-        <v>2600000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1827,52 +1836,52 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D23">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F23">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M23">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="P23" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="Q23">
-        <v>9375000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1880,105 +1889,105 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D24">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F24">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="G24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M24">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P24" t="s">
         <v>33</v>
       </c>
       <c r="Q24">
-        <v>787111</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D25">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F25">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K25" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M25">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q25">
-        <v>846540</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1986,52 +1995,52 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F26">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="G26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K26" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M26">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="P26" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="Q26">
-        <v>1119600</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2039,52 +2048,52 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D27">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F27">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="G27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K27" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L27" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M27">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="P27" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="Q27">
-        <v>2880000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2092,52 +2101,52 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D28">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="E28" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="F28">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="G28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L28" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M28">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="P28" t="s">
-        <v>91</v>
+        <v>36</v>
       </c>
       <c r="Q28">
-        <v>577500</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2145,52 +2154,52 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D29">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F29">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K29" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L29" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M29">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P29" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="Q29">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2198,51 +2207,104 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D30">
+        <v>520</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30">
+        <v>520</v>
+      </c>
+      <c r="G30" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" t="s">
+        <v>78</v>
+      </c>
+      <c r="I30" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" t="s">
+        <v>78</v>
+      </c>
+      <c r="K30" t="s">
+        <v>79</v>
+      </c>
+      <c r="L30" t="s">
+        <v>78</v>
+      </c>
+      <c r="M30">
+        <v>26000</v>
+      </c>
+      <c r="N30">
+        <v>100</v>
+      </c>
+      <c r="O30" t="s">
+        <v>92</v>
+      </c>
+      <c r="P30" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q30">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31">
         <v>442.659</v>
       </c>
-      <c r="E30" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30">
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31">
         <v>442.659</v>
       </c>
-      <c r="G30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H30" t="s">
-        <v>76</v>
-      </c>
-      <c r="I30" t="s">
-        <v>76</v>
-      </c>
-      <c r="J30" t="s">
-        <v>76</v>
-      </c>
-      <c r="K30" t="s">
-        <v>77</v>
-      </c>
-      <c r="L30" t="s">
-        <v>76</v>
-      </c>
-      <c r="M30">
+      <c r="G31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s">
+        <v>78</v>
+      </c>
+      <c r="I31" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L31" t="s">
+        <v>78</v>
+      </c>
+      <c r="M31">
         <v>10700</v>
       </c>
-      <c r="N30">
-        <v>100</v>
-      </c>
-      <c r="O30" t="s">
-        <v>90</v>
-      </c>
-      <c r="P30" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q30">
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>93</v>
+      </c>
+      <c r="P31" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q31">
         <v>3102750</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-06
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="101">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-12-05</t>
+  </si>
+  <si>
     <t>2023-12-04</t>
   </si>
   <si>
@@ -130,6 +133,12 @@
     <t>2023-10-18</t>
   </si>
   <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
     <t>삼성스팩9호</t>
   </si>
   <si>
@@ -215,6 +224,12 @@
   </si>
   <si>
     <t>코스피</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>유안타</t>
   </si>
   <si>
     <t>삼성</t>
@@ -659,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -723,37 +738,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -762,66 +777,66 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q2">
-        <v>7500000</v>
+        <v>2625000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D3">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F3">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M3">
-        <v>18000</v>
+        <v>9000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="P3" t="s">
         <v>20</v>
       </c>
       <c r="Q3">
-        <v>487500</v>
+        <v>1055000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -829,37 +844,37 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D4">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F4">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -868,13 +883,13 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="P4" t="s">
         <v>20</v>
       </c>
       <c r="Q4">
-        <v>6000000</v>
+        <v>7500000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -882,211 +897,211 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D5">
-        <v>393.96</v>
+        <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F5">
-        <v>393.96</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M5">
-        <v>28000</v>
+        <v>18000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q5">
-        <v>1055250</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D6">
-        <v>278.8</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F6">
-        <v>278.8</v>
+        <v>160</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M6">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="Q6">
-        <v>1221420</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D7">
-        <v>368.5</v>
+        <v>393.96</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F7">
-        <v>368.5</v>
+        <v>393.96</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M7">
-        <v>11000</v>
+        <v>28000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="P7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="Q7">
-        <v>2374500</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D8">
-        <v>297.5</v>
+        <v>278.8</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F8">
-        <v>297.5</v>
+        <v>278.8</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M8">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="Q8">
-        <v>3187500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1094,158 +1109,158 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D9">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F9">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M9">
-        <v>34700</v>
+        <v>11000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" t="s">
         <v>29</v>
       </c>
-      <c r="P9" t="s">
-        <v>25</v>
-      </c>
       <c r="Q9">
-        <v>1537150</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D10">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F10">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="G10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L10" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M10">
-        <v>30000</v>
+        <v>7000</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="Q10">
-        <v>1072999</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D11">
-        <v>4192.2496</v>
+        <v>721.413</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F11">
-        <v>2846.537406</v>
+        <v>721.413</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M11">
-        <v>36200</v>
+        <v>34700</v>
       </c>
       <c r="N11">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q11">
-        <v>19108320</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1253,102 +1268,102 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D12">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F12">
-        <v>1219.944706</v>
+        <v>441.12</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L12" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M12">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N12">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q12">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>4192.2496</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F13">
-        <v>125.767488</v>
+        <v>2846.537406</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="L13" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M13">
         <v>36200</v>
       </c>
       <c r="N13">
-        <v>3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O13" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="P13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q13">
         <v>19108320</v>
@@ -1359,105 +1374,105 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D14">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F14">
-        <v>63.84</v>
+        <v>1219.944706</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M14">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N14">
-        <v>100</v>
+        <v>29.1</v>
       </c>
       <c r="O14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="P14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q14">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D15">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="F15">
-        <v>160</v>
+        <v>125.767488</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M15">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N15">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="P15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="Q15">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1465,52 +1480,52 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D16">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="F16">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M16">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N16">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="P16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q16">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1518,52 +1533,52 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17">
+        <v>320</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>160</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" t="s">
+        <v>83</v>
+      </c>
+      <c r="M17">
+        <v>20000</v>
+      </c>
+      <c r="N17">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17">
-        <v>659.0825</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17">
-        <v>659.0825</v>
-      </c>
-      <c r="G17" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" t="s">
-        <v>78</v>
-      </c>
-      <c r="J17" t="s">
-        <v>78</v>
-      </c>
-      <c r="K17" t="s">
-        <v>79</v>
-      </c>
-      <c r="L17" t="s">
-        <v>78</v>
-      </c>
-      <c r="M17">
-        <v>25000</v>
-      </c>
-      <c r="N17">
-        <v>100</v>
-      </c>
       <c r="O17" t="s">
+        <v>92</v>
+      </c>
+      <c r="P17" t="s">
         <v>32</v>
       </c>
-      <c r="P17" t="s">
-        <v>30</v>
-      </c>
       <c r="Q17">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1571,52 +1586,52 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D18">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F18">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="L18" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N18">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O18" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="P18" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="Q18">
-        <v>3000000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1624,370 +1639,370 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D19">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L19" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M19">
-        <v>1800</v>
+        <v>25000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="P19" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="Q19">
-        <v>4550000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D20">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F20">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M20">
-        <v>4800</v>
+        <v>2000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P20" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="Q20">
-        <v>3900000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D21">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F21">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M21">
-        <v>22500</v>
+        <v>1800</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P21" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="Q21">
-        <v>1545000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D22">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F22">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L22" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M22">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="P22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q22">
-        <v>840000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D23">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F23">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K23" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L23" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M23">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="P23" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
       <c r="Q23">
-        <v>2600000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D24">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F24">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M24">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="P24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q24">
-        <v>9375000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D25">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="E25" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="F25">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="G25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K25" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M25">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="P25" t="s">
-        <v>34</v>
+        <v>92</v>
       </c>
       <c r="Q25">
-        <v>787111</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1995,52 +2010,52 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D26">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F26">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="G26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L26" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M26">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="P26" t="s">
         <v>34</v>
       </c>
       <c r="Q26">
-        <v>846540</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2048,37 +2063,37 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D27">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="E27" t="s">
         <v>74</v>
       </c>
       <c r="F27">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="G27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K27" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L27" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M27">
         <v>17000</v>
@@ -2087,224 +2102,330 @@
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="P27" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="Q27">
-        <v>1119600</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D28">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F28">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K28" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L28" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M28">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="P28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q28">
-        <v>2880000</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D29">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F29">
-        <v>53.9</v>
+        <v>306</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K29" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M29">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="P29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="Q29">
-        <v>577500</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D30">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="F30">
-        <v>520</v>
+        <v>260</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="H30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="I30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="K30" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="L30" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M30">
-        <v>26000</v>
+        <v>6500</v>
       </c>
       <c r="N30">
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P30" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="Q30">
-        <v>1300000</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31">
+        <v>53.9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31">
+        <v>53.9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H31" t="s">
+        <v>83</v>
+      </c>
+      <c r="I31" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" t="s">
+        <v>83</v>
+      </c>
+      <c r="M31">
+        <v>7000</v>
+      </c>
+      <c r="N31">
+        <v>100</v>
+      </c>
+      <c r="O31" t="s">
+        <v>97</v>
+      </c>
+      <c r="P31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q31">
+        <v>577500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31">
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32">
+        <v>520</v>
+      </c>
+      <c r="E32" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32">
+        <v>520</v>
+      </c>
+      <c r="G32" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" t="s">
+        <v>83</v>
+      </c>
+      <c r="I32" t="s">
+        <v>83</v>
+      </c>
+      <c r="J32" t="s">
+        <v>83</v>
+      </c>
+      <c r="K32" t="s">
+        <v>84</v>
+      </c>
+      <c r="L32" t="s">
+        <v>83</v>
+      </c>
+      <c r="M32">
+        <v>26000</v>
+      </c>
+      <c r="N32">
+        <v>100</v>
+      </c>
+      <c r="O32" t="s">
+        <v>97</v>
+      </c>
+      <c r="P32" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q32">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33">
         <v>442.659</v>
       </c>
-      <c r="E31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31">
+      <c r="E33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33">
         <v>442.659</v>
       </c>
-      <c r="G31" t="s">
-        <v>78</v>
-      </c>
-      <c r="H31" t="s">
-        <v>78</v>
-      </c>
-      <c r="I31" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" t="s">
-        <v>78</v>
-      </c>
-      <c r="K31" t="s">
-        <v>79</v>
-      </c>
-      <c r="L31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M31">
+      <c r="G33" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" t="s">
+        <v>83</v>
+      </c>
+      <c r="M33">
         <v>10700</v>
       </c>
-      <c r="N31">
-        <v>100</v>
-      </c>
-      <c r="O31" t="s">
-        <v>93</v>
-      </c>
-      <c r="P31" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q31">
+      <c r="N33">
+        <v>100</v>
+      </c>
+      <c r="O33" t="s">
+        <v>98</v>
+      </c>
+      <c r="P33" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q33">
         <v>3102750</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-07
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="106">
   <si>
     <t>상장일</t>
   </si>
@@ -70,6 +70,9 @@
     <t>2023-12-05</t>
   </si>
   <si>
+    <t>2023-12-06</t>
+  </si>
+  <si>
     <t>2023-12-04</t>
   </si>
   <si>
@@ -136,6 +139,9 @@
     <t>교보15호스팩</t>
   </si>
   <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
     <t>와이바이오로직스</t>
   </si>
   <si>
@@ -229,6 +235,9 @@
     <t>교보</t>
   </si>
   <si>
+    <t>신영</t>
+  </si>
+  <si>
     <t>유안타</t>
   </si>
   <si>
@@ -283,6 +292,9 @@
     <t>2023-11-23</t>
   </si>
   <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
     <t>2023-11-16</t>
   </si>
   <si>
@@ -311,6 +323,9 @@
   </si>
   <si>
     <t>2023-10-05</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
   </si>
   <si>
     <t>2023-10-13</t>
@@ -674,7 +689,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -738,37 +753,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F2">
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -777,10 +792,10 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q2">
         <v>2625000</v>
@@ -788,108 +803,108 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D3">
-        <v>135</v>
+        <v>172.5</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F3">
-        <v>135</v>
+        <v>172.5</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M3">
-        <v>9000</v>
+        <v>23000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="Q3">
-        <v>1055000</v>
+        <v>475800</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F4">
-        <v>200</v>
+        <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4">
-        <v>7500000</v>
+        <v>1055000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -897,105 +912,105 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D5">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F5">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M5">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="P5" t="s">
         <v>21</v>
       </c>
       <c r="Q5">
-        <v>487500</v>
+        <v>7500000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D6">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F6">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q6">
-        <v>6000000</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1003,52 +1018,52 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D7">
-        <v>393.96</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F7">
-        <v>393.96</v>
+        <v>160</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M7">
-        <v>28000</v>
+        <v>2000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7">
-        <v>1055250</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1056,52 +1071,52 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D8">
-        <v>278.8</v>
+        <v>393.96</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F8">
-        <v>278.8</v>
+        <v>393.96</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K8" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L8" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M8">
-        <v>17000</v>
+        <v>28000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="P8" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="Q8">
-        <v>1221420</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1109,93 +1124,93 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D9">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9">
-        <v>368.5</v>
+        <v>278.8</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K9" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L9" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M9">
-        <v>11000</v>
+        <v>17000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P9" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="Q9">
-        <v>2374500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D10">
-        <v>297.5</v>
+        <v>368.5</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F10">
-        <v>297.5</v>
+        <v>368.5</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L10" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M10">
-        <v>7000</v>
+        <v>11000</v>
       </c>
       <c r="N10">
         <v>100</v>
@@ -1204,63 +1219,63 @@
         <v>28</v>
       </c>
       <c r="P10" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
       <c r="Q10">
-        <v>3187500</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D11">
-        <v>721.413</v>
+        <v>297.5</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F11">
-        <v>721.413</v>
+        <v>297.5</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K11" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M11">
-        <v>34700</v>
+        <v>7000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="Q11">
-        <v>1537150</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1268,52 +1283,52 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12">
-        <v>441.12</v>
+        <v>721.413</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F12">
-        <v>441.12</v>
+        <v>721.413</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K12" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M12">
-        <v>30000</v>
+        <v>34700</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" t="s">
         <v>27</v>
       </c>
-      <c r="P12" t="s">
-        <v>29</v>
-      </c>
       <c r="Q12">
-        <v>1072999</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1321,102 +1336,102 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D13">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F13">
-        <v>2846.537406</v>
+        <v>441.12</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K13" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M13">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N13">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="P13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q13">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D14">
         <v>4192.2496</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F14">
-        <v>1219.944706</v>
+        <v>2846.537406</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M14">
         <v>36200</v>
       </c>
       <c r="N14">
-        <v>29.1</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="P14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q14">
         <v>19108320</v>
@@ -1424,52 +1439,52 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D15">
         <v>4192.2496</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F15">
-        <v>125.767488</v>
+        <v>1219.944706</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M15">
         <v>36200</v>
       </c>
       <c r="N15">
-        <v>3</v>
+        <v>29.1</v>
       </c>
       <c r="O15" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="P15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q15">
         <v>19108320</v>
@@ -1480,52 +1495,52 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D16">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F16">
-        <v>63.84</v>
+        <v>125.767488</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K16" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M16">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N16">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O16" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="P16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q16">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1533,90 +1548,90 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D17">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F17">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K17" t="s">
         <v>87</v>
       </c>
       <c r="L17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M17">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N17">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="P17" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q17">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18">
         <v>320</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K18" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L18" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M18">
         <v>20000</v>
@@ -1625,10 +1640,10 @@
         <v>50</v>
       </c>
       <c r="O18" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q18">
         <v>2254770</v>
@@ -1639,105 +1654,105 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D19">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F19">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K19" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="L19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M19">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N19">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O19" t="s">
+        <v>96</v>
+      </c>
+      <c r="P19" t="s">
         <v>33</v>
       </c>
-      <c r="P19" t="s">
-        <v>31</v>
-      </c>
       <c r="Q19">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>659.0825</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>25000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="P20" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="Q20">
-        <v>3000000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1745,52 +1760,52 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D21">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F21">
-        <v>126</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M21">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="P21" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="Q21">
-        <v>4550000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1798,211 +1813,211 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D22">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F22">
-        <v>249.6</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L22" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M22">
-        <v>4800</v>
+        <v>1800</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="P22" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="Q22">
-        <v>3900000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D23">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="E23" t="s">
         <v>77</v>
       </c>
       <c r="F23">
-        <v>463.5</v>
+        <v>249.6</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M23">
-        <v>22500</v>
+        <v>4800</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q23">
-        <v>1545000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D24">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="E24" t="s">
         <v>80</v>
       </c>
       <c r="F24">
-        <v>156</v>
+        <v>463.5</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L24" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M24">
-        <v>13000</v>
+        <v>22500</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="P24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q24">
-        <v>840000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D25">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F25">
-        <v>270</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L25" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M25">
-        <v>7500</v>
+        <v>13000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="P25" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="Q25">
-        <v>2600000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2010,52 +2025,52 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D26">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F26">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L26" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M26">
-        <v>2000</v>
+        <v>7500</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="P26" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="Q26">
-        <v>9375000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2063,105 +2078,105 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D27">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="F27">
-        <v>178.41194</v>
+        <v>250</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M27">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="P27" t="s">
         <v>35</v>
       </c>
       <c r="Q27">
-        <v>787111</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D28">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F28">
-        <v>49.66368</v>
+        <v>178.41194</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K28" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M28">
-        <v>4400</v>
+        <v>17000</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="P28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q28">
-        <v>846540</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2169,52 +2184,52 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D29">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F29">
-        <v>306</v>
+        <v>49.66368</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K29" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L29" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M29">
-        <v>17000</v>
+        <v>4400</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="P29" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="Q29">
-        <v>1119600</v>
+        <v>846540</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2222,52 +2237,52 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D30">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="E30" t="s">
         <v>82</v>
       </c>
       <c r="F30">
-        <v>260</v>
+        <v>306</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K30" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M30">
-        <v>6500</v>
+        <v>17000</v>
       </c>
       <c r="N30">
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="P30" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="Q30">
-        <v>2880000</v>
+        <v>1119600</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2275,52 +2290,52 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D31">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="F31">
-        <v>53.9</v>
+        <v>260</v>
       </c>
       <c r="G31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K31" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L31" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M31">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="P31" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="Q31">
-        <v>577500</v>
+        <v>2880000</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2328,52 +2343,52 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D32">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="E32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F32">
-        <v>520</v>
+        <v>53.9</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="J32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K32" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L32" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="M32">
-        <v>26000</v>
+        <v>7000</v>
       </c>
       <c r="N32">
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="P32" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="Q32">
-        <v>1300000</v>
+        <v>577500</v>
       </c>
     </row>
     <row r="33" spans="1:17">
@@ -2381,51 +2396,104 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D33">
+        <v>520</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33">
+        <v>520</v>
+      </c>
+      <c r="G33" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" t="s">
+        <v>86</v>
+      </c>
+      <c r="J33" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" t="s">
+        <v>87</v>
+      </c>
+      <c r="L33" t="s">
+        <v>86</v>
+      </c>
+      <c r="M33">
+        <v>26000</v>
+      </c>
+      <c r="N33">
+        <v>100</v>
+      </c>
+      <c r="O33" t="s">
+        <v>101</v>
+      </c>
+      <c r="P33" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q33">
+        <v>1300000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34">
         <v>442.659</v>
       </c>
-      <c r="E33" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33">
+      <c r="E34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34">
         <v>442.659</v>
       </c>
-      <c r="G33" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" t="s">
-        <v>83</v>
-      </c>
-      <c r="J33" t="s">
-        <v>83</v>
-      </c>
-      <c r="K33" t="s">
-        <v>84</v>
-      </c>
-      <c r="L33" t="s">
-        <v>83</v>
-      </c>
-      <c r="M33">
+      <c r="G34" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" t="s">
+        <v>86</v>
+      </c>
+      <c r="J34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K34" t="s">
+        <v>87</v>
+      </c>
+      <c r="L34" t="s">
+        <v>86</v>
+      </c>
+      <c r="M34">
         <v>10700</v>
       </c>
-      <c r="N33">
-        <v>100</v>
-      </c>
-      <c r="O33" t="s">
-        <v>98</v>
-      </c>
-      <c r="P33" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q33">
+      <c r="N34">
+        <v>100</v>
+      </c>
+      <c r="O34" t="s">
+        <v>102</v>
+      </c>
+      <c r="P34" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q34">
         <v>3102750</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-11
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="103">
   <si>
     <t>상장일</t>
   </si>
@@ -133,205 +133,196 @@
     <t>2023-10-19</t>
   </si>
   <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>에스엘에스바이오</t>
+  </si>
+  <si>
+    <t>신성에스티</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
     <t>2023-10-18</t>
   </si>
   <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>퓨릿</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
     <t>2023-10-16</t>
   </si>
   <si>
     <t>2023-10-10</t>
   </si>
   <si>
-    <t>2023-10-05</t>
-  </si>
-  <si>
     <t>2023-11-30</t>
   </si>
   <si>
     <t>2023-10-13</t>
-  </si>
-  <si>
-    <t>2023-10-11</t>
   </si>
 </sst>
 </file>
@@ -689,7 +680,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -753,37 +744,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D2">
         <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2">
         <v>70</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -792,7 +783,7 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P2" t="s">
         <v>21</v>
@@ -806,37 +797,37 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3">
         <v>172.5</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>172.5</v>
       </c>
       <c r="G3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M3">
         <v>23000</v>
@@ -845,10 +836,10 @@
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Q3">
         <v>475800</v>
@@ -859,37 +850,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F4">
         <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M4">
         <v>9000</v>
@@ -898,7 +889,7 @@
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P4" t="s">
         <v>21</v>
@@ -912,37 +903,37 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5">
         <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F5">
         <v>200</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -951,7 +942,7 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P5" t="s">
         <v>21</v>
@@ -965,37 +956,37 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6">
         <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F6">
         <v>117</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M6">
         <v>18000</v>
@@ -1018,37 +1009,37 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7">
         <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7">
         <v>160</v>
       </c>
       <c r="G7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1071,37 +1062,37 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D8">
         <v>393.96</v>
       </c>
       <c r="E8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8">
         <v>393.96</v>
       </c>
       <c r="G8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M8">
         <v>28000</v>
@@ -1110,7 +1101,7 @@
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P8" t="s">
         <v>24</v>
@@ -1124,37 +1115,37 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9">
         <v>278.8</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F9">
         <v>278.8</v>
       </c>
       <c r="G9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M9">
         <v>17000</v>
@@ -1166,7 +1157,7 @@
         <v>29</v>
       </c>
       <c r="P9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q9">
         <v>1221420</v>
@@ -1177,37 +1168,37 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10">
         <v>368.5</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10">
         <v>368.5</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M10">
         <v>11000</v>
@@ -1230,37 +1221,37 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>297.5</v>
       </c>
       <c r="E11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F11">
         <v>297.5</v>
       </c>
       <c r="G11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M11">
         <v>7000</v>
@@ -1272,7 +1263,7 @@
         <v>29</v>
       </c>
       <c r="P11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q11">
         <v>3187500</v>
@@ -1283,37 +1274,37 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D12">
         <v>721.413</v>
       </c>
       <c r="E12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F12">
         <v>721.413</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M12">
         <v>34700</v>
@@ -1336,37 +1327,37 @@
         <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D13">
         <v>441.12</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13">
         <v>441.12</v>
       </c>
       <c r="G13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M13">
         <v>30000</v>
@@ -1389,37 +1380,37 @@
         <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14">
         <v>4192.2496</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14">
         <v>2846.537406</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M14">
         <v>36200</v>
@@ -1428,7 +1419,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P14" t="s">
         <v>29</v>
@@ -1442,37 +1433,37 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15">
         <v>4192.2496</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F15">
         <v>1219.944706</v>
       </c>
       <c r="G15" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" t="s">
+        <v>84</v>
+      </c>
+      <c r="J15" t="s">
+        <v>84</v>
+      </c>
+      <c r="K15" t="s">
         <v>86</v>
       </c>
-      <c r="H15" t="s">
-        <v>86</v>
-      </c>
-      <c r="I15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" t="s">
-        <v>86</v>
-      </c>
-      <c r="K15" t="s">
-        <v>88</v>
-      </c>
       <c r="L15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M15">
         <v>36200</v>
@@ -1481,7 +1472,7 @@
         <v>29.1</v>
       </c>
       <c r="O15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P15" t="s">
         <v>29</v>
@@ -1495,37 +1486,37 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16">
         <v>4192.2496</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F16">
         <v>125.767488</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M16">
         <v>36200</v>
@@ -1534,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="O16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P16" t="s">
         <v>29</v>
@@ -1548,37 +1539,37 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D17">
         <v>63.84</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F17">
         <v>63.84</v>
       </c>
       <c r="G17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M17">
         <v>4000</v>
@@ -1587,7 +1578,7 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P17" t="s">
         <v>28</v>
@@ -1601,37 +1592,37 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18">
         <v>320</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M18">
         <v>20000</v>
@@ -1640,7 +1631,7 @@
         <v>50</v>
       </c>
       <c r="O18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P18" t="s">
         <v>33</v>
@@ -1654,37 +1645,37 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19">
         <v>320</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F19">
         <v>160</v>
       </c>
       <c r="G19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M19">
         <v>20000</v>
@@ -1693,7 +1684,7 @@
         <v>50</v>
       </c>
       <c r="O19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P19" t="s">
         <v>33</v>
@@ -1707,37 +1698,37 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D20">
         <v>659.0825</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F20">
         <v>659.0825</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M20">
         <v>25000</v>
@@ -1760,37 +1751,37 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D21">
         <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F21">
         <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1799,10 +1790,10 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q21">
         <v>3000000</v>
@@ -1813,37 +1804,37 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D22">
         <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F22">
         <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M22">
         <v>1800</v>
@@ -1852,10 +1843,10 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="P22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q22">
         <v>4550000</v>
@@ -1866,37 +1857,37 @@
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D23">
         <v>249.6</v>
       </c>
       <c r="E23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F23">
         <v>249.6</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M23">
         <v>4800</v>
@@ -1905,7 +1896,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P23" t="s">
         <v>33</v>
@@ -1919,37 +1910,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24">
         <v>463.5</v>
       </c>
       <c r="E24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F24">
         <v>463.5</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M24">
         <v>22500</v>
@@ -1958,7 +1949,7 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P24" t="s">
         <v>33</v>
@@ -1972,37 +1963,37 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D25">
         <v>156</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F25">
         <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M25">
         <v>13000</v>
@@ -2011,7 +2002,7 @@
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P25" t="s">
         <v>33</v>
@@ -2025,37 +2016,37 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26">
         <v>270</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F26">
         <v>270</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M26">
         <v>7500</v>
@@ -2067,7 +2058,7 @@
         <v>36</v>
       </c>
       <c r="P26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="Q26">
         <v>2600000</v>
@@ -2078,37 +2069,37 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27">
         <v>250</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F27">
         <v>250</v>
       </c>
       <c r="G27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M27">
         <v>2000</v>
@@ -2117,7 +2108,7 @@
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="P27" t="s">
         <v>35</v>
@@ -2131,37 +2122,37 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28">
         <v>178.41194</v>
       </c>
       <c r="E28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F28">
         <v>178.41194</v>
       </c>
       <c r="G28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M28">
         <v>17000</v>
@@ -2170,7 +2161,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P28" t="s">
         <v>36</v>
@@ -2184,37 +2175,37 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29">
         <v>49.66368</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F29">
         <v>49.66368</v>
       </c>
       <c r="G29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K29" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M29">
         <v>4400</v>
@@ -2223,7 +2214,7 @@
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P29" t="s">
         <v>36</v>
@@ -2237,37 +2228,37 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D30">
         <v>306</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F30">
         <v>306</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M30">
         <v>17000</v>
@@ -2276,10 +2267,10 @@
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="P30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q30">
         <v>1119600</v>
@@ -2290,37 +2281,37 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D31">
         <v>260</v>
       </c>
       <c r="E31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F31">
         <v>260</v>
       </c>
       <c r="G31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M31">
         <v>6500</v>
@@ -2329,7 +2320,7 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P31" t="s">
         <v>38</v>
@@ -2343,37 +2334,37 @@
         <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D32">
         <v>53.9</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F32">
         <v>53.9</v>
       </c>
       <c r="G32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M32">
         <v>7000</v>
@@ -2382,10 +2373,10 @@
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q32">
         <v>577500</v>
@@ -2396,37 +2387,37 @@
         <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D33">
         <v>520</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F33">
         <v>520</v>
       </c>
       <c r="G33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M33">
         <v>26000</v>
@@ -2435,66 +2426,13 @@
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="Q33">
         <v>1300000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" t="s">
-        <v>70</v>
-      </c>
-      <c r="D34">
-        <v>442.659</v>
-      </c>
-      <c r="E34" t="s">
-        <v>78</v>
-      </c>
-      <c r="F34">
-        <v>442.659</v>
-      </c>
-      <c r="G34" t="s">
-        <v>86</v>
-      </c>
-      <c r="H34" t="s">
-        <v>86</v>
-      </c>
-      <c r="I34" t="s">
-        <v>86</v>
-      </c>
-      <c r="J34" t="s">
-        <v>86</v>
-      </c>
-      <c r="K34" t="s">
-        <v>87</v>
-      </c>
-      <c r="L34" t="s">
-        <v>86</v>
-      </c>
-      <c r="M34">
-        <v>10700</v>
-      </c>
-      <c r="N34">
-        <v>100</v>
-      </c>
-      <c r="O34" t="s">
-        <v>102</v>
-      </c>
-      <c r="P34" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q34">
-        <v>3102750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-13
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="101">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-12-12</t>
+  </si>
+  <si>
     <t>2023-12-05</t>
   </si>
   <si>
@@ -127,202 +130,193 @@
     <t>2023-10-26</t>
   </si>
   <si>
-    <t>2023-10-20</t>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>워트</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-10-18</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
   </si>
   <si>
     <t>2023-10-19</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>에스엘에스바이오</t>
-  </si>
-  <si>
-    <t>신성에스티</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-18</t>
-  </si>
-  <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
-    <t>2023-10-10</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
-  </si>
-  <si>
-    <t>2023-10-13</t>
   </si>
 </sst>
 </file>
@@ -680,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -744,105 +738,105 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2">
+        <v>877.5</v>
+      </c>
+      <c r="E2" t="s">
         <v>68</v>
       </c>
-      <c r="D2">
-        <v>70</v>
-      </c>
-      <c r="E2" t="s">
-        <v>70</v>
-      </c>
       <c r="F2">
-        <v>70</v>
+        <v>361.96872</v>
       </c>
       <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" t="s">
         <v>84</v>
       </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K2" t="s">
-        <v>85</v>
-      </c>
       <c r="L2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="N2">
-        <v>100</v>
+        <v>41.25</v>
       </c>
       <c r="O2" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q2">
-        <v>2625000</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3">
-        <v>172.5</v>
+        <v>877.5</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F3">
-        <v>172.5</v>
+        <v>361.96872</v>
       </c>
       <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" t="s">
         <v>84</v>
       </c>
-      <c r="H3" t="s">
-        <v>84</v>
-      </c>
-      <c r="I3" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" t="s">
-        <v>85</v>
-      </c>
       <c r="L3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M3">
-        <v>23000</v>
+        <v>6000</v>
       </c>
       <c r="N3">
-        <v>100</v>
+        <v>41.25</v>
       </c>
       <c r="O3" t="s">
-        <v>90</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="Q3">
-        <v>475800</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -850,196 +844,196 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4">
-        <v>135</v>
+        <v>877.5</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4">
-        <v>135</v>
+        <v>65.81256</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K4" t="s">
         <v>85</v>
       </c>
       <c r="L4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M4">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="N4">
-        <v>100</v>
+        <v>7.5</v>
       </c>
       <c r="O4" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q4">
-        <v>1055000</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5">
-        <v>200</v>
+        <v>877.5</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5">
-        <v>200</v>
+        <v>43.875</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" t="s">
         <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M5">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="N5">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="P5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q5">
-        <v>7500000</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6">
-        <v>117</v>
+        <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6">
-        <v>117</v>
+        <v>43.875</v>
       </c>
       <c r="G6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" t="s">
         <v>85</v>
       </c>
       <c r="L6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M6">
-        <v>18000</v>
+        <v>6000</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q6">
-        <v>487500</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7">
-        <v>160</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7">
-        <v>160</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M7">
         <v>2000</v>
@@ -1048,1391 +1042,1550 @@
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="P7" t="s">
         <v>22</v>
       </c>
       <c r="Q7">
-        <v>6000000</v>
+        <v>2625000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8">
-        <v>393.96</v>
+        <v>172.5</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8">
-        <v>393.96</v>
+        <v>172.5</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M8">
-        <v>28000</v>
+        <v>23000</v>
       </c>
       <c r="N8">
         <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="Q8">
-        <v>1055250</v>
+        <v>475800</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9">
-        <v>278.8</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
         <v>75</v>
       </c>
       <c r="F9">
-        <v>278.8</v>
+        <v>135</v>
       </c>
       <c r="G9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K9" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M9">
-        <v>17000</v>
+        <v>9000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="P9" t="s">
-        <v>91</v>
+        <v>22</v>
       </c>
       <c r="Q9">
-        <v>1221420</v>
+        <v>1055000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10">
-        <v>368.5</v>
+        <v>200</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F10">
-        <v>368.5</v>
+        <v>200</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M10">
-        <v>11000</v>
+        <v>2000</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="P10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="Q10">
-        <v>2374500</v>
+        <v>7500000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11">
-        <v>297.5</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F11">
-        <v>297.5</v>
+        <v>117</v>
       </c>
       <c r="G11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M11">
-        <v>7000</v>
+        <v>18000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="Q11">
-        <v>3187500</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12">
-        <v>721.413</v>
+        <v>160</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F12">
-        <v>721.413</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M12">
-        <v>34700</v>
+        <v>2000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="Q12">
-        <v>1537150</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D13">
-        <v>441.12</v>
+        <v>393.96</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F13">
-        <v>441.12</v>
+        <v>393.96</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M13">
-        <v>30000</v>
+        <v>28000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="P13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Q13">
-        <v>1072999</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14">
-        <v>4192.2496</v>
+        <v>278.8</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F14">
-        <v>2846.537406</v>
+        <v>278.8</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M14">
-        <v>36200</v>
+        <v>17000</v>
       </c>
       <c r="N14">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="P14" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="Q14">
-        <v>19108320</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D15">
-        <v>4192.2496</v>
+        <v>368.5</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F15">
-        <v>1219.944706</v>
+        <v>368.5</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
         <v>86</v>
       </c>
       <c r="L15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M15">
-        <v>36200</v>
+        <v>11000</v>
       </c>
       <c r="N15">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="P15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q15">
-        <v>19108320</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D16">
-        <v>4192.2496</v>
+        <v>297.5</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F16">
-        <v>125.767488</v>
+        <v>297.5</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M16">
-        <v>36200</v>
+        <v>7000</v>
       </c>
       <c r="N16">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="P16" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="Q16">
-        <v>19108320</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17">
-        <v>63.84</v>
+        <v>721.413</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F17">
-        <v>63.84</v>
+        <v>721.413</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M17">
-        <v>4000</v>
+        <v>34700</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="P17" t="s">
         <v>28</v>
       </c>
       <c r="Q17">
-        <v>1197000</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18">
-        <v>320</v>
+        <v>441.12</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F18">
-        <v>160</v>
+        <v>441.12</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M18">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="N18">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="P18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q18">
-        <v>2254770</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D19">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F19">
-        <v>160</v>
+        <v>2846.537406</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M19">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N19">
-        <v>50</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="P19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="Q19">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20">
-        <v>659.0825</v>
+        <v>4192.2496</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20">
-        <v>659.0825</v>
+        <v>1219.944706</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M20">
-        <v>25000</v>
+        <v>36200</v>
       </c>
       <c r="N20">
-        <v>100</v>
+        <v>29.1</v>
       </c>
       <c r="O20" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="P20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q20">
-        <v>1827247</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21">
-        <v>80</v>
+        <v>4192.2496</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F21">
-        <v>80</v>
+        <v>125.767488</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
         <v>85</v>
       </c>
       <c r="L21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M21">
-        <v>2000</v>
+        <v>36200</v>
       </c>
       <c r="N21">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O21" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="P21" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="Q21">
-        <v>3000000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22">
-        <v>126</v>
+        <v>63.84</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F22">
-        <v>126</v>
+        <v>63.84</v>
       </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M22">
-        <v>1800</v>
+        <v>4000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="P22" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="Q22">
-        <v>4550000</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23">
-        <v>249.6</v>
+        <v>320</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F23">
-        <v>249.6</v>
+        <v>160</v>
       </c>
       <c r="G23" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" t="s">
         <v>84</v>
       </c>
-      <c r="H23" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" t="s">
-        <v>84</v>
-      </c>
-      <c r="J23" t="s">
-        <v>84</v>
-      </c>
-      <c r="K23" t="s">
-        <v>85</v>
-      </c>
       <c r="L23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M23">
-        <v>4800</v>
+        <v>20000</v>
       </c>
       <c r="N23">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q23">
-        <v>3900000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24">
-        <v>463.5</v>
+        <v>320</v>
       </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F24">
-        <v>463.5</v>
+        <v>160</v>
       </c>
       <c r="G24" t="s">
+        <v>83</v>
+      </c>
+      <c r="H24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" t="s">
+        <v>83</v>
+      </c>
+      <c r="J24" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" t="s">
         <v>84</v>
       </c>
-      <c r="H24" t="s">
-        <v>84</v>
-      </c>
-      <c r="I24" t="s">
-        <v>84</v>
-      </c>
-      <c r="J24" t="s">
-        <v>84</v>
-      </c>
-      <c r="K24" t="s">
-        <v>85</v>
-      </c>
       <c r="L24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M24">
-        <v>22500</v>
+        <v>20000</v>
       </c>
       <c r="N24">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q24">
-        <v>1545000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25">
-        <v>156</v>
+        <v>659.0825</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F25">
-        <v>156</v>
+        <v>659.0825</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M25">
-        <v>13000</v>
+        <v>25000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="P25" t="s">
         <v>33</v>
       </c>
       <c r="Q25">
-        <v>840000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26">
-        <v>270</v>
+        <v>80</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F26">
-        <v>270</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M26">
-        <v>7500</v>
+        <v>2000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="P26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q26">
-        <v>2600000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27">
-        <v>250</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F27">
-        <v>250</v>
+        <v>126</v>
       </c>
       <c r="G27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M27">
-        <v>2000</v>
+        <v>1800</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P27" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="Q27">
-        <v>9375000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28">
-        <v>178.41194</v>
+        <v>249.6</v>
       </c>
       <c r="E28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F28">
-        <v>178.41194</v>
+        <v>249.6</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M28">
-        <v>17000</v>
+        <v>4800</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q28">
-        <v>787111</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29">
-        <v>49.66368</v>
+        <v>463.5</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F29">
-        <v>49.66368</v>
+        <v>463.5</v>
       </c>
       <c r="G29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M29">
-        <v>4400</v>
+        <v>22500</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q29">
-        <v>846540</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30">
-        <v>306</v>
+        <v>156</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F30">
-        <v>306</v>
+        <v>156</v>
       </c>
       <c r="G30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M30">
-        <v>17000</v>
+        <v>13000</v>
       </c>
       <c r="N30">
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="P30" t="s">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="Q30">
-        <v>1119600</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="F31">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="G31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M31">
-        <v>6500</v>
+        <v>7500</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="P31" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="Q31">
-        <v>2880000</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D32">
-        <v>53.9</v>
+        <v>250</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F32">
-        <v>53.9</v>
+        <v>250</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K32" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M32">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="N32">
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P32" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="Q32">
-        <v>577500</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D33">
-        <v>520</v>
+        <v>178.41194</v>
       </c>
       <c r="E33" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F33">
-        <v>520</v>
+        <v>178.41194</v>
       </c>
       <c r="G33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M33">
-        <v>26000</v>
+        <v>17000</v>
       </c>
       <c r="N33">
         <v>100</v>
       </c>
       <c r="O33" t="s">
+        <v>96</v>
+      </c>
+      <c r="P33" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q33">
+        <v>787111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34">
+        <v>49.66368</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34">
+        <v>49.66368</v>
+      </c>
+      <c r="G34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H34" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" t="s">
+        <v>83</v>
+      </c>
+      <c r="K34" t="s">
+        <v>86</v>
+      </c>
+      <c r="L34" t="s">
+        <v>83</v>
+      </c>
+      <c r="M34">
+        <v>4400</v>
+      </c>
+      <c r="N34">
         <v>100</v>
       </c>
-      <c r="P33" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q33">
-        <v>1300000</v>
+      <c r="O34" t="s">
+        <v>96</v>
+      </c>
+      <c r="P34" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q34">
+        <v>846540</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D35">
+        <v>306</v>
+      </c>
+      <c r="E35" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35">
+        <v>306</v>
+      </c>
+      <c r="G35" t="s">
+        <v>83</v>
+      </c>
+      <c r="H35" t="s">
+        <v>83</v>
+      </c>
+      <c r="I35" t="s">
+        <v>83</v>
+      </c>
+      <c r="J35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" t="s">
+        <v>86</v>
+      </c>
+      <c r="L35" t="s">
+        <v>83</v>
+      </c>
+      <c r="M35">
+        <v>17000</v>
+      </c>
+      <c r="N35">
+        <v>100</v>
+      </c>
+      <c r="O35" t="s">
+        <v>97</v>
+      </c>
+      <c r="P35" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q35">
+        <v>1119600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36">
+        <v>260</v>
+      </c>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36">
+        <v>260</v>
+      </c>
+      <c r="G36" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" t="s">
+        <v>83</v>
+      </c>
+      <c r="J36" t="s">
+        <v>83</v>
+      </c>
+      <c r="K36" t="s">
+        <v>86</v>
+      </c>
+      <c r="L36" t="s">
+        <v>83</v>
+      </c>
+      <c r="M36">
+        <v>6500</v>
+      </c>
+      <c r="N36">
+        <v>100</v>
+      </c>
+      <c r="O36" t="s">
+        <v>98</v>
+      </c>
+      <c r="P36" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q36">
+        <v>2880000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-14
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="104">
   <si>
     <t>상장일</t>
   </si>
@@ -70,6 +70,9 @@
     <t>2023-12-12</t>
   </si>
   <si>
+    <t>2023-12-13</t>
+  </si>
+  <si>
     <t>2023-12-05</t>
   </si>
   <si>
@@ -133,6 +136,9 @@
     <t>LS머트리얼즈</t>
   </si>
   <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
     <t>교보15호스팩</t>
   </si>
   <si>
@@ -235,6 +241,9 @@
     <t>NH</t>
   </si>
   <si>
+    <t>하나</t>
+  </si>
+  <si>
     <t>교보</t>
   </si>
   <si>
@@ -247,9 +256,6 @@
     <t>삼성</t>
   </si>
   <si>
-    <t>하나</t>
-  </si>
-  <si>
     <t>미래</t>
   </si>
   <si>
@@ -311,6 +317,9 @@
   </si>
   <si>
     <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
   </si>
   <si>
     <t>2023-11-30</t>
@@ -674,7 +683,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -738,37 +747,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D2">
         <v>877.5</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F2">
         <v>361.96872</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M2">
         <v>6000</v>
@@ -777,10 +786,10 @@
         <v>41.25</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q2">
         <v>52832240</v>
@@ -791,37 +800,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3">
         <v>877.5</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F3">
         <v>361.96872</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M3">
         <v>6000</v>
@@ -830,10 +839,10 @@
         <v>41.25</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q3">
         <v>52832240</v>
@@ -844,37 +853,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D4">
         <v>877.5</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F4">
         <v>65.81256</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M4">
         <v>6000</v>
@@ -883,10 +892,10 @@
         <v>7.5</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q4">
         <v>52832240</v>
@@ -897,37 +906,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D5">
         <v>877.5</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F5">
         <v>43.875</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M5">
         <v>6000</v>
@@ -936,10 +945,10 @@
         <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q5">
         <v>52832240</v>
@@ -950,37 +959,37 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F6">
         <v>43.875</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -989,10 +998,10 @@
         <v>5</v>
       </c>
       <c r="O6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q6">
         <v>52832240</v>
@@ -1003,158 +1012,158 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D7">
+        <v>266</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <v>186.2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7">
+        <v>19000</v>
+      </c>
+      <c r="N7">
         <v>70</v>
       </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7">
-        <v>70</v>
-      </c>
-      <c r="G7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" t="s">
-        <v>83</v>
-      </c>
-      <c r="J7" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" t="s">
-        <v>86</v>
-      </c>
-      <c r="L7" t="s">
-        <v>83</v>
-      </c>
-      <c r="M7">
-        <v>2000</v>
-      </c>
-      <c r="N7">
-        <v>100</v>
-      </c>
       <c r="O7" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="Q7">
-        <v>2625000</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D8">
-        <v>172.5</v>
+        <v>266</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F8">
-        <v>172.5</v>
+        <v>79.8</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K8" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M8">
-        <v>23000</v>
+        <v>19000</v>
       </c>
       <c r="N8">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O8" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="P8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="Q8">
-        <v>475800</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D9">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F9">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M9">
-        <v>9000</v>
+        <v>2000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="P9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q9">
-        <v>1055000</v>
+        <v>2625000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1165,102 +1174,102 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D10">
-        <v>200</v>
+        <v>172.5</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F10">
-        <v>200</v>
+        <v>172.5</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M10">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="N10">
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="P10" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="Q10">
-        <v>7500000</v>
+        <v>475800</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D11">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M11">
-        <v>18000</v>
+        <v>9000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="P11" t="s">
         <v>23</v>
       </c>
       <c r="Q11">
-        <v>487500</v>
+        <v>1055000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1271,34 +1280,34 @@
         <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D12">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F12">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1307,13 +1316,13 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="P12" t="s">
         <v>23</v>
       </c>
       <c r="Q12">
-        <v>6000000</v>
+        <v>7500000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1324,208 +1333,208 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D13">
-        <v>393.96</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F13">
-        <v>393.96</v>
+        <v>117</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M13">
-        <v>28000</v>
+        <v>18000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>90</v>
+        <v>26</v>
       </c>
       <c r="P13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q13">
-        <v>1055250</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D14">
-        <v>278.8</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F14">
-        <v>278.8</v>
+        <v>160</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M14">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P14" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="Q14">
-        <v>1221420</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D15">
-        <v>368.5</v>
+        <v>393.96</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F15">
-        <v>368.5</v>
+        <v>393.96</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M15">
-        <v>11000</v>
+        <v>28000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="P15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="Q15">
-        <v>2374500</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D16">
-        <v>297.5</v>
+        <v>278.8</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F16">
-        <v>297.5</v>
+        <v>278.8</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M16">
-        <v>7000</v>
+        <v>17000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P16" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Q16">
-        <v>3187500</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1536,155 +1545,155 @@
         <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D17">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F17">
-        <v>721.413</v>
+        <v>368.5</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M17">
-        <v>34700</v>
+        <v>11000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" t="s">
         <v>32</v>
       </c>
-      <c r="P17" t="s">
-        <v>28</v>
-      </c>
       <c r="Q17">
-        <v>1537150</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F18">
-        <v>441.12</v>
+        <v>297.5</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M18">
-        <v>30000</v>
+        <v>7000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P18" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="Q18">
-        <v>1072999</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19">
-        <v>4192.2496</v>
+        <v>721.413</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F19">
-        <v>2846.537406</v>
+        <v>721.413</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K19" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M19">
-        <v>36200</v>
+        <v>34700</v>
       </c>
       <c r="N19">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="P19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Q19">
-        <v>19108320</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1692,102 +1701,102 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20">
-        <v>4192.2496</v>
+        <v>441.12</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F20">
-        <v>1219.944706</v>
+        <v>441.12</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M20">
-        <v>36200</v>
+        <v>30000</v>
       </c>
       <c r="N20">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="P20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q20">
-        <v>19108320</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21">
         <v>4192.2496</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="F21">
-        <v>125.767488</v>
+        <v>2846.537406</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K21" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="L21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M21">
         <v>36200</v>
       </c>
       <c r="N21">
-        <v>3</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="P21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q21">
         <v>19108320</v>
@@ -1798,105 +1807,105 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D22">
-        <v>63.84</v>
+        <v>4192.2496</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F22">
-        <v>63.84</v>
+        <v>1219.944706</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M22">
-        <v>4000</v>
+        <v>36200</v>
       </c>
       <c r="N22">
-        <v>100</v>
+        <v>29.1</v>
       </c>
       <c r="O22" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q22">
-        <v>1197000</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D23">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F23">
-        <v>160</v>
+        <v>125.767488</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M23">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N23">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="O23" t="s">
         <v>93</v>
       </c>
       <c r="P23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="Q23">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1904,52 +1913,52 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D24">
-        <v>320</v>
+        <v>63.84</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F24">
-        <v>160</v>
+        <v>63.84</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K24" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="L24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M24">
-        <v>20000</v>
+        <v>4000</v>
       </c>
       <c r="N24">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Q24">
-        <v>2254770</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1957,52 +1966,52 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25">
-        <v>659.0825</v>
+        <v>320</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F25">
-        <v>659.0825</v>
+        <v>160</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K25" t="s">
         <v>86</v>
       </c>
       <c r="L25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M25">
-        <v>25000</v>
+        <v>20000</v>
       </c>
       <c r="N25">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O25" t="s">
+        <v>95</v>
+      </c>
+      <c r="P25" t="s">
         <v>35</v>
       </c>
-      <c r="P25" t="s">
-        <v>33</v>
-      </c>
       <c r="Q25">
-        <v>1827247</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -2013,49 +2022,49 @@
         <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D26">
-        <v>80</v>
+        <v>320</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K26" t="s">
         <v>86</v>
       </c>
       <c r="L26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M26">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="N26">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P26" t="s">
-        <v>92</v>
+        <v>35</v>
       </c>
       <c r="Q26">
-        <v>3000000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2066,302 +2075,302 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D27">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F27">
-        <v>126</v>
+        <v>659.0825</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K27" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M27">
-        <v>1800</v>
+        <v>25000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="P27" t="s">
-        <v>92</v>
+        <v>34</v>
       </c>
       <c r="Q27">
-        <v>4550000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D28">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F28">
-        <v>249.6</v>
+        <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M28">
-        <v>4800</v>
+        <v>2000</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="P28" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="Q28">
-        <v>3900000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s">
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D29">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F29">
-        <v>463.5</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K29" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M29">
-        <v>22500</v>
+        <v>1800</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="P29" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="Q29">
-        <v>1545000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D30">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F30">
-        <v>156</v>
+        <v>249.6</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M30">
-        <v>13000</v>
+        <v>4800</v>
       </c>
       <c r="N30">
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="P30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q30">
-        <v>840000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D31">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="E31" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F31">
-        <v>270</v>
+        <v>463.5</v>
       </c>
       <c r="G31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M31">
-        <v>7500</v>
+        <v>22500</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="P31" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
       <c r="Q31">
-        <v>2600000</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D32">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="F32">
-        <v>250</v>
+        <v>156</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M32">
-        <v>2000</v>
+        <v>13000</v>
       </c>
       <c r="N32">
         <v>100</v>
@@ -2370,63 +2379,63 @@
         <v>95</v>
       </c>
       <c r="P32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q32">
-        <v>9375000</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D33">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F33">
-        <v>178.41194</v>
+        <v>270</v>
       </c>
       <c r="G33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K33" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M33">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N33">
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="P33" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="Q33">
-        <v>787111</v>
+        <v>2600000</v>
       </c>
     </row>
     <row r="34" spans="1:17">
@@ -2437,49 +2446,49 @@
         <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="F34">
-        <v>49.66368</v>
+        <v>250</v>
       </c>
       <c r="G34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M34">
-        <v>4400</v>
+        <v>2000</v>
       </c>
       <c r="N34">
         <v>100</v>
       </c>
       <c r="O34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P34" t="s">
         <v>37</v>
       </c>
       <c r="Q34">
-        <v>846540</v>
+        <v>9375000</v>
       </c>
     </row>
     <row r="35" spans="1:17">
@@ -2490,34 +2499,34 @@
         <v>64</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D35">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="E35" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F35">
-        <v>306</v>
+        <v>178.41194</v>
       </c>
       <c r="G35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K35" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M35">
         <v>17000</v>
@@ -2526,54 +2535,54 @@
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P35" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="Q35">
-        <v>1119600</v>
+        <v>787111</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D36">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="F36">
-        <v>260</v>
+        <v>49.66368</v>
       </c>
       <c r="G36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K36" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M36">
-        <v>6500</v>
+        <v>4400</v>
       </c>
       <c r="N36">
         <v>100</v>
@@ -2582,9 +2591,115 @@
         <v>98</v>
       </c>
       <c r="P36" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q36">
+        <v>846540</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37">
+        <v>306</v>
+      </c>
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37">
+        <v>306</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" t="s">
+        <v>85</v>
+      </c>
+      <c r="I37" t="s">
+        <v>85</v>
+      </c>
+      <c r="J37" t="s">
+        <v>85</v>
+      </c>
+      <c r="K37" t="s">
+        <v>88</v>
+      </c>
+      <c r="L37" t="s">
+        <v>85</v>
+      </c>
+      <c r="M37">
+        <v>17000</v>
+      </c>
+      <c r="N37">
         <v>100</v>
       </c>
-      <c r="Q36">
+      <c r="O37" t="s">
+        <v>99</v>
+      </c>
+      <c r="P37" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q37">
+        <v>1119600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38">
+        <v>260</v>
+      </c>
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38">
+        <v>260</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" t="s">
+        <v>85</v>
+      </c>
+      <c r="I38" t="s">
+        <v>85</v>
+      </c>
+      <c r="J38" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38" t="s">
+        <v>88</v>
+      </c>
+      <c r="L38" t="s">
+        <v>85</v>
+      </c>
+      <c r="M38">
+        <v>6500</v>
+      </c>
+      <c r="N38">
+        <v>100</v>
+      </c>
+      <c r="O38" t="s">
+        <v>100</v>
+      </c>
+      <c r="P38" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q38">
         <v>2880000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-19
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="101">
   <si>
     <t>상장일</t>
   </si>
@@ -130,183 +130,180 @@
     <t>2023-10-27</t>
   </si>
   <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>퀄리타스반도체</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
     <t>2023-10-26</t>
   </si>
   <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>워트</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
     <t>2023-10-24</t>
   </si>
   <si>
@@ -316,16 +313,10 @@
     <t>2023-10-18</t>
   </si>
   <si>
-    <t>2023-10-16</t>
-  </si>
-  <si>
     <t>2023-12-07</t>
   </si>
   <si>
     <t>2023-11-30</t>
-  </si>
-  <si>
-    <t>2023-10-19</t>
   </si>
 </sst>
 </file>
@@ -683,7 +674,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q38"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -747,37 +738,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2">
         <v>877.5</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2">
         <v>361.96872</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M2">
         <v>6000</v>
@@ -800,37 +791,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3">
         <v>877.5</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F3">
         <v>361.96872</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M3">
         <v>6000</v>
@@ -853,37 +844,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4">
         <v>877.5</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4">
         <v>65.81256</v>
       </c>
       <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
         <v>85</v>
       </c>
-      <c r="H4" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" t="s">
-        <v>87</v>
-      </c>
       <c r="L4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M4">
         <v>6000</v>
@@ -906,37 +897,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>877.5</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F5">
         <v>43.875</v>
       </c>
       <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" t="s">
         <v>85</v>
       </c>
-      <c r="H5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K5" t="s">
-        <v>87</v>
-      </c>
       <c r="L5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M5">
         <v>6000</v>
@@ -959,37 +950,37 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6">
         <v>43.875</v>
       </c>
       <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" t="s">
+        <v>83</v>
+      </c>
+      <c r="J6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" t="s">
         <v>85</v>
       </c>
-      <c r="H6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" t="s">
-        <v>85</v>
-      </c>
-      <c r="K6" t="s">
-        <v>87</v>
-      </c>
       <c r="L6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -1012,37 +1003,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>266</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7">
         <v>186.2</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M7">
         <v>19000</v>
@@ -1054,7 +1045,7 @@
         <v>21</v>
       </c>
       <c r="P7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q7">
         <v>2100000</v>
@@ -1065,37 +1056,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>266</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8">
         <v>79.8</v>
       </c>
       <c r="G8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M8">
         <v>19000</v>
@@ -1107,7 +1098,7 @@
         <v>21</v>
       </c>
       <c r="P8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="Q8">
         <v>2100000</v>
@@ -1118,37 +1109,37 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F9">
         <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M9">
         <v>2000</v>
@@ -1157,7 +1148,7 @@
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P9" t="s">
         <v>23</v>
@@ -1171,37 +1162,37 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10">
         <v>172.5</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F10">
         <v>172.5</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M10">
         <v>23000</v>
@@ -1210,10 +1201,10 @@
         <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q10">
         <v>475800</v>
@@ -1224,37 +1215,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11">
         <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11">
         <v>135</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M11">
         <v>9000</v>
@@ -1263,7 +1254,7 @@
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P11" t="s">
         <v>23</v>
@@ -1277,37 +1268,37 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F12">
         <v>200</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M12">
         <v>2000</v>
@@ -1316,7 +1307,7 @@
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P12" t="s">
         <v>23</v>
@@ -1330,37 +1321,37 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F13">
         <v>117</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M13">
         <v>18000</v>
@@ -1383,37 +1374,37 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D14">
         <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F14">
         <v>160</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M14">
         <v>2000</v>
@@ -1436,37 +1427,37 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>393.96</v>
       </c>
       <c r="E15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F15">
         <v>393.96</v>
       </c>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M15">
         <v>28000</v>
@@ -1475,7 +1466,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P15" t="s">
         <v>26</v>
@@ -1489,37 +1480,37 @@
         <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>278.8</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F16">
         <v>278.8</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M16">
         <v>17000</v>
@@ -1531,7 +1522,7 @@
         <v>31</v>
       </c>
       <c r="P16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q16">
         <v>1221420</v>
@@ -1542,37 +1533,37 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D17">
         <v>368.5</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F17">
         <v>368.5</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M17">
         <v>11000</v>
@@ -1595,37 +1586,37 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>297.5</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F18">
         <v>297.5</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M18">
         <v>7000</v>
@@ -1637,7 +1628,7 @@
         <v>31</v>
       </c>
       <c r="P18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q18">
         <v>3187500</v>
@@ -1648,37 +1639,37 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>721.413</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F19">
         <v>721.413</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M19">
         <v>34700</v>
@@ -1701,37 +1692,37 @@
         <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D20">
         <v>441.12</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F20">
         <v>441.12</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M20">
         <v>30000</v>
@@ -1754,37 +1745,37 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21">
         <v>4192.2496</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F21">
         <v>2846.537406</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M21">
         <v>36200</v>
@@ -1793,7 +1784,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O21" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P21" t="s">
         <v>31</v>
@@ -1807,37 +1798,37 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D22">
         <v>4192.2496</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F22">
         <v>1219.944706</v>
       </c>
       <c r="G22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M22">
         <v>36200</v>
@@ -1846,7 +1837,7 @@
         <v>29.1</v>
       </c>
       <c r="O22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P22" t="s">
         <v>31</v>
@@ -1860,37 +1851,37 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D23">
         <v>4192.2496</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F23">
         <v>125.767488</v>
       </c>
       <c r="G23" t="s">
+        <v>83</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+      <c r="I23" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" t="s">
+        <v>83</v>
+      </c>
+      <c r="K23" t="s">
         <v>85</v>
       </c>
-      <c r="H23" t="s">
-        <v>85</v>
-      </c>
-      <c r="I23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J23" t="s">
-        <v>85</v>
-      </c>
-      <c r="K23" t="s">
-        <v>87</v>
-      </c>
       <c r="L23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M23">
         <v>36200</v>
@@ -1899,7 +1890,7 @@
         <v>3</v>
       </c>
       <c r="O23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P23" t="s">
         <v>31</v>
@@ -1913,37 +1904,37 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24">
         <v>63.84</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F24">
         <v>63.84</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M24">
         <v>4000</v>
@@ -1952,7 +1943,7 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P24" t="s">
         <v>30</v>
@@ -1966,37 +1957,37 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>320</v>
       </c>
       <c r="E25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F25">
         <v>160</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M25">
         <v>20000</v>
@@ -2005,7 +1996,7 @@
         <v>50</v>
       </c>
       <c r="O25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P25" t="s">
         <v>35</v>
@@ -2019,37 +2010,37 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26">
         <v>320</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F26">
         <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M26">
         <v>20000</v>
@@ -2058,7 +2049,7 @@
         <v>50</v>
       </c>
       <c r="O26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P26" t="s">
         <v>35</v>
@@ -2072,37 +2063,37 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27">
         <v>659.0825</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27">
         <v>659.0825</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M27">
         <v>25000</v>
@@ -2125,37 +2116,37 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28">
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F28">
         <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K28" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M28">
         <v>2000</v>
@@ -2164,10 +2155,10 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q28">
         <v>3000000</v>
@@ -2178,37 +2169,37 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D29">
         <v>126</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F29">
         <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M29">
         <v>1800</v>
@@ -2217,10 +2208,10 @@
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q29">
         <v>4550000</v>
@@ -2231,37 +2222,37 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D30">
         <v>249.6</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F30">
         <v>249.6</v>
       </c>
       <c r="G30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M30">
         <v>4800</v>
@@ -2270,7 +2261,7 @@
         <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P30" t="s">
         <v>35</v>
@@ -2284,37 +2275,37 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31">
         <v>463.5</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F31">
         <v>463.5</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M31">
         <v>22500</v>
@@ -2323,7 +2314,7 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P31" t="s">
         <v>35</v>
@@ -2337,37 +2328,37 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D32">
         <v>156</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F32">
         <v>156</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M32">
         <v>13000</v>
@@ -2376,7 +2367,7 @@
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P32" t="s">
         <v>35</v>
@@ -2390,37 +2381,37 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D33">
         <v>270</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F33">
         <v>270</v>
       </c>
       <c r="G33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M33">
         <v>7500</v>
@@ -2429,10 +2420,10 @@
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="P33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="Q33">
         <v>2600000</v>
@@ -2443,37 +2434,37 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D34">
         <v>250</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F34">
         <v>250</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M34">
         <v>2000</v>
@@ -2482,7 +2473,7 @@
         <v>100</v>
       </c>
       <c r="O34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P34" t="s">
         <v>37</v>
@@ -2496,37 +2487,37 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D35">
         <v>178.41194</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F35">
         <v>178.41194</v>
       </c>
       <c r="G35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M35">
         <v>17000</v>
@@ -2535,10 +2526,10 @@
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P35" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="Q35">
         <v>787111</v>
@@ -2549,37 +2540,37 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D36">
         <v>49.66368</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F36">
         <v>49.66368</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M36">
         <v>4400</v>
@@ -2588,10 +2579,10 @@
         <v>100</v>
       </c>
       <c r="O36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P36" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="Q36">
         <v>846540</v>
@@ -2602,37 +2593,37 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D37">
         <v>306</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F37">
         <v>306</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M37">
         <v>17000</v>
@@ -2641,66 +2632,13 @@
         <v>100</v>
       </c>
       <c r="O37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q37">
         <v>1119600</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38">
-        <v>260</v>
-      </c>
-      <c r="E38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38">
-        <v>260</v>
-      </c>
-      <c r="G38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38" t="s">
-        <v>85</v>
-      </c>
-      <c r="I38" t="s">
-        <v>85</v>
-      </c>
-      <c r="J38" t="s">
-        <v>85</v>
-      </c>
-      <c r="K38" t="s">
-        <v>88</v>
-      </c>
-      <c r="L38" t="s">
-        <v>85</v>
-      </c>
-      <c r="M38">
-        <v>6500</v>
-      </c>
-      <c r="N38">
-        <v>100</v>
-      </c>
-      <c r="O38" t="s">
-        <v>100</v>
-      </c>
-      <c r="P38" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q38">
-        <v>2880000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-23
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="107">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2023-12-22</t>
+  </si>
+  <si>
     <t>2023-12-12</t>
   </si>
   <si>
@@ -127,196 +130,211 @@
     <t>2023-11-02</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>KB제27호스팩</t>
+  </si>
+  <si>
+    <t>유진테크놀로지</t>
+  </si>
+  <si>
+    <t>유투바이오</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>신한</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-26</t>
+  </si>
+  <si>
+    <t>2023-10-24</t>
+  </si>
+  <si>
+    <t>2023-10-23</t>
+  </si>
+  <si>
+    <t>2023-12-19</t>
+  </si>
+  <si>
+    <t>2023-12-18</t>
+  </si>
+  <si>
+    <t>2023-12-15</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
     <t>2023-10-27</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>퀄리타스반도체</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-26</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-10-18</t>
-  </si>
-  <si>
-    <t>2023-12-07</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
   </si>
 </sst>
 </file>
@@ -674,7 +692,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -741,49 +759,49 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D2">
-        <v>877.5</v>
+        <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F2">
-        <v>361.96872</v>
+        <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M2">
-        <v>6000</v>
+        <v>100000</v>
       </c>
       <c r="N2">
-        <v>41.25</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="P2" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="Q2">
-        <v>52832240</v>
+        <v>1830000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -794,49 +812,49 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D3">
-        <v>877.5</v>
+        <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F3">
-        <v>361.96872</v>
+        <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M3">
-        <v>6000</v>
+        <v>100000</v>
       </c>
       <c r="N3">
-        <v>41.25</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="P3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="Q3">
-        <v>52832240</v>
+        <v>1830000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -844,52 +862,52 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D4">
-        <v>877.5</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F4">
-        <v>65.81256</v>
+        <v>140</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M4">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="N4">
-        <v>7.5</v>
+        <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="Q4">
-        <v>52832240</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -897,102 +915,102 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D5">
-        <v>877.5</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F5">
-        <v>43.875</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M5">
-        <v>6000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="Q5">
-        <v>52832240</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F6">
-        <v>43.875</v>
+        <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K6" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M6">
         <v>6000</v>
       </c>
       <c r="N6">
-        <v>5</v>
+        <v>41.25</v>
       </c>
       <c r="O6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q6">
         <v>52832240</v>
@@ -1003,52 +1021,52 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D7">
-        <v>266</v>
+        <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F7">
-        <v>186.2</v>
+        <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K7" t="s">
         <v>86</v>
       </c>
       <c r="L7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M7">
-        <v>19000</v>
+        <v>6000</v>
       </c>
       <c r="N7">
-        <v>70</v>
+        <v>41.25</v>
       </c>
       <c r="O7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" t="s">
         <v>21</v>
       </c>
-      <c r="P7" t="s">
-        <v>99</v>
-      </c>
       <c r="Q7">
-        <v>2100000</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1056,158 +1074,158 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D8">
-        <v>266</v>
+        <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F8">
-        <v>79.8</v>
+        <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="L8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M8">
-        <v>19000</v>
+        <v>6000</v>
       </c>
       <c r="N8">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="O8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" t="s">
         <v>21</v>
       </c>
-      <c r="P8" t="s">
-        <v>99</v>
-      </c>
       <c r="Q8">
-        <v>2100000</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D9">
-        <v>70</v>
+        <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F9">
-        <v>70</v>
+        <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>6000</v>
       </c>
       <c r="N9">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O9" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q9">
-        <v>2625000</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D10">
-        <v>172.5</v>
+        <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F10">
-        <v>172.5</v>
+        <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M10">
-        <v>23000</v>
+        <v>6000</v>
       </c>
       <c r="N10">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="P10" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="Q10">
-        <v>475800</v>
+        <v>52832240</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1218,1256 +1236,1256 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D11">
-        <v>135</v>
+        <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F11">
-        <v>135</v>
+        <v>186.2</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M11">
-        <v>9000</v>
+        <v>19000</v>
       </c>
       <c r="N11">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="Q11">
-        <v>1055000</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D12">
-        <v>200</v>
+        <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F12">
-        <v>200</v>
+        <v>79.8</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K12" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="L12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>19000</v>
       </c>
       <c r="N12">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O12" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>23</v>
+        <v>104</v>
       </c>
       <c r="Q12">
-        <v>7500000</v>
+        <v>2100000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D13">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F13">
-        <v>117</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L13" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M13">
-        <v>18000</v>
+        <v>2000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
       </c>
       <c r="Q13">
-        <v>487500</v>
+        <v>2625000</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D14">
-        <v>160</v>
+        <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F14">
-        <v>160</v>
+        <v>172.5</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>23000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="Q14">
-        <v>6000000</v>
+        <v>475800</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D15">
-        <v>393.96</v>
+        <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F15">
-        <v>393.96</v>
+        <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L15" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M15">
-        <v>28000</v>
+        <v>9000</v>
       </c>
       <c r="N15">
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="P15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Q15">
-        <v>1055250</v>
+        <v>1055000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D16">
-        <v>278.8</v>
+        <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F16">
-        <v>278.8</v>
+        <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M16">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="P16" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="Q16">
-        <v>1221420</v>
+        <v>7500000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D17">
-        <v>368.5</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F17">
-        <v>368.5</v>
+        <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M17">
-        <v>11000</v>
+        <v>18000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="P17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="Q17">
-        <v>2374500</v>
+        <v>487500</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D18">
-        <v>297.5</v>
+        <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F18">
-        <v>297.5</v>
+        <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L18" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M18">
-        <v>7000</v>
+        <v>2000</v>
       </c>
       <c r="N18">
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="P18" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="Q18">
-        <v>3187500</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D19">
-        <v>721.413</v>
+        <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F19">
-        <v>721.413</v>
+        <v>393.96</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M19">
-        <v>34700</v>
+        <v>28000</v>
       </c>
       <c r="N19">
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="P19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Q19">
-        <v>1537150</v>
+        <v>1055250</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D20">
-        <v>441.12</v>
+        <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F20">
-        <v>441.12</v>
+        <v>278.8</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M20">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P20" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="Q20">
-        <v>1072999</v>
+        <v>1221420</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21">
-        <v>4192.2496</v>
+        <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F21">
-        <v>2846.537406</v>
+        <v>368.5</v>
       </c>
       <c r="G21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K21" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M21">
-        <v>36200</v>
+        <v>11000</v>
       </c>
       <c r="N21">
-        <v>67.90000000000001</v>
+        <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="P21" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q21">
-        <v>19108320</v>
+        <v>2374500</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D22">
-        <v>4192.2496</v>
+        <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F22">
-        <v>1219.944706</v>
+        <v>297.5</v>
       </c>
       <c r="G22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K22" t="s">
         <v>87</v>
       </c>
       <c r="L22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M22">
-        <v>36200</v>
+        <v>7000</v>
       </c>
       <c r="N22">
-        <v>29.1</v>
+        <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="Q22">
-        <v>19108320</v>
+        <v>3187500</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D23">
-        <v>4192.2496</v>
+        <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23">
-        <v>125.767488</v>
+        <v>721.413</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K23" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M23">
-        <v>36200</v>
+        <v>34700</v>
       </c>
       <c r="N23">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>91</v>
+        <v>34</v>
       </c>
       <c r="P23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q23">
-        <v>19108320</v>
+        <v>1537150</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D24">
-        <v>63.84</v>
+        <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F24">
-        <v>63.84</v>
+        <v>441.12</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K24" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M24">
-        <v>4000</v>
+        <v>30000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="P24" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q24">
-        <v>1197000</v>
+        <v>1072999</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D25">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F25">
-        <v>160</v>
+        <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K25" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M25">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N25">
-        <v>50</v>
+        <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q25">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D26">
-        <v>320</v>
+        <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F26">
-        <v>160</v>
+        <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K26" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="L26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M26">
-        <v>20000</v>
+        <v>36200</v>
       </c>
       <c r="N26">
-        <v>50</v>
+        <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="P26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="Q26">
-        <v>2254770</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D27">
-        <v>659.0825</v>
+        <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F27">
-        <v>659.0825</v>
+        <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K27" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="L27" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M27">
-        <v>25000</v>
+        <v>36200</v>
       </c>
       <c r="N27">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>36</v>
+        <v>94</v>
       </c>
       <c r="P27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q27">
-        <v>1827247</v>
+        <v>19108320</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D28">
-        <v>80</v>
+        <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F28">
-        <v>80</v>
+        <v>63.84</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L28" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M28">
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P28" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="Q28">
-        <v>3000000</v>
+        <v>1197000</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D29">
-        <v>126</v>
+        <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="F29">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K29" t="s">
         <v>86</v>
       </c>
       <c r="L29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M29">
-        <v>1800</v>
+        <v>20000</v>
       </c>
       <c r="N29">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O29" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="P29" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="Q29">
-        <v>4550000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D30">
-        <v>249.6</v>
+        <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="F30">
-        <v>249.6</v>
+        <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K30" t="s">
         <v>86</v>
       </c>
       <c r="L30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M30">
-        <v>4800</v>
+        <v>20000</v>
       </c>
       <c r="N30">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O30" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="P30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q30">
-        <v>3900000</v>
+        <v>2254770</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D31">
-        <v>463.5</v>
+        <v>659.0825</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F31">
-        <v>463.5</v>
+        <v>659.0825</v>
       </c>
       <c r="G31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L31" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M31">
-        <v>22500</v>
+        <v>25000</v>
       </c>
       <c r="N31">
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="P31" t="s">
         <v>35</v>
       </c>
       <c r="Q31">
-        <v>1545000</v>
+        <v>1827247</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D32">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F32">
-        <v>156</v>
+        <v>80</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L32" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M32">
-        <v>13000</v>
+        <v>2000</v>
       </c>
       <c r="N32">
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="P32" t="s">
-        <v>35</v>
+        <v>95</v>
       </c>
       <c r="Q32">
-        <v>840000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D33">
-        <v>270</v>
+        <v>126</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F33">
-        <v>270</v>
+        <v>126</v>
       </c>
       <c r="G33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K33" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M33">
-        <v>7500</v>
+        <v>1800</v>
       </c>
       <c r="N33">
         <v>100</v>
       </c>
       <c r="O33" t="s">
+        <v>97</v>
+      </c>
+      <c r="P33" t="s">
         <v>95</v>
       </c>
-      <c r="P33" t="s">
-        <v>93</v>
-      </c>
       <c r="Q33">
-        <v>2600000</v>
+        <v>4550000</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D34">
-        <v>250</v>
+        <v>249.6</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F34">
-        <v>250</v>
+        <v>249.6</v>
       </c>
       <c r="G34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K34" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M34">
-        <v>2000</v>
+        <v>4800</v>
       </c>
       <c r="N34">
         <v>100</v>
@@ -2476,157 +2494,157 @@
         <v>96</v>
       </c>
       <c r="P34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q34">
-        <v>9375000</v>
+        <v>3900000</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D35">
-        <v>178.41194</v>
+        <v>463.5</v>
       </c>
       <c r="E35" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F35">
-        <v>178.41194</v>
+        <v>463.5</v>
       </c>
       <c r="G35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K35" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L35" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M35">
-        <v>17000</v>
+        <v>22500</v>
       </c>
       <c r="N35">
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P35" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="Q35">
-        <v>787111</v>
+        <v>1545000</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D36">
-        <v>49.66368</v>
+        <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="F36">
-        <v>49.66368</v>
+        <v>156</v>
       </c>
       <c r="G36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L36" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M36">
-        <v>4400</v>
+        <v>13000</v>
       </c>
       <c r="N36">
         <v>100</v>
       </c>
       <c r="O36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="P36" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="Q36">
-        <v>846540</v>
+        <v>840000</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D37">
-        <v>306</v>
+        <v>270</v>
       </c>
       <c r="E37" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F37">
-        <v>306</v>
+        <v>270</v>
       </c>
       <c r="G37" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H37" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="I37" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J37" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="L37" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M37">
-        <v>17000</v>
+        <v>7500</v>
       </c>
       <c r="N37">
         <v>100</v>
@@ -2635,10 +2653,169 @@
         <v>98</v>
       </c>
       <c r="P37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q37">
-        <v>1119600</v>
+        <v>2600000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38">
+        <v>250</v>
+      </c>
+      <c r="E38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38">
+        <v>250</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" t="s">
+        <v>85</v>
+      </c>
+      <c r="I38" t="s">
+        <v>85</v>
+      </c>
+      <c r="J38" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38" t="s">
+        <v>87</v>
+      </c>
+      <c r="L38" t="s">
+        <v>85</v>
+      </c>
+      <c r="M38">
+        <v>2000</v>
+      </c>
+      <c r="N38">
+        <v>100</v>
+      </c>
+      <c r="O38" t="s">
+        <v>99</v>
+      </c>
+      <c r="P38" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q38">
+        <v>9375000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>178.41194</v>
+      </c>
+      <c r="E39" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39">
+        <v>178.41194</v>
+      </c>
+      <c r="G39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39" t="s">
+        <v>85</v>
+      </c>
+      <c r="I39" t="s">
+        <v>85</v>
+      </c>
+      <c r="J39" t="s">
+        <v>85</v>
+      </c>
+      <c r="K39" t="s">
+        <v>87</v>
+      </c>
+      <c r="L39" t="s">
+        <v>85</v>
+      </c>
+      <c r="M39">
+        <v>17000</v>
+      </c>
+      <c r="N39">
+        <v>100</v>
+      </c>
+      <c r="O39" t="s">
+        <v>100</v>
+      </c>
+      <c r="P39" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q39">
+        <v>787111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>49.66368</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40">
+        <v>49.66368</v>
+      </c>
+      <c r="G40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" t="s">
+        <v>85</v>
+      </c>
+      <c r="I40" t="s">
+        <v>85</v>
+      </c>
+      <c r="J40" t="s">
+        <v>85</v>
+      </c>
+      <c r="K40" t="s">
+        <v>87</v>
+      </c>
+      <c r="L40" t="s">
+        <v>85</v>
+      </c>
+      <c r="M40">
+        <v>4400</v>
+      </c>
+      <c r="N40">
+        <v>100</v>
+      </c>
+      <c r="O40" t="s">
+        <v>100</v>
+      </c>
+      <c r="P40" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q40">
+        <v>846540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-27
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="100">
   <si>
     <t>상장일</t>
   </si>
@@ -124,217 +124,196 @@
     <t>2023-11-07</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>쏘닉스</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-02</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-10-26</t>
+  </si>
+  <si>
+    <t>2023-12-19</t>
+  </si>
+  <si>
+    <t>2023-12-18</t>
+  </si>
+  <si>
+    <t>2023-12-15</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
     <t>2023-11-03</t>
-  </si>
-  <si>
-    <t>2023-11-02</t>
-  </si>
-  <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>KB제27호스팩</t>
-  </si>
-  <si>
-    <t>유진테크놀로지</t>
-  </si>
-  <si>
-    <t>유투바이오</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>신한</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-26</t>
-  </si>
-  <si>
-    <t>2023-10-24</t>
-  </si>
-  <si>
-    <t>2023-10-23</t>
-  </si>
-  <si>
-    <t>2023-12-19</t>
-  </si>
-  <si>
-    <t>2023-12-18</t>
-  </si>
-  <si>
-    <t>2023-12-15</t>
-  </si>
-  <si>
-    <t>2023-12-07</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
-  </si>
-  <si>
-    <t>2023-10-27</t>
   </si>
 </sst>
 </file>
@@ -692,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -756,37 +735,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -795,10 +774,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -809,37 +788,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -848,10 +827,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P3" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -862,37 +841,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -904,7 +883,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -915,37 +894,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -957,7 +936,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -968,37 +947,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -1021,37 +1000,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1074,37 +1053,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="L8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1127,37 +1106,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K9" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="L9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1180,37 +1159,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="L10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1233,37 +1212,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1275,7 +1254,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1286,37 +1265,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K12" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1328,7 +1307,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1339,37 +1318,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1378,7 +1357,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1392,37 +1371,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1431,10 +1410,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="P14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1445,37 +1424,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1484,7 +1463,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1498,37 +1477,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1537,7 +1516,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1551,37 +1530,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1604,37 +1583,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K18" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1657,37 +1636,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1696,7 +1675,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1710,37 +1689,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1752,7 +1731,7 @@
         <v>32</v>
       </c>
       <c r="P20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1763,37 +1742,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K21" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1816,37 +1795,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K22" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L22" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1858,7 +1837,7 @@
         <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1869,37 +1848,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K23" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -1922,37 +1901,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -1975,37 +1954,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -2014,7 +1993,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="P25" t="s">
         <v>32</v>
@@ -2028,37 +2007,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L26" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2067,7 +2046,7 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="P26" t="s">
         <v>32</v>
@@ -2081,37 +2060,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H27" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I27" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J27" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="L27" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2120,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="P27" t="s">
         <v>32</v>
@@ -2134,37 +2113,37 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D28">
         <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F28">
         <v>63.84</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I28" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J28" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K28" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L28" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M28">
         <v>4000</v>
@@ -2173,7 +2152,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
@@ -2187,37 +2166,37 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D29">
         <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F29">
         <v>160</v>
       </c>
       <c r="G29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K29" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L29" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M29">
         <v>20000</v>
@@ -2226,10 +2205,10 @@
         <v>50</v>
       </c>
       <c r="O29" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P29" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="Q29">
         <v>2254770</v>
@@ -2240,37 +2219,37 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D30">
         <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F30">
         <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K30" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="L30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M30">
         <v>20000</v>
@@ -2279,10 +2258,10 @@
         <v>50</v>
       </c>
       <c r="O30" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P30" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="Q30">
         <v>2254770</v>
@@ -2293,37 +2272,37 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D31">
         <v>659.0825</v>
       </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F31">
         <v>659.0825</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L31" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M31">
         <v>25000</v>
@@ -2332,7 +2311,7 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="P31" t="s">
         <v>35</v>
@@ -2346,37 +2325,37 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D32">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F32">
         <v>80</v>
       </c>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K32" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L32" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M32">
         <v>2000</v>
@@ -2385,10 +2364,10 @@
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="P32" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Q32">
         <v>3000000</v>
@@ -2399,37 +2378,37 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>126</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F33">
         <v>126</v>
       </c>
       <c r="G33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K33" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L33" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M33">
         <v>1800</v>
@@ -2438,10 +2417,10 @@
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="P33" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="Q33">
         <v>4550000</v>
@@ -2452,37 +2431,37 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>249.6</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F34">
         <v>249.6</v>
       </c>
       <c r="G34" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H34" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I34" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J34" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K34" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L34" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M34">
         <v>4800</v>
@@ -2491,10 +2470,10 @@
         <v>100</v>
       </c>
       <c r="O34" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P34" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="Q34">
         <v>3900000</v>
@@ -2505,37 +2484,37 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D35">
         <v>463.5</v>
       </c>
       <c r="E35" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F35">
         <v>463.5</v>
       </c>
       <c r="G35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K35" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M35">
         <v>22500</v>
@@ -2544,10 +2523,10 @@
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P35" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="Q35">
         <v>1545000</v>
@@ -2558,37 +2537,37 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D36">
         <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F36">
         <v>156</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K36" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L36" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M36">
         <v>13000</v>
@@ -2597,10 +2576,10 @@
         <v>100</v>
       </c>
       <c r="O36" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="P36" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="Q36">
         <v>840000</v>
@@ -2611,37 +2590,37 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D37">
         <v>270</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F37">
         <v>270</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="K37" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="L37" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M37">
         <v>7500</v>
@@ -2650,172 +2629,13 @@
         <v>100</v>
       </c>
       <c r="O37" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="P37" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="Q37">
         <v>2600000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" t="s">
-        <v>69</v>
-      </c>
-      <c r="D38">
-        <v>250</v>
-      </c>
-      <c r="E38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38">
-        <v>250</v>
-      </c>
-      <c r="G38" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38" t="s">
-        <v>85</v>
-      </c>
-      <c r="I38" t="s">
-        <v>85</v>
-      </c>
-      <c r="J38" t="s">
-        <v>85</v>
-      </c>
-      <c r="K38" t="s">
-        <v>87</v>
-      </c>
-      <c r="L38" t="s">
-        <v>85</v>
-      </c>
-      <c r="M38">
-        <v>2000</v>
-      </c>
-      <c r="N38">
-        <v>100</v>
-      </c>
-      <c r="O38" t="s">
-        <v>99</v>
-      </c>
-      <c r="P38" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q38">
-        <v>9375000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39">
-        <v>178.41194</v>
-      </c>
-      <c r="E39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39">
-        <v>178.41194</v>
-      </c>
-      <c r="G39" t="s">
-        <v>85</v>
-      </c>
-      <c r="H39" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" t="s">
-        <v>85</v>
-      </c>
-      <c r="J39" t="s">
-        <v>85</v>
-      </c>
-      <c r="K39" t="s">
-        <v>87</v>
-      </c>
-      <c r="L39" t="s">
-        <v>85</v>
-      </c>
-      <c r="M39">
-        <v>17000</v>
-      </c>
-      <c r="N39">
-        <v>100</v>
-      </c>
-      <c r="O39" t="s">
-        <v>100</v>
-      </c>
-      <c r="P39" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q39">
-        <v>787111</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40">
-        <v>49.66368</v>
-      </c>
-      <c r="E40" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40">
-        <v>49.66368</v>
-      </c>
-      <c r="G40" t="s">
-        <v>85</v>
-      </c>
-      <c r="H40" t="s">
-        <v>85</v>
-      </c>
-      <c r="I40" t="s">
-        <v>85</v>
-      </c>
-      <c r="J40" t="s">
-        <v>85</v>
-      </c>
-      <c r="K40" t="s">
-        <v>87</v>
-      </c>
-      <c r="L40" t="s">
-        <v>85</v>
-      </c>
-      <c r="M40">
-        <v>4400</v>
-      </c>
-      <c r="N40">
-        <v>100</v>
-      </c>
-      <c r="O40" t="s">
-        <v>100</v>
-      </c>
-      <c r="P40" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q40">
-        <v>846540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2023-12-31
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="98">
   <si>
     <t>상장일</t>
   </si>
@@ -121,199 +121,193 @@
     <t>2023-11-10</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>메가터치</t>
+  </si>
+  <si>
+    <t>컨텍</t>
+  </si>
+  <si>
+    <t>비아이매트릭스</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-02</t>
+  </si>
+  <si>
+    <t>2023-11-01</t>
+  </si>
+  <si>
+    <t>2023-12-19</t>
+  </si>
+  <si>
+    <t>2023-12-18</t>
+  </si>
+  <si>
+    <t>2023-12-15</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
+    <t>2023-11-03</t>
+  </si>
+  <si>
     <t>2023-11-07</t>
-  </si>
-  <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>쏘닉스</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-02</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-10-26</t>
-  </si>
-  <si>
-    <t>2023-12-19</t>
-  </si>
-  <si>
-    <t>2023-12-18</t>
-  </si>
-  <si>
-    <t>2023-12-15</t>
-  </si>
-  <si>
-    <t>2023-12-07</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
-  </si>
-  <si>
-    <t>2023-11-03</t>
   </si>
 </sst>
 </file>
@@ -671,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -735,37 +729,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -774,10 +768,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -788,37 +782,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -827,10 +821,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -841,37 +835,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" t="s">
         <v>79</v>
       </c>
-      <c r="H4" t="s">
-        <v>79</v>
-      </c>
-      <c r="I4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J4" t="s">
-        <v>79</v>
-      </c>
-      <c r="K4" t="s">
-        <v>81</v>
-      </c>
       <c r="L4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -883,7 +877,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -894,37 +888,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+      <c r="I5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K5" t="s">
         <v>79</v>
       </c>
-      <c r="H5" t="s">
-        <v>79</v>
-      </c>
-      <c r="I5" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" t="s">
-        <v>79</v>
-      </c>
-      <c r="K5" t="s">
-        <v>81</v>
-      </c>
       <c r="L5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -936,7 +930,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -947,37 +941,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -1000,37 +994,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1053,37 +1047,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1106,37 +1100,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1159,37 +1153,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1212,37 +1206,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K11" t="s">
         <v>79</v>
       </c>
-      <c r="H11" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" t="s">
-        <v>81</v>
-      </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1254,7 +1248,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1265,37 +1259,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1307,7 +1301,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1318,37 +1312,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K13" t="s">
         <v>79</v>
       </c>
-      <c r="H13" t="s">
-        <v>79</v>
-      </c>
-      <c r="I13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J13" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" t="s">
-        <v>81</v>
-      </c>
       <c r="L13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1357,7 +1351,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1371,37 +1365,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I14" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" t="s">
         <v>79</v>
       </c>
-      <c r="H14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" t="s">
-        <v>79</v>
-      </c>
-      <c r="K14" t="s">
-        <v>81</v>
-      </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1410,10 +1404,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1424,37 +1418,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" t="s">
         <v>79</v>
       </c>
-      <c r="H15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I15" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" t="s">
-        <v>79</v>
-      </c>
-      <c r="K15" t="s">
-        <v>81</v>
-      </c>
       <c r="L15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1463,7 +1457,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1477,37 +1471,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
         <v>79</v>
       </c>
-      <c r="H16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I16" t="s">
-        <v>79</v>
-      </c>
-      <c r="J16" t="s">
-        <v>79</v>
-      </c>
-      <c r="K16" t="s">
-        <v>81</v>
-      </c>
       <c r="L16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1516,7 +1510,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1530,37 +1524,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="s">
         <v>79</v>
       </c>
-      <c r="H17" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" t="s">
-        <v>79</v>
-      </c>
-      <c r="J17" t="s">
-        <v>79</v>
-      </c>
-      <c r="K17" t="s">
-        <v>81</v>
-      </c>
       <c r="L17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1583,37 +1577,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I18" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
         <v>79</v>
       </c>
-      <c r="H18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" t="s">
-        <v>79</v>
-      </c>
-      <c r="J18" t="s">
-        <v>79</v>
-      </c>
-      <c r="K18" t="s">
-        <v>81</v>
-      </c>
       <c r="L18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1636,37 +1630,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" t="s">
         <v>79</v>
       </c>
-      <c r="H19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" t="s">
-        <v>79</v>
-      </c>
-      <c r="J19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K19" t="s">
-        <v>81</v>
-      </c>
       <c r="L19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1675,7 +1669,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1689,37 +1683,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>77</v>
+      </c>
+      <c r="I20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" t="s">
         <v>79</v>
       </c>
-      <c r="H20" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" t="s">
-        <v>79</v>
-      </c>
-      <c r="J20" t="s">
-        <v>79</v>
-      </c>
-      <c r="K20" t="s">
-        <v>81</v>
-      </c>
       <c r="L20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1731,7 +1725,7 @@
         <v>32</v>
       </c>
       <c r="P20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1742,37 +1736,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" t="s">
         <v>79</v>
       </c>
-      <c r="H21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K21" t="s">
-        <v>81</v>
-      </c>
       <c r="L21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1795,37 +1789,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I22" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" t="s">
         <v>79</v>
       </c>
-      <c r="H22" t="s">
-        <v>79</v>
-      </c>
-      <c r="I22" t="s">
-        <v>79</v>
-      </c>
-      <c r="J22" t="s">
-        <v>79</v>
-      </c>
-      <c r="K22" t="s">
-        <v>81</v>
-      </c>
       <c r="L22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1837,7 +1831,7 @@
         <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1848,37 +1842,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" t="s">
+        <v>77</v>
+      </c>
+      <c r="J23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" t="s">
         <v>79</v>
       </c>
-      <c r="H23" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J23" t="s">
-        <v>79</v>
-      </c>
-      <c r="K23" t="s">
-        <v>81</v>
-      </c>
       <c r="L23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -1901,37 +1895,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H24" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" t="s">
+        <v>77</v>
+      </c>
+      <c r="J24" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" t="s">
         <v>79</v>
       </c>
-      <c r="H24" t="s">
-        <v>79</v>
-      </c>
-      <c r="I24" t="s">
-        <v>79</v>
-      </c>
-      <c r="J24" t="s">
-        <v>79</v>
-      </c>
-      <c r="K24" t="s">
-        <v>81</v>
-      </c>
       <c r="L24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -1954,37 +1948,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
         <v>79</v>
       </c>
-      <c r="H25" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" t="s">
-        <v>79</v>
-      </c>
-      <c r="J25" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" t="s">
-        <v>81</v>
-      </c>
       <c r="L25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -1993,7 +1987,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P25" t="s">
         <v>32</v>
@@ -2007,37 +2001,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2046,7 +2040,7 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P26" t="s">
         <v>32</v>
@@ -2060,37 +2054,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2099,7 +2093,7 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P27" t="s">
         <v>32</v>
@@ -2113,37 +2107,37 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28">
         <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F28">
         <v>63.84</v>
       </c>
       <c r="G28" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" t="s">
+        <v>77</v>
+      </c>
+      <c r="I28" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28" t="s">
         <v>79</v>
       </c>
-      <c r="H28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" t="s">
-        <v>79</v>
-      </c>
-      <c r="K28" t="s">
-        <v>81</v>
-      </c>
       <c r="L28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M28">
         <v>4000</v>
@@ -2152,7 +2146,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
@@ -2166,37 +2160,37 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F29">
         <v>160</v>
       </c>
       <c r="G29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M29">
         <v>20000</v>
@@ -2205,10 +2199,10 @@
         <v>50</v>
       </c>
       <c r="O29" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P29" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q29">
         <v>2254770</v>
@@ -2219,37 +2213,37 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D30">
         <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F30">
         <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M30">
         <v>20000</v>
@@ -2258,10 +2252,10 @@
         <v>50</v>
       </c>
       <c r="O30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P30" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q30">
         <v>2254770</v>
@@ -2272,37 +2266,37 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D31">
         <v>659.0825</v>
       </c>
       <c r="E31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F31">
         <v>659.0825</v>
       </c>
       <c r="G31" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" t="s">
+        <v>77</v>
+      </c>
+      <c r="I31" t="s">
+        <v>77</v>
+      </c>
+      <c r="J31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="s">
         <v>79</v>
       </c>
-      <c r="H31" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" t="s">
-        <v>79</v>
-      </c>
-      <c r="J31" t="s">
-        <v>79</v>
-      </c>
-      <c r="K31" t="s">
-        <v>81</v>
-      </c>
       <c r="L31" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M31">
         <v>25000</v>
@@ -2311,10 +2305,10 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P31" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="Q31">
         <v>1827247</v>
@@ -2325,37 +2319,37 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D32">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F32">
         <v>80</v>
       </c>
       <c r="G32" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32" t="s">
+        <v>77</v>
+      </c>
+      <c r="J32" t="s">
+        <v>77</v>
+      </c>
+      <c r="K32" t="s">
         <v>79</v>
       </c>
-      <c r="H32" t="s">
-        <v>79</v>
-      </c>
-      <c r="I32" t="s">
-        <v>79</v>
-      </c>
-      <c r="J32" t="s">
-        <v>79</v>
-      </c>
-      <c r="K32" t="s">
-        <v>81</v>
-      </c>
       <c r="L32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M32">
         <v>2000</v>
@@ -2364,10 +2358,10 @@
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q32">
         <v>3000000</v>
@@ -2378,37 +2372,37 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D33">
         <v>126</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F33">
         <v>126</v>
       </c>
       <c r="G33" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" t="s">
+        <v>77</v>
+      </c>
+      <c r="I33" t="s">
+        <v>77</v>
+      </c>
+      <c r="J33" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" t="s">
         <v>79</v>
       </c>
-      <c r="H33" t="s">
-        <v>79</v>
-      </c>
-      <c r="I33" t="s">
-        <v>79</v>
-      </c>
-      <c r="J33" t="s">
-        <v>79</v>
-      </c>
-      <c r="K33" t="s">
-        <v>81</v>
-      </c>
       <c r="L33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M33">
         <v>1800</v>
@@ -2417,10 +2411,10 @@
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q33">
         <v>4550000</v>
@@ -2431,37 +2425,37 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D34">
         <v>249.6</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F34">
         <v>249.6</v>
       </c>
       <c r="G34" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" t="s">
+        <v>77</v>
+      </c>
+      <c r="I34" t="s">
+        <v>77</v>
+      </c>
+      <c r="J34" t="s">
+        <v>77</v>
+      </c>
+      <c r="K34" t="s">
         <v>79</v>
       </c>
-      <c r="H34" t="s">
-        <v>79</v>
-      </c>
-      <c r="I34" t="s">
-        <v>79</v>
-      </c>
-      <c r="J34" t="s">
-        <v>79</v>
-      </c>
-      <c r="K34" t="s">
-        <v>81</v>
-      </c>
       <c r="L34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M34">
         <v>4800</v>
@@ -2470,10 +2464,10 @@
         <v>100</v>
       </c>
       <c r="O34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q34">
         <v>3900000</v>
@@ -2484,37 +2478,37 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D35">
         <v>463.5</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F35">
         <v>463.5</v>
       </c>
       <c r="G35" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" t="s">
+        <v>77</v>
+      </c>
+      <c r="I35" t="s">
+        <v>77</v>
+      </c>
+      <c r="J35" t="s">
+        <v>77</v>
+      </c>
+      <c r="K35" t="s">
         <v>79</v>
       </c>
-      <c r="H35" t="s">
-        <v>79</v>
-      </c>
-      <c r="I35" t="s">
-        <v>79</v>
-      </c>
-      <c r="J35" t="s">
-        <v>79</v>
-      </c>
-      <c r="K35" t="s">
-        <v>81</v>
-      </c>
       <c r="L35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M35">
         <v>22500</v>
@@ -2523,10 +2517,10 @@
         <v>100</v>
       </c>
       <c r="O35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q35">
         <v>1545000</v>
@@ -2537,37 +2531,37 @@
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D36">
         <v>156</v>
       </c>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F36">
         <v>156</v>
       </c>
       <c r="G36" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" t="s">
+        <v>77</v>
+      </c>
+      <c r="J36" t="s">
+        <v>77</v>
+      </c>
+      <c r="K36" t="s">
         <v>79</v>
       </c>
-      <c r="H36" t="s">
-        <v>79</v>
-      </c>
-      <c r="I36" t="s">
-        <v>79</v>
-      </c>
-      <c r="J36" t="s">
-        <v>79</v>
-      </c>
-      <c r="K36" t="s">
-        <v>81</v>
-      </c>
       <c r="L36" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M36">
         <v>13000</v>
@@ -2576,66 +2570,13 @@
         <v>100</v>
       </c>
       <c r="O36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P36" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="Q36">
         <v>840000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37">
-        <v>270</v>
-      </c>
-      <c r="E37" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37">
-        <v>270</v>
-      </c>
-      <c r="G37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H37" t="s">
-        <v>79</v>
-      </c>
-      <c r="I37" t="s">
-        <v>79</v>
-      </c>
-      <c r="J37" t="s">
-        <v>79</v>
-      </c>
-      <c r="K37" t="s">
-        <v>81</v>
-      </c>
-      <c r="L37" t="s">
-        <v>79</v>
-      </c>
-      <c r="M37">
-        <v>7500</v>
-      </c>
-      <c r="N37">
-        <v>100</v>
-      </c>
-      <c r="O37" t="s">
-        <v>93</v>
-      </c>
-      <c r="P37" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q37">
-        <v>2600000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-01-03
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="95">
   <si>
     <t>상장일</t>
   </si>
@@ -118,160 +118,151 @@
     <t>2023-11-14</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>한국제13호스팩</t>
+  </si>
+  <si>
+    <t>에스와이스틸텍</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>한국</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
     <t>2023-11-10</t>
-  </si>
-  <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>메가터치</t>
-  </si>
-  <si>
-    <t>컨텍</t>
-  </si>
-  <si>
-    <t>비아이매트릭스</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
   </si>
   <si>
     <t>2023-11-08</t>
@@ -665,7 +656,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -729,37 +720,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -768,10 +759,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="P2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -782,37 +773,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -821,10 +812,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="P3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -835,37 +826,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -877,7 +868,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -888,37 +879,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -930,7 +921,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -941,37 +932,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -994,37 +985,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1047,37 +1038,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1100,37 +1091,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1153,37 +1144,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1206,37 +1197,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1248,7 +1239,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1259,37 +1250,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" t="s">
         <v>77</v>
       </c>
-      <c r="H12" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" t="s">
-        <v>77</v>
-      </c>
-      <c r="K12" t="s">
-        <v>81</v>
-      </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1301,7 +1292,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1312,37 +1303,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1351,7 +1342,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1365,37 +1356,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1404,10 +1395,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="P14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1418,37 +1409,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1457,7 +1448,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1471,37 +1462,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1510,7 +1501,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1524,37 +1515,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1577,37 +1568,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1630,37 +1621,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1669,7 +1660,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1683,37 +1674,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1725,7 +1716,7 @@
         <v>32</v>
       </c>
       <c r="P20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1736,37 +1727,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L21" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1789,37 +1780,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1831,7 +1822,7 @@
         <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1842,37 +1833,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -1881,7 +1872,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -1895,37 +1886,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -1948,37 +1939,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K25" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L25" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -1987,7 +1978,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P25" t="s">
         <v>32</v>
@@ -2001,37 +1992,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K26" t="s">
         <v>77</v>
       </c>
-      <c r="H26" t="s">
-        <v>77</v>
-      </c>
-      <c r="I26" t="s">
-        <v>77</v>
-      </c>
-      <c r="J26" t="s">
-        <v>77</v>
-      </c>
-      <c r="K26" t="s">
-        <v>81</v>
-      </c>
       <c r="L26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2040,7 +2031,7 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P26" t="s">
         <v>32</v>
@@ -2054,37 +2045,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="L27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2093,7 +2084,7 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P27" t="s">
         <v>32</v>
@@ -2107,37 +2098,37 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F28">
         <v>63.84</v>
       </c>
       <c r="G28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K28" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M28">
         <v>4000</v>
@@ -2146,7 +2137,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
@@ -2160,37 +2151,37 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D29">
         <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F29">
         <v>160</v>
       </c>
       <c r="G29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M29">
         <v>20000</v>
@@ -2199,10 +2190,10 @@
         <v>50</v>
       </c>
       <c r="O29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Q29">
         <v>2254770</v>
@@ -2213,37 +2204,37 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D30">
         <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F30">
         <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K30" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M30">
         <v>20000</v>
@@ -2252,10 +2243,10 @@
         <v>50</v>
       </c>
       <c r="O30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="P30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Q30">
         <v>2254770</v>
@@ -2266,37 +2257,37 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D31">
         <v>659.0825</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F31">
         <v>659.0825</v>
       </c>
       <c r="G31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L31" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M31">
         <v>25000</v>
@@ -2305,10 +2296,10 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="P31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q31">
         <v>1827247</v>
@@ -2319,37 +2310,37 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>80</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F32">
         <v>80</v>
       </c>
       <c r="G32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K32" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L32" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M32">
         <v>2000</v>
@@ -2358,10 +2349,10 @@
         <v>100</v>
       </c>
       <c r="O32" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q32">
         <v>3000000</v>
@@ -2372,37 +2363,37 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D33">
         <v>126</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F33">
         <v>126</v>
       </c>
       <c r="G33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="K33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="L33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M33">
         <v>1800</v>
@@ -2411,172 +2402,13 @@
         <v>100</v>
       </c>
       <c r="O33" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="P33" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q33">
         <v>4550000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34">
-        <v>249.6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34">
-        <v>249.6</v>
-      </c>
-      <c r="G34" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" t="s">
-        <v>77</v>
-      </c>
-      <c r="I34" t="s">
-        <v>77</v>
-      </c>
-      <c r="J34" t="s">
-        <v>77</v>
-      </c>
-      <c r="K34" t="s">
-        <v>79</v>
-      </c>
-      <c r="L34" t="s">
-        <v>77</v>
-      </c>
-      <c r="M34">
-        <v>4800</v>
-      </c>
-      <c r="N34">
-        <v>100</v>
-      </c>
-      <c r="O34" t="s">
-        <v>88</v>
-      </c>
-      <c r="P34" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q34">
-        <v>3900000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
-      <c r="A35" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35">
-        <v>463.5</v>
-      </c>
-      <c r="E35" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35">
-        <v>463.5</v>
-      </c>
-      <c r="G35" t="s">
-        <v>77</v>
-      </c>
-      <c r="H35" t="s">
-        <v>77</v>
-      </c>
-      <c r="I35" t="s">
-        <v>77</v>
-      </c>
-      <c r="J35" t="s">
-        <v>77</v>
-      </c>
-      <c r="K35" t="s">
-        <v>79</v>
-      </c>
-      <c r="L35" t="s">
-        <v>77</v>
-      </c>
-      <c r="M35">
-        <v>22500</v>
-      </c>
-      <c r="N35">
-        <v>100</v>
-      </c>
-      <c r="O35" t="s">
-        <v>88</v>
-      </c>
-      <c r="P35" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q35">
-        <v>1545000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-      <c r="D36">
-        <v>156</v>
-      </c>
-      <c r="E36" t="s">
-        <v>66</v>
-      </c>
-      <c r="F36">
-        <v>156</v>
-      </c>
-      <c r="G36" t="s">
-        <v>77</v>
-      </c>
-      <c r="H36" t="s">
-        <v>77</v>
-      </c>
-      <c r="I36" t="s">
-        <v>77</v>
-      </c>
-      <c r="J36" t="s">
-        <v>77</v>
-      </c>
-      <c r="K36" t="s">
-        <v>79</v>
-      </c>
-      <c r="L36" t="s">
-        <v>77</v>
-      </c>
-      <c r="M36">
-        <v>13000</v>
-      </c>
-      <c r="N36">
-        <v>100</v>
-      </c>
-      <c r="O36" t="s">
-        <v>88</v>
-      </c>
-      <c r="P36" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q36">
-        <v>840000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-01-06
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="91">
   <si>
     <t>상장일</t>
   </si>
@@ -115,184 +115,172 @@
     <t>2023-11-13</t>
   </si>
   <si>
+    <t>DS단석</t>
+  </si>
+  <si>
+    <t>하나30호스팩</t>
+  </si>
+  <si>
+    <t>IBKS제23호스팩</t>
+  </si>
+  <si>
+    <t>LS머트리얼즈</t>
+  </si>
+  <si>
+    <t>블루엠텍</t>
+  </si>
+  <si>
+    <t>교보15호스팩</t>
+  </si>
+  <si>
+    <t>케이엔에스</t>
+  </si>
+  <si>
+    <t>와이바이오로직스</t>
+  </si>
+  <si>
+    <t>삼성스팩9호</t>
+  </si>
+  <si>
+    <t>에이텀</t>
+  </si>
+  <si>
+    <t>엔에이치스팩30호</t>
+  </si>
+  <si>
+    <t>에이에스텍</t>
+  </si>
+  <si>
+    <t>그린리소스</t>
+  </si>
+  <si>
+    <t>스톰테크</t>
+  </si>
+  <si>
+    <t>한선엔지니어링</t>
+  </si>
+  <si>
+    <t>에코아이</t>
+  </si>
+  <si>
+    <t>동인기연</t>
+  </si>
+  <si>
+    <t>에코프로머티</t>
+  </si>
+  <si>
+    <t>캡스톤파트너스</t>
+  </si>
+  <si>
+    <t>큐로셀</t>
+  </si>
+  <si>
+    <t>에이직랜드</t>
+  </si>
+  <si>
+    <t>코스피</t>
+  </si>
+  <si>
+    <t>코스닥</t>
+  </si>
+  <si>
+    <t>KB</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>하나</t>
+  </si>
+  <si>
+    <t>IBK</t>
+  </si>
+  <si>
+    <t>키움</t>
+  </si>
+  <si>
+    <t>이베스트</t>
+  </si>
+  <si>
+    <t>하이</t>
+  </si>
+  <si>
+    <t>교보</t>
+  </si>
+  <si>
+    <t>신영</t>
+  </si>
+  <si>
+    <t>유안타</t>
+  </si>
+  <si>
+    <t>삼성</t>
+  </si>
+  <si>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>대신</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>공동대표</t>
+  </si>
+  <si>
+    <t>대표</t>
+  </si>
+  <si>
+    <t>인수</t>
+  </si>
+  <si>
+    <t>공동</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-10</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>2023-11-02</t>
+  </si>
+  <si>
+    <t>2023-12-19</t>
+  </si>
+  <si>
+    <t>2023-12-18</t>
+  </si>
+  <si>
+    <t>2023-12-15</t>
+  </si>
+  <si>
+    <t>2023-12-07</t>
+  </si>
+  <si>
+    <t>2023-11-30</t>
+  </si>
+  <si>
     <t>2023-11-14</t>
-  </si>
-  <si>
-    <t>DS단석</t>
-  </si>
-  <si>
-    <t>하나30호스팩</t>
-  </si>
-  <si>
-    <t>IBKS제23호스팩</t>
-  </si>
-  <si>
-    <t>LS머트리얼즈</t>
-  </si>
-  <si>
-    <t>블루엠텍</t>
-  </si>
-  <si>
-    <t>교보15호스팩</t>
-  </si>
-  <si>
-    <t>케이엔에스</t>
-  </si>
-  <si>
-    <t>와이바이오로직스</t>
-  </si>
-  <si>
-    <t>삼성스팩9호</t>
-  </si>
-  <si>
-    <t>에이텀</t>
-  </si>
-  <si>
-    <t>엔에이치스팩30호</t>
-  </si>
-  <si>
-    <t>에이에스텍</t>
-  </si>
-  <si>
-    <t>그린리소스</t>
-  </si>
-  <si>
-    <t>스톰테크</t>
-  </si>
-  <si>
-    <t>한선엔지니어링</t>
-  </si>
-  <si>
-    <t>에코아이</t>
-  </si>
-  <si>
-    <t>동인기연</t>
-  </si>
-  <si>
-    <t>에코프로머티</t>
-  </si>
-  <si>
-    <t>캡스톤파트너스</t>
-  </si>
-  <si>
-    <t>큐로셀</t>
-  </si>
-  <si>
-    <t>에이직랜드</t>
-  </si>
-  <si>
-    <t>한국제13호스팩</t>
-  </si>
-  <si>
-    <t>에스와이스틸텍</t>
-  </si>
-  <si>
-    <t>코스피</t>
-  </si>
-  <si>
-    <t>코스닥</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
-    <t>NH</t>
-  </si>
-  <si>
-    <t>하나</t>
-  </si>
-  <si>
-    <t>IBK</t>
-  </si>
-  <si>
-    <t>키움</t>
-  </si>
-  <si>
-    <t>이베스트</t>
-  </si>
-  <si>
-    <t>하이</t>
-  </si>
-  <si>
-    <t>교보</t>
-  </si>
-  <si>
-    <t>신영</t>
-  </si>
-  <si>
-    <t>유안타</t>
-  </si>
-  <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
-    <t>대신</t>
-  </si>
-  <si>
-    <t>한국</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>공동대표</t>
-  </si>
-  <si>
-    <t>대표</t>
-  </si>
-  <si>
-    <t>인수</t>
-  </si>
-  <si>
-    <t>공동</t>
-  </si>
-  <si>
-    <t>2023-12-14</t>
-  </si>
-  <si>
-    <t>2023-11-23</t>
-  </si>
-  <si>
-    <t>2023-11-27</t>
-  </si>
-  <si>
-    <t>2023-11-16</t>
-  </si>
-  <si>
-    <t>2023-11-10</t>
-  </si>
-  <si>
-    <t>2023-11-08</t>
-  </si>
-  <si>
-    <t>2023-11-06</t>
-  </si>
-  <si>
-    <t>2023-10-31</t>
-  </si>
-  <si>
-    <t>2023-11-02</t>
-  </si>
-  <si>
-    <t>2023-11-01</t>
-  </si>
-  <si>
-    <t>2023-12-19</t>
-  </si>
-  <si>
-    <t>2023-12-18</t>
-  </si>
-  <si>
-    <t>2023-12-15</t>
-  </si>
-  <si>
-    <t>2023-12-07</t>
-  </si>
-  <si>
-    <t>2023-11-30</t>
   </si>
   <si>
     <t>2023-11-03</t>
@@ -656,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -720,37 +708,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>1220</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F2">
         <v>793</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M2">
         <v>100000</v>
@@ -759,10 +747,10 @@
         <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Q2">
         <v>1830000</v>
@@ -773,37 +761,37 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>1220</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F3">
         <v>427</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M3">
         <v>100000</v>
@@ -812,10 +800,10 @@
         <v>35</v>
       </c>
       <c r="O3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="Q3">
         <v>1830000</v>
@@ -826,37 +814,37 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F4">
         <v>140</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M4">
         <v>2000</v>
@@ -868,7 +856,7 @@
         <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="Q4">
         <v>5250000</v>
@@ -879,37 +867,37 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F5">
         <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -921,7 +909,7 @@
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="Q5">
         <v>3000000</v>
@@ -932,37 +920,37 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>877.5</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6">
         <v>361.96872</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M6">
         <v>6000</v>
@@ -985,37 +973,37 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>877.5</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F7">
         <v>361.96872</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M7">
         <v>6000</v>
@@ -1038,37 +1026,37 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>877.5</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F8">
         <v>65.81256</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M8">
         <v>6000</v>
@@ -1091,37 +1079,37 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>877.5</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F9">
         <v>43.875</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M9">
         <v>6000</v>
@@ -1144,37 +1132,37 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D10">
         <v>877.5</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F10">
         <v>43.875</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M10">
         <v>6000</v>
@@ -1197,37 +1185,37 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D11">
         <v>266</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>186.2</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M11">
         <v>19000</v>
@@ -1239,7 +1227,7 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Q11">
         <v>2100000</v>
@@ -1250,37 +1238,37 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12">
         <v>266</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F12">
         <v>79.8</v>
       </c>
       <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="s">
         <v>73</v>
       </c>
-      <c r="H12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" t="s">
-        <v>77</v>
-      </c>
       <c r="L12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M12">
         <v>19000</v>
@@ -1292,7 +1280,7 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="Q12">
         <v>2100000</v>
@@ -1303,37 +1291,37 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D13">
         <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13">
         <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M13">
         <v>2000</v>
@@ -1342,7 +1330,7 @@
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
         <v>24</v>
@@ -1356,37 +1344,37 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D14">
         <v>172.5</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F14">
         <v>172.5</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M14">
         <v>23000</v>
@@ -1395,10 +1383,10 @@
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="P14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="Q14">
         <v>475800</v>
@@ -1409,37 +1397,37 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D15">
         <v>135</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F15">
         <v>135</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M15">
         <v>9000</v>
@@ -1448,7 +1436,7 @@
         <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P15" t="s">
         <v>24</v>
@@ -1462,37 +1450,37 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D16">
         <v>200</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F16">
         <v>200</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1501,7 +1489,7 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P16" t="s">
         <v>24</v>
@@ -1515,37 +1503,37 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D17">
         <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F17">
         <v>117</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M17">
         <v>18000</v>
@@ -1568,37 +1556,37 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D18">
         <v>160</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F18">
         <v>160</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1621,37 +1609,37 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D19">
         <v>393.96</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F19">
         <v>393.96</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M19">
         <v>28000</v>
@@ -1660,7 +1648,7 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
@@ -1674,37 +1662,37 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D20">
         <v>278.8</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F20">
         <v>278.8</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M20">
         <v>17000</v>
@@ -1716,7 +1704,7 @@
         <v>32</v>
       </c>
       <c r="P20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q20">
         <v>1221420</v>
@@ -1727,37 +1715,37 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D21">
         <v>368.5</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F21">
         <v>368.5</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M21">
         <v>11000</v>
@@ -1769,7 +1757,7 @@
         <v>31</v>
       </c>
       <c r="P21" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="Q21">
         <v>2374500</v>
@@ -1780,37 +1768,37 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D22">
         <v>297.5</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F22">
         <v>297.5</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M22">
         <v>7000</v>
@@ -1822,7 +1810,7 @@
         <v>32</v>
       </c>
       <c r="P22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="Q22">
         <v>3187500</v>
@@ -1833,37 +1821,37 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D23">
         <v>721.413</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F23">
         <v>721.413</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M23">
         <v>34700</v>
@@ -1872,7 +1860,7 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -1886,37 +1874,37 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D24">
         <v>441.12</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F24">
         <v>441.12</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M24">
         <v>30000</v>
@@ -1928,7 +1916,7 @@
         <v>31</v>
       </c>
       <c r="P24" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="Q24">
         <v>1072999</v>
@@ -1939,37 +1927,37 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D25">
         <v>4192.2496</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F25">
         <v>2846.537406</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M25">
         <v>36200</v>
@@ -1978,7 +1966,7 @@
         <v>67.90000000000001</v>
       </c>
       <c r="O25" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P25" t="s">
         <v>32</v>
@@ -1992,37 +1980,37 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26">
         <v>4192.2496</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F26">
         <v>1219.944706</v>
       </c>
       <c r="G26" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I26" t="s">
+        <v>69</v>
+      </c>
+      <c r="J26" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" t="s">
         <v>73</v>
       </c>
-      <c r="H26" t="s">
-        <v>73</v>
-      </c>
-      <c r="I26" t="s">
-        <v>73</v>
-      </c>
-      <c r="J26" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" t="s">
-        <v>77</v>
-      </c>
       <c r="L26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M26">
         <v>36200</v>
@@ -2031,7 +2019,7 @@
         <v>29.1</v>
       </c>
       <c r="O26" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P26" t="s">
         <v>32</v>
@@ -2045,37 +2033,37 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D27">
         <v>4192.2496</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F27">
         <v>125.767488</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M27">
         <v>36200</v>
@@ -2084,7 +2072,7 @@
         <v>3</v>
       </c>
       <c r="O27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="P27" t="s">
         <v>32</v>
@@ -2098,37 +2086,37 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D28">
         <v>63.84</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F28">
         <v>63.84</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M28">
         <v>4000</v>
@@ -2137,7 +2125,7 @@
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="P28" t="s">
         <v>31</v>
@@ -2151,37 +2139,37 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D29">
         <v>320</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F29">
         <v>160</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M29">
         <v>20000</v>
@@ -2190,10 +2178,10 @@
         <v>50</v>
       </c>
       <c r="O29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P29" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Q29">
         <v>2254770</v>
@@ -2204,37 +2192,37 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30">
         <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F30">
         <v>160</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M30">
         <v>20000</v>
@@ -2243,10 +2231,10 @@
         <v>50</v>
       </c>
       <c r="O30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="P30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Q30">
         <v>2254770</v>
@@ -2257,37 +2245,37 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D31">
         <v>659.0825</v>
       </c>
       <c r="E31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F31">
         <v>659.0825</v>
       </c>
       <c r="G31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="J31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="K31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="L31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M31">
         <v>25000</v>
@@ -2296,119 +2284,13 @@
         <v>100</v>
       </c>
       <c r="O31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="P31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="Q31">
         <v>1827247</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32">
-        <v>80</v>
-      </c>
-      <c r="E32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32">
-        <v>80</v>
-      </c>
-      <c r="G32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H32" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" t="s">
-        <v>73</v>
-      </c>
-      <c r="J32" t="s">
-        <v>73</v>
-      </c>
-      <c r="K32" t="s">
-        <v>75</v>
-      </c>
-      <c r="L32" t="s">
-        <v>73</v>
-      </c>
-      <c r="M32">
-        <v>2000</v>
-      </c>
-      <c r="N32">
-        <v>100</v>
-      </c>
-      <c r="O32" t="s">
-        <v>87</v>
-      </c>
-      <c r="P32" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q32">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" t="s">
-        <v>58</v>
-      </c>
-      <c r="D33">
-        <v>126</v>
-      </c>
-      <c r="E33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F33">
-        <v>126</v>
-      </c>
-      <c r="G33" t="s">
-        <v>73</v>
-      </c>
-      <c r="H33" t="s">
-        <v>73</v>
-      </c>
-      <c r="I33" t="s">
-        <v>73</v>
-      </c>
-      <c r="J33" t="s">
-        <v>73</v>
-      </c>
-      <c r="K33" t="s">
-        <v>75</v>
-      </c>
-      <c r="L33" t="s">
-        <v>73</v>
-      </c>
-      <c r="M33">
-        <v>1800</v>
-      </c>
-      <c r="N33">
-        <v>100</v>
-      </c>
-      <c r="O33" t="s">
-        <v>87</v>
-      </c>
-      <c r="P33" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q33">
-        <v>4550000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-16
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="88">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-07-15</t>
+  </si>
+  <si>
     <t>2024-07-11</t>
   </si>
   <si>
@@ -118,6 +121,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>엑셀세라퓨틱스</t>
+  </si>
+  <si>
     <t>시프트업</t>
   </si>
   <si>
@@ -181,10 +187,13 @@
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
+    <t>코스닥</t>
+  </si>
+  <si>
     <t>코스피</t>
   </si>
   <si>
-    <t>코스닥</t>
+    <t>대신</t>
   </si>
   <si>
     <t>한국</t>
@@ -220,9 +229,6 @@
     <t>IBK</t>
   </si>
   <si>
-    <t>대신</t>
-  </si>
-  <si>
     <t>DB</t>
   </si>
   <si>
@@ -260,6 +266,9 @@
   </si>
   <si>
     <t>2024-05-13</t>
+  </si>
+  <si>
+    <t>2024-07-08</t>
   </si>
   <si>
     <t>2024-07-05</t>
@@ -626,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -690,90 +699,90 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>4350</v>
+        <v>161.8</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F2">
-        <v>1435.5</v>
+        <v>161.8</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M2">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="N2">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
         <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q2">
-        <v>21750000</v>
+        <v>1187900</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>4350</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3">
         <v>1435.5</v>
       </c>
       <c r="G3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M3">
         <v>60000</v>
@@ -782,10 +791,10 @@
         <v>33</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q3">
         <v>21750000</v>
@@ -793,52 +802,52 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>4350</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F4">
-        <v>1305</v>
+        <v>1435.5</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M4">
         <v>60000</v>
       </c>
       <c r="N4">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q4">
         <v>21750000</v>
@@ -846,52 +855,52 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>4350</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F5">
-        <v>174</v>
+        <v>1305</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M5">
         <v>60000</v>
       </c>
       <c r="N5">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q5">
         <v>21750000</v>
@@ -902,52 +911,52 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D6">
-        <v>80</v>
+        <v>4350</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F6">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K6" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L6" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M6">
-        <v>2000</v>
+        <v>60000</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="O6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q6">
-        <v>3000000</v>
+        <v>21750000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -955,52 +964,52 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7">
-        <v>289.6</v>
+        <v>80</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F7">
-        <v>289.6</v>
+        <v>80</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M7">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N7">
         <v>100</v>
       </c>
       <c r="O7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P7" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
       <c r="Q7">
-        <v>1357500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1008,102 +1017,102 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8">
-        <v>575.89</v>
+        <v>289.6</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F8">
-        <v>541.3366</v>
+        <v>289.6</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M8">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N8">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O8" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q8">
-        <v>1906400</v>
+        <v>1357500</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>575.89</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F9">
-        <v>34.5534</v>
+        <v>541.3366</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M9">
         <v>43300</v>
       </c>
       <c r="N9">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="O9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q9">
         <v>1906400</v>
@@ -1114,52 +1123,52 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10">
-        <v>432</v>
+        <v>575.89</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F10">
-        <v>432</v>
+        <v>34.5534</v>
       </c>
       <c r="G10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K10" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M10">
-        <v>18000</v>
+        <v>43300</v>
       </c>
       <c r="N10">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="O10" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="P10" t="s">
         <v>25</v>
       </c>
       <c r="Q10">
-        <v>1758600</v>
+        <v>1906400</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1167,52 +1176,52 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D11">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F11">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="G11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M11">
-        <v>7000</v>
+        <v>18000</v>
       </c>
       <c r="N11">
         <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="P11" t="s">
         <v>26</v>
       </c>
       <c r="Q11">
-        <v>2350000</v>
+        <v>1758600</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1220,52 +1229,52 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D12">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F12">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="G12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M12">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P12" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="Q12">
-        <v>4687500</v>
+        <v>2350000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1273,102 +1282,102 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13">
-        <v>230</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F13">
-        <v>218.5</v>
+        <v>125</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M13">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N13">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P13" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="Q13">
-        <v>3000000</v>
+        <v>4687500</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D14">
         <v>230</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F14">
-        <v>11.5</v>
+        <v>218.5</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M14">
         <v>11500</v>
       </c>
       <c r="N14">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="O14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q14">
         <v>3000000</v>
@@ -1379,52 +1388,52 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15">
-        <v>129</v>
+        <v>230</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F15">
-        <v>129</v>
+        <v>11.5</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L15" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N15">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O15" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="P15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q15">
-        <v>4837500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1432,37 +1441,37 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D16">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F16">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M16">
         <v>2000</v>
@@ -1471,51 +1480,51 @@
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="P16" t="s">
         <v>30</v>
       </c>
       <c r="Q16">
-        <v>4500000</v>
+        <v>4837500</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D17">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F17">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M17">
         <v>2000</v>
@@ -1524,51 +1533,51 @@
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="P17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q17">
-        <v>5250000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F18">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1577,51 +1586,51 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P18" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="Q18">
-        <v>3000000</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F19">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M19">
         <v>2000</v>
@@ -1630,172 +1639,172 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
+        <v>79</v>
+      </c>
+      <c r="P19" t="s">
         <v>77</v>
       </c>
-      <c r="P19" t="s">
-        <v>75</v>
-      </c>
       <c r="Q19">
-        <v>3562500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D20">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="E20" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F20">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M20">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N20">
         <v>100</v>
       </c>
       <c r="O20" t="s">
+        <v>79</v>
+      </c>
+      <c r="P20" t="s">
         <v>77</v>
       </c>
-      <c r="P20" t="s">
-        <v>75</v>
-      </c>
       <c r="Q20">
-        <v>975000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D21">
-        <v>480</v>
+        <v>221</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="F21">
-        <v>480</v>
+        <v>221</v>
       </c>
       <c r="G21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M21">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N21">
         <v>100</v>
       </c>
       <c r="O21" t="s">
+        <v>79</v>
+      </c>
+      <c r="P21" t="s">
         <v>77</v>
       </c>
-      <c r="P21" t="s">
-        <v>75</v>
-      </c>
       <c r="Q21">
-        <v>1123925</v>
+        <v>975000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D22">
-        <v>207.68</v>
+        <v>480</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F22">
-        <v>207.68</v>
+        <v>480</v>
       </c>
       <c r="G22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L22" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M22">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Q22">
-        <v>957220</v>
+        <v>1123925</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1803,52 +1812,52 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D23">
-        <v>100</v>
+        <v>207.68</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F23">
-        <v>100</v>
+        <v>207.68</v>
       </c>
       <c r="G23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M23">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
+        <v>80</v>
+      </c>
+      <c r="P23" t="s">
         <v>78</v>
       </c>
-      <c r="P23" t="s">
-        <v>76</v>
-      </c>
       <c r="Q23">
-        <v>3750000</v>
+        <v>957220</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1856,52 +1865,52 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F24">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L24" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M24">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P24" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="Q24">
-        <v>1050000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1909,52 +1918,52 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D25">
-        <v>133</v>
+        <v>560</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F25">
-        <v>133</v>
+        <v>560</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M25">
-        <v>2000</v>
+        <v>40000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P25" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="Q25">
-        <v>4987500</v>
+        <v>1050000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1962,52 +1971,52 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F26">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="G26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M26">
-        <v>14000</v>
+        <v>2000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P26" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="Q26">
-        <v>900000</v>
+        <v>4987500</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2015,90 +2024,90 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D27">
-        <v>700.0000199999999</v>
+        <v>168</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F27">
-        <v>350.00001</v>
+        <v>168</v>
       </c>
       <c r="G27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K27" t="s">
         <v>73</v>
       </c>
       <c r="L27" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M27">
-        <v>3000</v>
+        <v>14000</v>
       </c>
       <c r="N27">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="P27" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="Q27">
-        <v>32666668</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>700.0000199999999</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F28">
         <v>350.00001</v>
       </c>
       <c r="G28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L28" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="M28">
         <v>3000</v>
@@ -2107,12 +2116,65 @@
         <v>50</v>
       </c>
       <c r="O28" t="s">
+        <v>77</v>
+      </c>
+      <c r="P28" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q28">
+        <v>32666668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29">
+        <v>700.0000199999999</v>
+      </c>
+      <c r="E29" t="s">
+        <v>60</v>
+      </c>
+      <c r="F29">
+        <v>350.00001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" t="s">
         <v>75</v>
       </c>
-      <c r="P28" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q28">
+      <c r="L29" t="s">
+        <v>72</v>
+      </c>
+      <c r="M29">
+        <v>3000</v>
+      </c>
+      <c r="N29">
+        <v>50</v>
+      </c>
+      <c r="O29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P29" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q29">
         <v>32666668</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-27
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="89">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-07-26</t>
+  </si>
+  <si>
     <t>2024-07-25</t>
   </si>
   <si>
@@ -118,6 +121,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>엔에이치스팩31호</t>
+  </si>
+  <si>
     <t>SK증권제13호스팩</t>
   </si>
   <si>
@@ -187,6 +193,9 @@
     <t>코스피</t>
   </si>
   <si>
+    <t>NH</t>
+  </si>
+  <si>
     <t>SK</t>
   </si>
   <si>
@@ -199,9 +208,6 @@
     <t>제이피모간회사</t>
   </si>
   <si>
-    <t>NH</t>
-  </si>
-  <si>
     <t>신한</t>
   </si>
   <si>
@@ -241,6 +247,9 @@
     <t>공동대표</t>
   </si>
   <si>
+    <t>2024-07-16</t>
+  </si>
+  <si>
     <t>2024-06-20</t>
   </si>
   <si>
@@ -257,6 +266,9 @@
   </si>
   <si>
     <t>2024-06-03</t>
+  </si>
+  <si>
+    <t>2024-07-19</t>
   </si>
   <si>
     <t>2024-07-18</t>
@@ -626,7 +638,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -690,37 +702,37 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F2">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M2">
         <v>2000</v>
@@ -729,13 +741,13 @@
         <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="Q2">
-        <v>3000000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -743,52 +755,52 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D3">
-        <v>161.8</v>
+        <v>80</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F3">
-        <v>161.8</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M3">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
         <v>100</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="Q3">
-        <v>1187900</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -796,90 +808,90 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D4">
-        <v>4350</v>
+        <v>161.8</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F4">
-        <v>1435.5</v>
+        <v>161.8</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M4">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="N4">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="O4" t="s">
         <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q4">
-        <v>21750000</v>
+        <v>1187900</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D5">
         <v>4350</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F5">
         <v>1435.5</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M5">
         <v>60000</v>
@@ -888,10 +900,10 @@
         <v>33</v>
       </c>
       <c r="O5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q5">
         <v>21750000</v>
@@ -899,52 +911,52 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>4350</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F6">
-        <v>1305</v>
+        <v>1435.5</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M6">
         <v>60000</v>
       </c>
       <c r="N6">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q6">
         <v>21750000</v>
@@ -952,52 +964,52 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7">
         <v>4350</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F7">
-        <v>174</v>
+        <v>1305</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M7">
         <v>60000</v>
       </c>
       <c r="N7">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="O7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q7">
         <v>21750000</v>
@@ -1008,52 +1020,52 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D8">
-        <v>80</v>
+        <v>4350</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F8">
-        <v>80</v>
+        <v>174</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M8">
-        <v>2000</v>
+        <v>60000</v>
       </c>
       <c r="N8">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="O8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q8">
-        <v>3000000</v>
+        <v>21750000</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1061,52 +1073,52 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D9">
-        <v>289.6</v>
+        <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F9">
-        <v>289.6</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M9">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N9">
         <v>100</v>
       </c>
       <c r="O9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="Q9">
-        <v>1357500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1114,102 +1126,102 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D10">
-        <v>575.89</v>
+        <v>289.6</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10">
-        <v>541.3366</v>
+        <v>289.6</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M10">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N10">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O10" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="P10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q10">
-        <v>1906400</v>
+        <v>1357500</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D11">
         <v>575.89</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F11">
-        <v>34.5534</v>
+        <v>541.3366</v>
       </c>
       <c r="G11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M11">
         <v>43300</v>
       </c>
       <c r="N11">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="O11" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="P11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q11">
         <v>1906400</v>
@@ -1220,52 +1232,52 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D12">
-        <v>432</v>
+        <v>575.89</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F12">
-        <v>432</v>
+        <v>34.5534</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M12">
-        <v>18000</v>
+        <v>43300</v>
       </c>
       <c r="N12">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="O12" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="P12" t="s">
         <v>27</v>
       </c>
       <c r="Q12">
-        <v>1758600</v>
+        <v>1906400</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1273,52 +1285,52 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D13">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
       </c>
       <c r="F13">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M13">
-        <v>7000</v>
+        <v>18000</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13" t="s">
         <v>28</v>
       </c>
       <c r="Q13">
-        <v>2350000</v>
+        <v>1758600</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1326,52 +1338,52 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F14">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L14" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M14">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N14">
         <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P14" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="Q14">
-        <v>4687500</v>
+        <v>2350000</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1379,102 +1391,102 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D15">
-        <v>230</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F15">
-        <v>218.5</v>
+        <v>125</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L15" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M15">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N15">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P15" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="Q15">
-        <v>3000000</v>
+        <v>4687500</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D16">
         <v>230</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F16">
-        <v>11.5</v>
+        <v>218.5</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L16" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M16">
         <v>11500</v>
       </c>
       <c r="N16">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="O16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q16">
         <v>3000000</v>
@@ -1485,52 +1497,52 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D17">
-        <v>129</v>
+        <v>230</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F17">
-        <v>129</v>
+        <v>11.5</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N17">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O17" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="P17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q17">
-        <v>4837500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1538,37 +1550,37 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D18">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
         <v>67</v>
       </c>
       <c r="F18">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L18" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M18">
         <v>2000</v>
@@ -1577,51 +1589,51 @@
         <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P18" t="s">
         <v>32</v>
       </c>
       <c r="Q18">
-        <v>4500000</v>
+        <v>4837500</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D19">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F19">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M19">
         <v>2000</v>
@@ -1630,51 +1642,51 @@
         <v>100</v>
       </c>
       <c r="O19" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q19">
-        <v>5250000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D20">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K20" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L20" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1683,51 +1695,51 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="P20" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="Q20">
-        <v>3000000</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D21">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F21">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1736,172 +1748,172 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q21">
-        <v>3562500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D22">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F22">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L22" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M22">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N22">
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q22">
-        <v>975000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D23">
-        <v>480</v>
+        <v>221</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F23">
-        <v>480</v>
+        <v>221</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M23">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Q23">
-        <v>1123925</v>
+        <v>975000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D24">
-        <v>207.68</v>
+        <v>480</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F24">
-        <v>207.68</v>
+        <v>480</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M24">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
+        <v>81</v>
+      </c>
+      <c r="P24" t="s">
         <v>79</v>
       </c>
-      <c r="P24" t="s">
-        <v>77</v>
-      </c>
       <c r="Q24">
-        <v>957220</v>
+        <v>1123925</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1909,52 +1921,52 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D25">
-        <v>100</v>
+        <v>207.68</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F25">
-        <v>100</v>
+        <v>207.68</v>
       </c>
       <c r="G25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L25" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M25">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="P25" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="Q25">
-        <v>3750000</v>
+        <v>957220</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1962,52 +1974,52 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D26">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="F26">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K26" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L26" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M26">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
+        <v>82</v>
+      </c>
+      <c r="P26" t="s">
         <v>80</v>
       </c>
-      <c r="P26" t="s">
-        <v>84</v>
-      </c>
       <c r="Q26">
-        <v>1050000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2015,90 +2027,90 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27">
-        <v>700.0000199999999</v>
+        <v>560</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F27">
-        <v>350.00001</v>
+        <v>560</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K27" t="s">
         <v>74</v>
       </c>
       <c r="L27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M27">
-        <v>3000</v>
+        <v>40000</v>
       </c>
       <c r="N27">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="P27" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="Q27">
-        <v>32666668</v>
+        <v>1050000</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>700.0000199999999</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F28">
         <v>350.00001</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M28">
         <v>3000</v>
@@ -2107,12 +2119,65 @@
         <v>50</v>
       </c>
       <c r="O28" t="s">
+        <v>79</v>
+      </c>
+      <c r="P28" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q28">
+        <v>32666668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29">
+        <v>700.0000199999999</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29">
+        <v>350.00001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" t="s">
         <v>76</v>
       </c>
-      <c r="P28" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q28">
+      <c r="L29" t="s">
+        <v>73</v>
+      </c>
+      <c r="M29">
+        <v>3000</v>
+      </c>
+      <c r="N29">
+        <v>50</v>
+      </c>
+      <c r="O29" t="s">
+        <v>79</v>
+      </c>
+      <c r="P29" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q29">
         <v>32666668</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-07-30
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="92">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-07-29</t>
+  </si>
+  <si>
     <t>2024-07-26</t>
   </si>
   <si>
@@ -121,6 +124,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>산일전기</t>
+  </si>
+  <si>
     <t>엔에이치스팩31호</t>
   </si>
   <si>
@@ -187,10 +193,16 @@
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
+    <t>코스피</t>
+  </si>
+  <si>
     <t>코스닥</t>
   </si>
   <si>
-    <t>코스피</t>
+    <t>미래</t>
+  </si>
+  <si>
+    <t>삼성</t>
   </si>
   <si>
     <t>NH</t>
@@ -214,12 +226,6 @@
     <t>LS</t>
   </si>
   <si>
-    <t>삼성</t>
-  </si>
-  <si>
-    <t>미래</t>
-  </si>
-  <si>
     <t>BNK</t>
   </si>
   <si>
@@ -247,6 +253,9 @@
     <t>공동대표</t>
   </si>
   <si>
+    <t>2024-07-18</t>
+  </si>
+  <si>
     <t>2024-07-16</t>
   </si>
   <si>
@@ -268,10 +277,10 @@
     <t>2024-06-03</t>
   </si>
   <si>
+    <t>2024-07-23</t>
+  </si>
+  <si>
     <t>2024-07-19</t>
-  </si>
-  <si>
-    <t>2024-07-18</t>
   </si>
   <si>
     <t>2024-07-08</t>
@@ -638,7 +647,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -702,211 +711,211 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>2660</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F2">
-        <v>120</v>
+        <v>2553.6</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M2">
-        <v>2000</v>
+        <v>35000</v>
       </c>
       <c r="N2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="O2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Q2">
-        <v>4500000</v>
+        <v>9340690</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D3">
-        <v>80</v>
+        <v>2660</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F3">
-        <v>80</v>
+        <v>106.4</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M3">
-        <v>2000</v>
+        <v>35000</v>
       </c>
       <c r="N3">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="P3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="Q3">
-        <v>3000000</v>
+        <v>9340690</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D4">
-        <v>161.8</v>
+        <v>120</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F4">
-        <v>161.8</v>
+        <v>120</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M4">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N4">
         <v>100</v>
       </c>
       <c r="O4" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="P4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="Q4">
-        <v>1187900</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>4350</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F5">
-        <v>1435.5</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M5">
-        <v>60000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="P5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="Q5">
-        <v>21750000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -914,102 +923,102 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D6">
-        <v>4350</v>
+        <v>161.8</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F6">
-        <v>1435.5</v>
+        <v>161.8</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M6">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="N6">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="O6" t="s">
         <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="Q6">
-        <v>21750000</v>
+        <v>1187900</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7">
         <v>4350</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F7">
-        <v>1305</v>
+        <v>1435.5</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M7">
         <v>60000</v>
       </c>
       <c r="N7">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Q7">
         <v>21750000</v>
@@ -1017,52 +1026,52 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D8">
         <v>4350</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F8">
-        <v>174</v>
+        <v>1435.5</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M8">
         <v>60000</v>
       </c>
       <c r="N8">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Q8">
         <v>21750000</v>
@@ -1073,158 +1082,158 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D9">
-        <v>80</v>
+        <v>4350</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9">
-        <v>80</v>
+        <v>1305</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M9">
-        <v>2000</v>
+        <v>60000</v>
       </c>
       <c r="N9">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="O9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Q9">
-        <v>3000000</v>
+        <v>21750000</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10">
-        <v>289.6</v>
+        <v>4350</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F10">
-        <v>289.6</v>
+        <v>174</v>
       </c>
       <c r="G10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K10" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M10">
-        <v>16000</v>
+        <v>60000</v>
       </c>
       <c r="N10">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="Q10">
-        <v>1357500</v>
+        <v>21750000</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D11">
-        <v>575.89</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F11">
-        <v>541.3366</v>
+        <v>80</v>
       </c>
       <c r="G11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M11">
-        <v>43300</v>
+        <v>2000</v>
       </c>
       <c r="N11">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O11" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="Q11">
-        <v>1906400</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1232,52 +1241,52 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D12">
-        <v>575.89</v>
+        <v>289.6</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12">
-        <v>34.5534</v>
+        <v>289.6</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L12" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M12">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N12">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="P12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q12">
-        <v>1906400</v>
+        <v>1357500</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1285,146 +1294,146 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D13">
-        <v>432</v>
+        <v>575.89</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F13">
-        <v>432</v>
+        <v>541.3366</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M13">
-        <v>18000</v>
+        <v>43300</v>
       </c>
       <c r="N13">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="O13" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="P13" t="s">
         <v>28</v>
       </c>
       <c r="Q13">
-        <v>1758600</v>
+        <v>1906400</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>238</v>
+        <v>575.89</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F14">
-        <v>238</v>
+        <v>34.5534</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M14">
-        <v>7000</v>
+        <v>43300</v>
       </c>
       <c r="N14">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="O14" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="P14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q14">
-        <v>2350000</v>
+        <v>1906400</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>125</v>
+        <v>432</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15">
-        <v>125</v>
+        <v>432</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M15">
-        <v>2000</v>
+        <v>18000</v>
       </c>
       <c r="N15">
         <v>100</v>
@@ -1433,54 +1442,54 @@
         <v>31</v>
       </c>
       <c r="P15" t="s">
-        <v>78</v>
+        <v>29</v>
       </c>
       <c r="Q15">
-        <v>4687500</v>
+        <v>1758600</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D16">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F16">
-        <v>218.5</v>
+        <v>238</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M16">
-        <v>11500</v>
+        <v>7000</v>
       </c>
       <c r="N16">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O16" t="s">
         <v>33</v>
@@ -1489,7 +1498,7 @@
         <v>30</v>
       </c>
       <c r="Q16">
-        <v>3000000</v>
+        <v>2350000</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1497,52 +1506,52 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>230</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17">
-        <v>11.5</v>
+        <v>125</v>
       </c>
       <c r="G17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M17">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N17">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P17" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="Q17">
-        <v>3000000</v>
+        <v>4687500</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1550,143 +1559,143 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D18">
-        <v>129</v>
+        <v>230</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18">
-        <v>129</v>
+        <v>218.5</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K18" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L18" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M18">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N18">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O18" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="P18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q18">
-        <v>4837500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D19">
-        <v>120</v>
+        <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F19">
-        <v>120</v>
+        <v>11.5</v>
       </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="L19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M19">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N19">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O19" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="P19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q19">
-        <v>4500000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D20">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F20">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L20" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M20">
         <v>2000</v>
@@ -1695,13 +1704,13 @@
         <v>100</v>
       </c>
       <c r="O20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="P20" t="s">
         <v>33</v>
       </c>
       <c r="Q20">
-        <v>5250000</v>
+        <v>4837500</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1712,34 +1721,34 @@
         <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D21">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="F21">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K21" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1748,51 +1757,51 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P21" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="Q21">
-        <v>3000000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F22">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K22" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1801,119 +1810,119 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P22" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="Q22">
-        <v>3562500</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D23">
-        <v>221</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F23">
-        <v>221</v>
+        <v>80</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M23">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N23">
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="Q23">
-        <v>975000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D24">
-        <v>480</v>
+        <v>95</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F24">
-        <v>480</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M24">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N24">
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="P24" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="Q24">
-        <v>1123925</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1924,208 +1933,208 @@
         <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D25">
-        <v>207.68</v>
+        <v>221</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F25">
-        <v>207.68</v>
+        <v>221</v>
       </c>
       <c r="G25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M25">
-        <v>16000</v>
+        <v>17000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
+        <v>84</v>
+      </c>
+      <c r="P25" t="s">
         <v>82</v>
       </c>
-      <c r="P25" t="s">
-        <v>80</v>
-      </c>
       <c r="Q25">
-        <v>957220</v>
+        <v>975000</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>480</v>
       </c>
       <c r="E26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F26">
-        <v>100</v>
+        <v>480</v>
       </c>
       <c r="G26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L26" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M26">
-        <v>2000</v>
+        <v>30000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
+        <v>84</v>
+      </c>
+      <c r="P26" t="s">
         <v>82</v>
       </c>
-      <c r="P26" t="s">
-        <v>80</v>
-      </c>
       <c r="Q26">
-        <v>3750000</v>
+        <v>1123925</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D27">
-        <v>560</v>
+        <v>207.68</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27">
-        <v>560</v>
+        <v>207.68</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K27" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L27" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M27">
-        <v>40000</v>
+        <v>16000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
+        <v>85</v>
+      </c>
+      <c r="P27" t="s">
         <v>83</v>
       </c>
-      <c r="P27" t="s">
-        <v>88</v>
-      </c>
       <c r="Q27">
-        <v>1050000</v>
+        <v>957220</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D28">
-        <v>700.0000199999999</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F28">
-        <v>350.00001</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K28" t="s">
         <v>76</v>
       </c>
       <c r="L28" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M28">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="N28">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="P28" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="Q28">
-        <v>32666668</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2133,51 +2142,157 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D29">
-        <v>700.0000199999999</v>
+        <v>560</v>
       </c>
       <c r="E29" t="s">
         <v>62</v>
       </c>
       <c r="F29">
-        <v>350.00001</v>
+        <v>560</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K29" t="s">
         <v>76</v>
       </c>
       <c r="L29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M29">
+        <v>40000</v>
+      </c>
+      <c r="N29">
+        <v>100</v>
+      </c>
+      <c r="O29" t="s">
+        <v>86</v>
+      </c>
+      <c r="P29" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q29">
+        <v>1050000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>700.0000199999999</v>
+      </c>
+      <c r="E30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30">
+        <v>350.00001</v>
+      </c>
+      <c r="G30" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30" t="s">
+        <v>75</v>
+      </c>
+      <c r="K30" t="s">
+        <v>78</v>
+      </c>
+      <c r="L30" t="s">
+        <v>75</v>
+      </c>
+      <c r="M30">
         <v>3000</v>
       </c>
-      <c r="N29">
+      <c r="N30">
         <v>50</v>
       </c>
-      <c r="O29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P29" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q29">
+      <c r="O30" t="s">
+        <v>82</v>
+      </c>
+      <c r="P30" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q30">
+        <v>32666668</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>700.0000199999999</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31">
+        <v>350.00001</v>
+      </c>
+      <c r="G31" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" t="s">
+        <v>75</v>
+      </c>
+      <c r="K31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31" t="s">
+        <v>75</v>
+      </c>
+      <c r="M31">
+        <v>3000</v>
+      </c>
+      <c r="N31">
+        <v>50</v>
+      </c>
+      <c r="O31" t="s">
+        <v>82</v>
+      </c>
+      <c r="P31" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q31">
         <v>32666668</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RPA datasets push 2024-08-01
</commit_message>
<xml_diff>
--- a/datasets/form1.xlsx
+++ b/datasets/form1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="96">
   <si>
     <t>상장일</t>
   </si>
@@ -67,6 +67,9 @@
     <t>총기관배정수량</t>
   </si>
   <si>
+    <t>2024-07-31</t>
+  </si>
+  <si>
     <t>2024-07-29</t>
   </si>
   <si>
@@ -124,6 +127,9 @@
     <t>2024-07-01</t>
   </si>
   <si>
+    <t>피앤에스미캐닉스</t>
+  </si>
+  <si>
     <t>산일전기</t>
   </si>
   <si>
@@ -193,10 +199,13 @@
     <t>신한글로벌액티브리츠</t>
   </si>
   <si>
+    <t>코스닥</t>
+  </si>
+  <si>
     <t>코스피</t>
   </si>
   <si>
-    <t>코스닥</t>
+    <t>키움</t>
   </si>
   <si>
     <t>미래</t>
@@ -251,6 +260,9 @@
   </si>
   <si>
     <t>공동대표</t>
+  </si>
+  <si>
+    <t>2024-07-22</t>
   </si>
   <si>
     <t>2024-07-18</t>
@@ -647,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -711,102 +723,102 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D2">
-        <v>2660</v>
+        <v>297</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F2">
-        <v>2553.6</v>
+        <v>297</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M2">
-        <v>35000</v>
+        <v>22000</v>
       </c>
       <c r="N2">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="P2" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="Q2">
-        <v>9340690</v>
+        <v>1012500</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>2660</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F3">
-        <v>106.4</v>
+        <v>2553.6</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M3">
         <v>35000</v>
       </c>
       <c r="N3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="O3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="P3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="Q3">
         <v>9340690</v>
@@ -817,52 +829,52 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D4">
-        <v>120</v>
+        <v>2660</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F4">
-        <v>120</v>
+        <v>106.4</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M4">
-        <v>2000</v>
+        <v>35000</v>
       </c>
       <c r="N4">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="P4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Q4">
-        <v>4500000</v>
+        <v>9340690</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -870,37 +882,37 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F5">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M5">
         <v>2000</v>
@@ -909,13 +921,13 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="P5" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="Q5">
-        <v>3000000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -923,52 +935,52 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D6">
-        <v>161.8</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F6">
-        <v>161.8</v>
+        <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M6">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="N6">
         <v>100</v>
       </c>
       <c r="O6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="P6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="Q6">
-        <v>1187900</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -976,90 +988,90 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D7">
-        <v>4350</v>
+        <v>161.8</v>
       </c>
       <c r="E7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F7">
-        <v>1435.5</v>
+        <v>161.8</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M7">
-        <v>60000</v>
+        <v>10000</v>
       </c>
       <c r="N7">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="O7" t="s">
         <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="Q7">
-        <v>21750000</v>
+        <v>1187900</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D8">
         <v>4350</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F8">
         <v>1435.5</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K8" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M8">
         <v>60000</v>
@@ -1068,10 +1080,10 @@
         <v>33</v>
       </c>
       <c r="O8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q8">
         <v>21750000</v>
@@ -1079,52 +1091,52 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>4350</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="F9">
-        <v>1305</v>
+        <v>1435.5</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K9" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M9">
         <v>60000</v>
       </c>
       <c r="N9">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q9">
         <v>21750000</v>
@@ -1132,52 +1144,52 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>4350</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F10">
-        <v>174</v>
+        <v>1305</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M10">
         <v>60000</v>
       </c>
       <c r="N10">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="O10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P10" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q10">
         <v>21750000</v>
@@ -1188,52 +1200,52 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11">
+        <v>4350</v>
+      </c>
+      <c r="E11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11">
+        <v>174</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11" t="s">
         <v>80</v>
       </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11">
-        <v>80</v>
-      </c>
-      <c r="G11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" t="s">
-        <v>75</v>
-      </c>
-      <c r="J11" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" t="s">
-        <v>76</v>
-      </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M11">
-        <v>2000</v>
+        <v>60000</v>
       </c>
       <c r="N11">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="O11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q11">
-        <v>3000000</v>
+        <v>21750000</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1241,52 +1253,52 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12">
-        <v>289.6</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F12">
-        <v>289.6</v>
+        <v>80</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M12">
-        <v>16000</v>
+        <v>2000</v>
       </c>
       <c r="N12">
         <v>100</v>
       </c>
       <c r="O12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P12" t="s">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="Q12">
-        <v>1357500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1294,102 +1306,102 @@
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D13">
-        <v>575.89</v>
+        <v>289.6</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F13">
-        <v>541.3366</v>
+        <v>289.6</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L13" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M13">
-        <v>43300</v>
+        <v>16000</v>
       </c>
       <c r="N13">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O13" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="P13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q13">
-        <v>1906400</v>
+        <v>1357500</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14">
         <v>575.89</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F14">
-        <v>34.5534</v>
+        <v>541.3366</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L14" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M14">
         <v>43300</v>
       </c>
       <c r="N14">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="O14" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="P14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q14">
         <v>1906400</v>
@@ -1400,52 +1412,52 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D15">
-        <v>432</v>
+        <v>575.89</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F15">
-        <v>432</v>
+        <v>34.5534</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K15" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M15">
-        <v>18000</v>
+        <v>43300</v>
       </c>
       <c r="N15">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="O15" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="P15" t="s">
         <v>29</v>
       </c>
       <c r="Q15">
-        <v>1758600</v>
+        <v>1906400</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1453,52 +1465,52 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="E16" t="s">
         <v>66</v>
       </c>
       <c r="F16">
-        <v>238</v>
+        <v>432</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L16" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M16">
-        <v>7000</v>
+        <v>18000</v>
       </c>
       <c r="N16">
         <v>100</v>
       </c>
       <c r="O16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P16" t="s">
         <v>30</v>
       </c>
       <c r="Q16">
-        <v>2350000</v>
+        <v>1758600</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1506,52 +1518,52 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F17">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M17">
-        <v>2000</v>
+        <v>7000</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P17" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="Q17">
-        <v>4687500</v>
+        <v>2350000</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1559,102 +1571,102 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D18">
-        <v>230</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F18">
-        <v>218.5</v>
+        <v>125</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M18">
-        <v>11500</v>
+        <v>2000</v>
       </c>
       <c r="N18">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="O18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P18" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="Q18">
-        <v>3000000</v>
+        <v>4687500</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19">
-        <v>11.5</v>
+        <v>218.5</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M19">
         <v>11500</v>
       </c>
       <c r="N19">
-        <v>5</v>
+        <v>95</v>
       </c>
       <c r="O19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q19">
         <v>3000000</v>
@@ -1665,52 +1677,52 @@
         <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20">
-        <v>129</v>
+        <v>230</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="F20">
-        <v>129</v>
+        <v>11.5</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M20">
-        <v>2000</v>
+        <v>11500</v>
       </c>
       <c r="N20">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="O20" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="P20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q20">
-        <v>4837500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1718,37 +1730,37 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D21">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F21">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L21" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M21">
         <v>2000</v>
@@ -1757,51 +1769,51 @@
         <v>100</v>
       </c>
       <c r="O21" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="P21" t="s">
         <v>34</v>
       </c>
       <c r="Q21">
-        <v>4500000</v>
+        <v>4837500</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F22">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M22">
         <v>2000</v>
@@ -1810,51 +1822,51 @@
         <v>100</v>
       </c>
       <c r="O22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="P22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q22">
-        <v>5250000</v>
+        <v>4500000</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D23">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="E23" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F23">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="G23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K23" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M23">
         <v>2000</v>
@@ -1863,51 +1875,51 @@
         <v>100</v>
       </c>
       <c r="O23" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="P23" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="Q23">
-        <v>3000000</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F24">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="G24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K24" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L24" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M24">
         <v>2000</v>
@@ -1916,172 +1928,172 @@
         <v>100</v>
       </c>
       <c r="O24" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P24" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="Q24">
-        <v>3562500</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D25">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F25">
-        <v>221</v>
+        <v>95</v>
       </c>
       <c r="G25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K25" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M25">
-        <v>17000</v>
+        <v>2000</v>
       </c>
       <c r="N25">
         <v>100</v>
       </c>
       <c r="O25" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P25" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="Q25">
-        <v>975000</v>
+        <v>3562500</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D26">
-        <v>480</v>
+        <v>221</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F26">
-        <v>480</v>
+        <v>221</v>
       </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K26" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L26" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M26">
-        <v>30000</v>
+        <v>17000</v>
       </c>
       <c r="N26">
         <v>100</v>
       </c>
       <c r="O26" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="P26" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="Q26">
-        <v>1123925</v>
+        <v>975000</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D27">
-        <v>207.68</v>
+        <v>480</v>
       </c>
       <c r="E27" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="F27">
-        <v>207.68</v>
+        <v>480</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K27" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M27">
-        <v>16000</v>
+        <v>30000</v>
       </c>
       <c r="N27">
         <v>100</v>
       </c>
       <c r="O27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="P27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q27">
-        <v>957220</v>
+        <v>1123925</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -2089,52 +2101,52 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D28">
-        <v>100</v>
+        <v>207.68</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F28">
-        <v>100</v>
+        <v>207.68</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K28" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L28" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M28">
-        <v>2000</v>
+        <v>16000</v>
       </c>
       <c r="N28">
         <v>100</v>
       </c>
       <c r="O28" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="P28" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="Q28">
-        <v>3750000</v>
+        <v>957220</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2142,52 +2154,52 @@
         <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D29">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="F29">
-        <v>560</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L29" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M29">
-        <v>40000</v>
+        <v>2000</v>
       </c>
       <c r="N29">
         <v>100</v>
       </c>
       <c r="O29" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="P29" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="Q29">
-        <v>1050000</v>
+        <v>3750000</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2195,90 +2207,90 @@
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D30">
-        <v>700.0000199999999</v>
+        <v>560</v>
       </c>
       <c r="E30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F30">
-        <v>350.00001</v>
+        <v>560</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M30">
-        <v>3000</v>
+        <v>40000</v>
       </c>
       <c r="N30">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O30" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="P30" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="Q30">
-        <v>32666668</v>
+        <v>1050000</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D31">
         <v>700.0000199999999</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F31">
         <v>350.00001</v>
       </c>
       <c r="G31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L31" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="M31">
         <v>3000</v>
@@ -2287,12 +2299,65 @@
         <v>50</v>
       </c>
       <c r="O31" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="P31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q31">
+        <v>32666668</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32">
+        <v>700.0000199999999</v>
+      </c>
+      <c r="E32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32">
+        <v>350.00001</v>
+      </c>
+      <c r="G32" t="s">
+        <v>78</v>
+      </c>
+      <c r="H32" t="s">
+        <v>78</v>
+      </c>
+      <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K32" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" t="s">
+        <v>78</v>
+      </c>
+      <c r="M32">
+        <v>3000</v>
+      </c>
+      <c r="N32">
+        <v>50</v>
+      </c>
+      <c r="O32" t="s">
+        <v>86</v>
+      </c>
+      <c r="P32" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32">
         <v>32666668</v>
       </c>
     </row>

</xml_diff>